<commit_message>
[SMAL] QMM008 Screen F
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_標準報酬月額表（厚生年金).xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_標準報酬月額表（厚生年金).xlsx
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="17">
   <si>
     <t>名称</t>
     <rPh sb="0" eb="2">
@@ -829,15 +829,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="38" fontId="4" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -886,6 +877,15 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
@@ -924,7 +924,7 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>17518</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>22412</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -933,8 +933,72 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="285271" y="688840"/>
-          <a:ext cx="9705482" cy="14584778"/>
+          <a:off x="285271" y="218193"/>
+          <a:ext cx="9862365" cy="14562366"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 390"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>173212</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>5281</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>17518</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="角丸四角形 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="285271" y="218193"/>
+          <a:ext cx="9862365" cy="14562366"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -44543,11 +44607,9 @@
   <sheetPr codeName="Sheet7">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:O67"/>
+  <dimension ref="B1:O135"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12"/>
   <cols>
@@ -44574,33 +44636,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:15" ht="9.75" customHeight="1">
+    <row r="2" spans="2:15" ht="4.9000000000000004" customHeight="1">
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="2:15" ht="18" customHeight="1">
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="44" t="s">
+      <c r="D3" s="40"/>
+      <c r="E3" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="45"/>
-      <c r="G3" s="46" t="s">
+      <c r="F3" s="42"/>
+      <c r="G3" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="46" t="s">
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="41" t="s">
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="38" t="s">
         <v>8</v>
       </c>
     </row>
@@ -44609,23 +44671,23 @@
       <c r="D4" s="23"/>
       <c r="E4" s="24"/>
       <c r="F4" s="25"/>
-      <c r="G4" s="50" t="s">
+      <c r="G4" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="51"/>
-      <c r="I4" s="52" t="s">
+      <c r="H4" s="48"/>
+      <c r="I4" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="53"/>
-      <c r="K4" s="50" t="s">
+      <c r="J4" s="50"/>
+      <c r="K4" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="51"/>
-      <c r="M4" s="52" t="s">
+      <c r="L4" s="48"/>
+      <c r="M4" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="53"/>
-      <c r="O4" s="41"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="38"/>
     </row>
     <row r="5" spans="2:15" ht="18" customHeight="1" thickBot="1">
       <c r="C5" s="5" t="s">
@@ -44664,10 +44726,10 @@
       <c r="N5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="41"/>
+      <c r="O5" s="38"/>
     </row>
     <row r="6" spans="2:15" ht="18" customHeight="1" thickTop="1">
-      <c r="C6" s="35"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="32"/>
       <c r="E6" s="11"/>
       <c r="F6" s="12"/>
@@ -44682,7 +44744,7 @@
       <c r="O6" s="26"/>
     </row>
     <row r="7" spans="2:15" ht="18" customHeight="1">
-      <c r="C7" s="36"/>
+      <c r="C7" s="52"/>
       <c r="D7" s="17"/>
       <c r="E7" s="13"/>
       <c r="F7" s="14"/>
@@ -44697,7 +44759,7 @@
       <c r="O7" s="27"/>
     </row>
     <row r="8" spans="2:15" ht="18" customHeight="1">
-      <c r="C8" s="37"/>
+      <c r="C8" s="53"/>
       <c r="D8" s="22"/>
       <c r="E8" s="18"/>
       <c r="F8" s="19"/>
@@ -44712,7 +44774,7 @@
       <c r="O8" s="26"/>
     </row>
     <row r="9" spans="2:15" ht="18" customHeight="1">
-      <c r="C9" s="36"/>
+      <c r="C9" s="52"/>
       <c r="D9" s="17"/>
       <c r="E9" s="13"/>
       <c r="F9" s="14"/>
@@ -44727,7 +44789,7 @@
       <c r="O9" s="27"/>
     </row>
     <row r="10" spans="2:15" ht="18" customHeight="1">
-      <c r="C10" s="37"/>
+      <c r="C10" s="53"/>
       <c r="D10" s="22"/>
       <c r="E10" s="18"/>
       <c r="F10" s="19"/>
@@ -44742,7 +44804,7 @@
       <c r="O10" s="26"/>
     </row>
     <row r="11" spans="2:15" ht="18" customHeight="1">
-      <c r="C11" s="36"/>
+      <c r="C11" s="52"/>
       <c r="D11" s="17"/>
       <c r="E11" s="13"/>
       <c r="F11" s="14"/>
@@ -44757,7 +44819,7 @@
       <c r="O11" s="27"/>
     </row>
     <row r="12" spans="2:15" ht="18" customHeight="1">
-      <c r="C12" s="37"/>
+      <c r="C12" s="53"/>
       <c r="D12" s="22"/>
       <c r="E12" s="18"/>
       <c r="F12" s="19"/>
@@ -44772,7 +44834,7 @@
       <c r="O12" s="26"/>
     </row>
     <row r="13" spans="2:15" ht="18" customHeight="1">
-      <c r="C13" s="36"/>
+      <c r="C13" s="52"/>
       <c r="D13" s="17"/>
       <c r="E13" s="13"/>
       <c r="F13" s="14"/>
@@ -44787,7 +44849,7 @@
       <c r="O13" s="27"/>
     </row>
     <row r="14" spans="2:15" ht="18" customHeight="1">
-      <c r="C14" s="37"/>
+      <c r="C14" s="53"/>
       <c r="D14" s="22"/>
       <c r="E14" s="18"/>
       <c r="F14" s="19"/>
@@ -44802,7 +44864,7 @@
       <c r="O14" s="26"/>
     </row>
     <row r="15" spans="2:15" ht="18" customHeight="1">
-      <c r="C15" s="36"/>
+      <c r="C15" s="52"/>
       <c r="D15" s="17"/>
       <c r="E15" s="13"/>
       <c r="F15" s="14"/>
@@ -44817,7 +44879,7 @@
       <c r="O15" s="27"/>
     </row>
     <row r="16" spans="2:15" ht="18" customHeight="1">
-      <c r="C16" s="37"/>
+      <c r="C16" s="53"/>
       <c r="D16" s="22"/>
       <c r="E16" s="18"/>
       <c r="F16" s="19"/>
@@ -44832,7 +44894,7 @@
       <c r="O16" s="26"/>
     </row>
     <row r="17" spans="3:15" ht="18" customHeight="1">
-      <c r="C17" s="36"/>
+      <c r="C17" s="52"/>
       <c r="D17" s="17"/>
       <c r="E17" s="13"/>
       <c r="F17" s="14"/>
@@ -44847,7 +44909,7 @@
       <c r="O17" s="27"/>
     </row>
     <row r="18" spans="3:15" ht="18" customHeight="1">
-      <c r="C18" s="37"/>
+      <c r="C18" s="53"/>
       <c r="D18" s="22"/>
       <c r="E18" s="18"/>
       <c r="F18" s="19"/>
@@ -44862,7 +44924,7 @@
       <c r="O18" s="26"/>
     </row>
     <row r="19" spans="3:15" ht="18" customHeight="1">
-      <c r="C19" s="36"/>
+      <c r="C19" s="52"/>
       <c r="D19" s="17"/>
       <c r="E19" s="13"/>
       <c r="F19" s="14"/>
@@ -44877,7 +44939,7 @@
       <c r="O19" s="27"/>
     </row>
     <row r="20" spans="3:15" ht="18" customHeight="1">
-      <c r="C20" s="37"/>
+      <c r="C20" s="53"/>
       <c r="D20" s="22"/>
       <c r="E20" s="18"/>
       <c r="F20" s="19"/>
@@ -44892,7 +44954,7 @@
       <c r="O20" s="26"/>
     </row>
     <row r="21" spans="3:15" ht="18" customHeight="1">
-      <c r="C21" s="36"/>
+      <c r="C21" s="52"/>
       <c r="D21" s="17"/>
       <c r="E21" s="13"/>
       <c r="F21" s="14"/>
@@ -44907,7 +44969,7 @@
       <c r="O21" s="27"/>
     </row>
     <row r="22" spans="3:15" ht="18" customHeight="1">
-      <c r="C22" s="37"/>
+      <c r="C22" s="53"/>
       <c r="D22" s="22"/>
       <c r="E22" s="18"/>
       <c r="F22" s="19"/>
@@ -44922,7 +44984,7 @@
       <c r="O22" s="26"/>
     </row>
     <row r="23" spans="3:15" ht="18" customHeight="1">
-      <c r="C23" s="36"/>
+      <c r="C23" s="52"/>
       <c r="D23" s="17"/>
       <c r="E23" s="13"/>
       <c r="F23" s="14"/>
@@ -44937,7 +44999,7 @@
       <c r="O23" s="27"/>
     </row>
     <row r="24" spans="3:15" ht="18" customHeight="1">
-      <c r="C24" s="37"/>
+      <c r="C24" s="53"/>
       <c r="D24" s="22"/>
       <c r="E24" s="18"/>
       <c r="F24" s="19"/>
@@ -44952,7 +45014,7 @@
       <c r="O24" s="26"/>
     </row>
     <row r="25" spans="3:15" ht="18" customHeight="1">
-      <c r="C25" s="36"/>
+      <c r="C25" s="52"/>
       <c r="D25" s="17"/>
       <c r="E25" s="13"/>
       <c r="F25" s="14"/>
@@ -44967,7 +45029,7 @@
       <c r="O25" s="27"/>
     </row>
     <row r="26" spans="3:15" ht="18" customHeight="1">
-      <c r="C26" s="37"/>
+      <c r="C26" s="53"/>
       <c r="D26" s="22"/>
       <c r="E26" s="18"/>
       <c r="F26" s="19"/>
@@ -44982,7 +45044,7 @@
       <c r="O26" s="26"/>
     </row>
     <row r="27" spans="3:15" ht="18" customHeight="1">
-      <c r="C27" s="36"/>
+      <c r="C27" s="52"/>
       <c r="D27" s="17"/>
       <c r="E27" s="13"/>
       <c r="F27" s="14"/>
@@ -44997,7 +45059,7 @@
       <c r="O27" s="27"/>
     </row>
     <row r="28" spans="3:15" ht="18" customHeight="1">
-      <c r="C28" s="37"/>
+      <c r="C28" s="53"/>
       <c r="D28" s="22"/>
       <c r="E28" s="18"/>
       <c r="F28" s="19"/>
@@ -45012,7 +45074,7 @@
       <c r="O28" s="26"/>
     </row>
     <row r="29" spans="3:15" ht="18" customHeight="1">
-      <c r="C29" s="36"/>
+      <c r="C29" s="52"/>
       <c r="D29" s="17"/>
       <c r="E29" s="13"/>
       <c r="F29" s="14"/>
@@ -45027,7 +45089,7 @@
       <c r="O29" s="27"/>
     </row>
     <row r="30" spans="3:15" ht="18" customHeight="1">
-      <c r="C30" s="37"/>
+      <c r="C30" s="53"/>
       <c r="D30" s="22"/>
       <c r="E30" s="18"/>
       <c r="F30" s="19"/>
@@ -45042,7 +45104,7 @@
       <c r="O30" s="26"/>
     </row>
     <row r="31" spans="3:15" ht="18" customHeight="1">
-      <c r="C31" s="36"/>
+      <c r="C31" s="52"/>
       <c r="D31" s="17"/>
       <c r="E31" s="13"/>
       <c r="F31" s="14"/>
@@ -45057,7 +45119,7 @@
       <c r="O31" s="27"/>
     </row>
     <row r="32" spans="3:15" ht="18" customHeight="1">
-      <c r="C32" s="37"/>
+      <c r="C32" s="53"/>
       <c r="D32" s="22"/>
       <c r="E32" s="18"/>
       <c r="F32" s="19"/>
@@ -45072,7 +45134,7 @@
       <c r="O32" s="26"/>
     </row>
     <row r="33" spans="3:15" ht="18" customHeight="1">
-      <c r="C33" s="36"/>
+      <c r="C33" s="52"/>
       <c r="D33" s="17"/>
       <c r="E33" s="13"/>
       <c r="F33" s="14"/>
@@ -45087,7 +45149,7 @@
       <c r="O33" s="27"/>
     </row>
     <row r="34" spans="3:15" ht="18" customHeight="1">
-      <c r="C34" s="37"/>
+      <c r="C34" s="53"/>
       <c r="D34" s="22"/>
       <c r="E34" s="18"/>
       <c r="F34" s="19"/>
@@ -45102,7 +45164,7 @@
       <c r="O34" s="26"/>
     </row>
     <row r="35" spans="3:15" ht="18" customHeight="1">
-      <c r="C35" s="36"/>
+      <c r="C35" s="52"/>
       <c r="D35" s="17"/>
       <c r="E35" s="13"/>
       <c r="F35" s="14"/>
@@ -45117,7 +45179,7 @@
       <c r="O35" s="27"/>
     </row>
     <row r="36" spans="3:15" ht="18" customHeight="1">
-      <c r="C36" s="37"/>
+      <c r="C36" s="53"/>
       <c r="D36" s="22"/>
       <c r="E36" s="18"/>
       <c r="F36" s="19"/>
@@ -45132,7 +45194,7 @@
       <c r="O36" s="26"/>
     </row>
     <row r="37" spans="3:15" ht="18" customHeight="1">
-      <c r="C37" s="36"/>
+      <c r="C37" s="52"/>
       <c r="D37" s="17"/>
       <c r="E37" s="13"/>
       <c r="F37" s="14"/>
@@ -45147,22 +45209,22 @@
       <c r="O37" s="27"/>
     </row>
     <row r="38" spans="3:15" ht="18" customHeight="1">
-      <c r="C38" s="35"/>
+      <c r="C38" s="51"/>
       <c r="D38" s="32"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="39"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="36"/>
       <c r="G38" s="28"/>
       <c r="H38" s="29"/>
       <c r="I38" s="29"/>
       <c r="J38" s="30"/>
-      <c r="K38" s="40"/>
+      <c r="K38" s="37"/>
       <c r="L38" s="29"/>
       <c r="M38" s="29"/>
       <c r="N38" s="29"/>
       <c r="O38" s="26"/>
     </row>
     <row r="39" spans="3:15" ht="18" customHeight="1">
-      <c r="C39" s="36"/>
+      <c r="C39" s="52"/>
       <c r="D39" s="17"/>
       <c r="E39" s="13"/>
       <c r="F39" s="14"/>
@@ -45177,7 +45239,7 @@
       <c r="O39" s="27"/>
     </row>
     <row r="40" spans="3:15" ht="18" customHeight="1">
-      <c r="C40" s="37"/>
+      <c r="C40" s="53"/>
       <c r="D40" s="22"/>
       <c r="E40" s="18"/>
       <c r="F40" s="19"/>
@@ -45192,7 +45254,7 @@
       <c r="O40" s="26"/>
     </row>
     <row r="41" spans="3:15" ht="18" customHeight="1">
-      <c r="C41" s="36"/>
+      <c r="C41" s="52"/>
       <c r="D41" s="17"/>
       <c r="E41" s="13"/>
       <c r="F41" s="14"/>
@@ -45207,7 +45269,7 @@
       <c r="O41" s="27"/>
     </row>
     <row r="42" spans="3:15" ht="18" customHeight="1">
-      <c r="C42" s="37"/>
+      <c r="C42" s="53"/>
       <c r="D42" s="22"/>
       <c r="E42" s="18"/>
       <c r="F42" s="19"/>
@@ -45222,7 +45284,7 @@
       <c r="O42" s="26"/>
     </row>
     <row r="43" spans="3:15" ht="18" customHeight="1">
-      <c r="C43" s="36"/>
+      <c r="C43" s="52"/>
       <c r="D43" s="17"/>
       <c r="E43" s="13"/>
       <c r="F43" s="14"/>
@@ -45237,7 +45299,7 @@
       <c r="O43" s="27"/>
     </row>
     <row r="44" spans="3:15" ht="18" customHeight="1">
-      <c r="C44" s="37"/>
+      <c r="C44" s="53"/>
       <c r="D44" s="22"/>
       <c r="E44" s="18"/>
       <c r="F44" s="19"/>
@@ -45252,7 +45314,7 @@
       <c r="O44" s="26"/>
     </row>
     <row r="45" spans="3:15" ht="18" customHeight="1">
-      <c r="C45" s="36"/>
+      <c r="C45" s="52"/>
       <c r="D45" s="17"/>
       <c r="E45" s="13"/>
       <c r="F45" s="14"/>
@@ -45267,7 +45329,7 @@
       <c r="O45" s="27"/>
     </row>
     <row r="46" spans="3:15" ht="18" customHeight="1">
-      <c r="C46" s="37"/>
+      <c r="C46" s="53"/>
       <c r="D46" s="22"/>
       <c r="E46" s="18"/>
       <c r="F46" s="19"/>
@@ -45282,7 +45344,7 @@
       <c r="O46" s="26"/>
     </row>
     <row r="47" spans="3:15" ht="18" customHeight="1">
-      <c r="C47" s="36"/>
+      <c r="C47" s="52"/>
       <c r="D47" s="17"/>
       <c r="E47" s="13"/>
       <c r="F47" s="14"/>
@@ -45297,7 +45359,7 @@
       <c r="O47" s="27"/>
     </row>
     <row r="48" spans="3:15" ht="18" customHeight="1">
-      <c r="C48" s="37"/>
+      <c r="C48" s="53"/>
       <c r="D48" s="22"/>
       <c r="E48" s="18"/>
       <c r="F48" s="19"/>
@@ -45312,7 +45374,7 @@
       <c r="O48" s="26"/>
     </row>
     <row r="49" spans="3:15" ht="18" customHeight="1">
-      <c r="C49" s="36"/>
+      <c r="C49" s="52"/>
       <c r="D49" s="17"/>
       <c r="E49" s="13"/>
       <c r="F49" s="14"/>
@@ -45327,7 +45389,7 @@
       <c r="O49" s="27"/>
     </row>
     <row r="50" spans="3:15" ht="18" customHeight="1">
-      <c r="C50" s="37"/>
+      <c r="C50" s="53"/>
       <c r="D50" s="22"/>
       <c r="E50" s="18"/>
       <c r="F50" s="19"/>
@@ -45342,7 +45404,7 @@
       <c r="O50" s="26"/>
     </row>
     <row r="51" spans="3:15" ht="18" customHeight="1">
-      <c r="C51" s="36"/>
+      <c r="C51" s="52"/>
       <c r="D51" s="17"/>
       <c r="E51" s="13"/>
       <c r="F51" s="14"/>
@@ -45357,7 +45419,7 @@
       <c r="O51" s="27"/>
     </row>
     <row r="52" spans="3:15" ht="18" customHeight="1">
-      <c r="C52" s="37"/>
+      <c r="C52" s="53"/>
       <c r="D52" s="22"/>
       <c r="E52" s="18"/>
       <c r="F52" s="19"/>
@@ -45372,7 +45434,7 @@
       <c r="O52" s="26"/>
     </row>
     <row r="53" spans="3:15" ht="18" customHeight="1">
-      <c r="C53" s="36"/>
+      <c r="C53" s="52"/>
       <c r="D53" s="17"/>
       <c r="E53" s="13"/>
       <c r="F53" s="14"/>
@@ -45387,7 +45449,7 @@
       <c r="O53" s="27"/>
     </row>
     <row r="54" spans="3:15" ht="18" customHeight="1">
-      <c r="C54" s="37"/>
+      <c r="C54" s="53"/>
       <c r="D54" s="22"/>
       <c r="E54" s="18"/>
       <c r="F54" s="19"/>
@@ -45402,7 +45464,7 @@
       <c r="O54" s="26"/>
     </row>
     <row r="55" spans="3:15" ht="18" customHeight="1">
-      <c r="C55" s="36"/>
+      <c r="C55" s="52"/>
       <c r="D55" s="17"/>
       <c r="E55" s="13"/>
       <c r="F55" s="14"/>
@@ -45417,7 +45479,7 @@
       <c r="O55" s="27"/>
     </row>
     <row r="56" spans="3:15" ht="18" customHeight="1">
-      <c r="C56" s="37"/>
+      <c r="C56" s="53"/>
       <c r="D56" s="22"/>
       <c r="E56" s="18"/>
       <c r="F56" s="19"/>
@@ -45432,7 +45494,7 @@
       <c r="O56" s="26"/>
     </row>
     <row r="57" spans="3:15" ht="18" customHeight="1">
-      <c r="C57" s="36"/>
+      <c r="C57" s="52"/>
       <c r="D57" s="17"/>
       <c r="E57" s="13"/>
       <c r="F57" s="14"/>
@@ -45447,7 +45509,7 @@
       <c r="O57" s="27"/>
     </row>
     <row r="58" spans="3:15" ht="18" customHeight="1">
-      <c r="C58" s="37"/>
+      <c r="C58" s="53"/>
       <c r="D58" s="22"/>
       <c r="E58" s="18"/>
       <c r="F58" s="19"/>
@@ -45462,7 +45524,7 @@
       <c r="O58" s="26"/>
     </row>
     <row r="59" spans="3:15" ht="18" customHeight="1">
-      <c r="C59" s="36"/>
+      <c r="C59" s="52"/>
       <c r="D59" s="17"/>
       <c r="E59" s="13"/>
       <c r="F59" s="14"/>
@@ -45477,7 +45539,7 @@
       <c r="O59" s="27"/>
     </row>
     <row r="60" spans="3:15" ht="18" customHeight="1">
-      <c r="C60" s="37"/>
+      <c r="C60" s="53"/>
       <c r="D60" s="22"/>
       <c r="E60" s="18"/>
       <c r="F60" s="19"/>
@@ -45492,7 +45554,7 @@
       <c r="O60" s="26"/>
     </row>
     <row r="61" spans="3:15" ht="18" customHeight="1">
-      <c r="C61" s="36"/>
+      <c r="C61" s="52"/>
       <c r="D61" s="17"/>
       <c r="E61" s="13"/>
       <c r="F61" s="14"/>
@@ -45507,7 +45569,7 @@
       <c r="O61" s="27"/>
     </row>
     <row r="62" spans="3:15" ht="18" customHeight="1">
-      <c r="C62" s="37"/>
+      <c r="C62" s="53"/>
       <c r="D62" s="22"/>
       <c r="E62" s="18"/>
       <c r="F62" s="19"/>
@@ -45522,7 +45584,7 @@
       <c r="O62" s="26"/>
     </row>
     <row r="63" spans="3:15" ht="18" customHeight="1">
-      <c r="C63" s="36"/>
+      <c r="C63" s="52"/>
       <c r="D63" s="17"/>
       <c r="E63" s="13"/>
       <c r="F63" s="14"/>
@@ -45537,7 +45599,7 @@
       <c r="O63" s="27"/>
     </row>
     <row r="64" spans="3:15" ht="18" customHeight="1">
-      <c r="C64" s="37"/>
+      <c r="C64" s="53"/>
       <c r="D64" s="22"/>
       <c r="E64" s="18"/>
       <c r="F64" s="19"/>
@@ -45551,8 +45613,8 @@
       <c r="N64" s="21"/>
       <c r="O64" s="26"/>
     </row>
-    <row r="65" spans="3:15" ht="18" customHeight="1">
-      <c r="C65" s="36"/>
+    <row r="65" spans="2:15" ht="18" customHeight="1">
+      <c r="C65" s="52"/>
       <c r="D65" s="17"/>
       <c r="E65" s="13"/>
       <c r="F65" s="14"/>
@@ -45566,8 +45628,8 @@
       <c r="N65" s="16"/>
       <c r="O65" s="27"/>
     </row>
-    <row r="66" spans="3:15" ht="18" customHeight="1">
-      <c r="C66" s="37"/>
+    <row r="66" spans="2:15" ht="18" customHeight="1">
+      <c r="C66" s="53"/>
       <c r="D66" s="22"/>
       <c r="E66" s="18"/>
       <c r="F66" s="19"/>
@@ -45581,8 +45643,8 @@
       <c r="N66" s="21"/>
       <c r="O66" s="26"/>
     </row>
-    <row r="67" spans="3:15" ht="18" customHeight="1">
-      <c r="C67" s="36"/>
+    <row r="67" spans="2:15" ht="18" customHeight="1">
+      <c r="C67" s="52"/>
       <c r="D67" s="17"/>
       <c r="E67" s="13"/>
       <c r="F67" s="14"/>
@@ -45596,8 +45658,1053 @@
       <c r="N67" s="16"/>
       <c r="O67" s="27"/>
     </row>
+    <row r="69" spans="2:15">
+      <c r="B69" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="2:15" ht="4.9000000000000004" customHeight="1">
+      <c r="D70" s="2"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="4"/>
+    </row>
+    <row r="71" spans="2:15" ht="18" customHeight="1">
+      <c r="C71" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D71" s="40"/>
+      <c r="E71" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="F71" s="42"/>
+      <c r="G71" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="H71" s="44"/>
+      <c r="I71" s="44"/>
+      <c r="J71" s="45"/>
+      <c r="K71" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="L71" s="44"/>
+      <c r="M71" s="44"/>
+      <c r="N71" s="46"/>
+      <c r="O71" s="38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="2:15" ht="18" customHeight="1">
+      <c r="C72" s="34"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="24"/>
+      <c r="F72" s="25"/>
+      <c r="G72" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="H72" s="48"/>
+      <c r="I72" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="J72" s="50"/>
+      <c r="K72" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="L72" s="48"/>
+      <c r="M72" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="N72" s="50"/>
+      <c r="O72" s="38"/>
+    </row>
+    <row r="73" spans="2:15" ht="18" customHeight="1" thickBot="1">
+      <c r="C73" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F73" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G73" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H73" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I73" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J73" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K73" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L73" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M73" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N73" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O73" s="38"/>
+    </row>
+    <row r="74" spans="2:15" ht="18" customHeight="1" thickTop="1">
+      <c r="C74" s="51"/>
+      <c r="D74" s="32"/>
+      <c r="E74" s="11"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="28"/>
+      <c r="H74" s="29"/>
+      <c r="I74" s="29"/>
+      <c r="J74" s="30"/>
+      <c r="K74" s="31"/>
+      <c r="L74" s="29"/>
+      <c r="M74" s="29"/>
+      <c r="N74" s="29"/>
+      <c r="O74" s="26"/>
+    </row>
+    <row r="75" spans="2:15" ht="18" customHeight="1">
+      <c r="C75" s="52"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="15"/>
+      <c r="H75" s="16"/>
+      <c r="I75" s="16"/>
+      <c r="J75" s="17"/>
+      <c r="K75" s="13"/>
+      <c r="L75" s="16"/>
+      <c r="M75" s="16"/>
+      <c r="N75" s="16"/>
+      <c r="O75" s="27"/>
+    </row>
+    <row r="76" spans="2:15" ht="18" customHeight="1">
+      <c r="C76" s="53"/>
+      <c r="D76" s="22"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="19"/>
+      <c r="G76" s="20"/>
+      <c r="H76" s="21"/>
+      <c r="I76" s="21"/>
+      <c r="J76" s="22"/>
+      <c r="K76" s="18"/>
+      <c r="L76" s="21"/>
+      <c r="M76" s="21"/>
+      <c r="N76" s="21"/>
+      <c r="O76" s="26"/>
+    </row>
+    <row r="77" spans="2:15" ht="18" customHeight="1">
+      <c r="C77" s="52"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="15"/>
+      <c r="H77" s="16"/>
+      <c r="I77" s="16"/>
+      <c r="J77" s="17"/>
+      <c r="K77" s="13"/>
+      <c r="L77" s="16"/>
+      <c r="M77" s="16"/>
+      <c r="N77" s="16"/>
+      <c r="O77" s="27"/>
+    </row>
+    <row r="78" spans="2:15" ht="18" customHeight="1">
+      <c r="C78" s="53"/>
+      <c r="D78" s="22"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="19"/>
+      <c r="G78" s="20"/>
+      <c r="H78" s="21"/>
+      <c r="I78" s="21"/>
+      <c r="J78" s="22"/>
+      <c r="K78" s="18"/>
+      <c r="L78" s="21"/>
+      <c r="M78" s="21"/>
+      <c r="N78" s="21"/>
+      <c r="O78" s="26"/>
+    </row>
+    <row r="79" spans="2:15" ht="18" customHeight="1">
+      <c r="C79" s="52"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="15"/>
+      <c r="H79" s="16"/>
+      <c r="I79" s="16"/>
+      <c r="J79" s="17"/>
+      <c r="K79" s="13"/>
+      <c r="L79" s="16"/>
+      <c r="M79" s="16"/>
+      <c r="N79" s="16"/>
+      <c r="O79" s="27"/>
+    </row>
+    <row r="80" spans="2:15" ht="18" customHeight="1">
+      <c r="C80" s="53"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="19"/>
+      <c r="G80" s="20"/>
+      <c r="H80" s="21"/>
+      <c r="I80" s="21"/>
+      <c r="J80" s="22"/>
+      <c r="K80" s="18"/>
+      <c r="L80" s="21"/>
+      <c r="M80" s="21"/>
+      <c r="N80" s="21"/>
+      <c r="O80" s="26"/>
+    </row>
+    <row r="81" spans="3:15" ht="18" customHeight="1">
+      <c r="C81" s="52"/>
+      <c r="D81" s="17"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="15"/>
+      <c r="H81" s="16"/>
+      <c r="I81" s="16"/>
+      <c r="J81" s="17"/>
+      <c r="K81" s="13"/>
+      <c r="L81" s="16"/>
+      <c r="M81" s="16"/>
+      <c r="N81" s="16"/>
+      <c r="O81" s="27"/>
+    </row>
+    <row r="82" spans="3:15" ht="18" customHeight="1">
+      <c r="C82" s="53"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="19"/>
+      <c r="G82" s="20"/>
+      <c r="H82" s="21"/>
+      <c r="I82" s="21"/>
+      <c r="J82" s="22"/>
+      <c r="K82" s="18"/>
+      <c r="L82" s="21"/>
+      <c r="M82" s="21"/>
+      <c r="N82" s="21"/>
+      <c r="O82" s="26"/>
+    </row>
+    <row r="83" spans="3:15" ht="18" customHeight="1">
+      <c r="C83" s="52"/>
+      <c r="D83" s="17"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="15"/>
+      <c r="H83" s="16"/>
+      <c r="I83" s="16"/>
+      <c r="J83" s="17"/>
+      <c r="K83" s="13"/>
+      <c r="L83" s="16"/>
+      <c r="M83" s="16"/>
+      <c r="N83" s="16"/>
+      <c r="O83" s="27"/>
+    </row>
+    <row r="84" spans="3:15" ht="18" customHeight="1">
+      <c r="C84" s="53"/>
+      <c r="D84" s="22"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="19"/>
+      <c r="G84" s="20"/>
+      <c r="H84" s="21"/>
+      <c r="I84" s="21"/>
+      <c r="J84" s="22"/>
+      <c r="K84" s="18"/>
+      <c r="L84" s="21"/>
+      <c r="M84" s="21"/>
+      <c r="N84" s="21"/>
+      <c r="O84" s="26"/>
+    </row>
+    <row r="85" spans="3:15" ht="18" customHeight="1">
+      <c r="C85" s="52"/>
+      <c r="D85" s="17"/>
+      <c r="E85" s="13"/>
+      <c r="F85" s="14"/>
+      <c r="G85" s="15"/>
+      <c r="H85" s="16"/>
+      <c r="I85" s="16"/>
+      <c r="J85" s="17"/>
+      <c r="K85" s="13"/>
+      <c r="L85" s="16"/>
+      <c r="M85" s="16"/>
+      <c r="N85" s="16"/>
+      <c r="O85" s="27"/>
+    </row>
+    <row r="86" spans="3:15" ht="18" customHeight="1">
+      <c r="C86" s="53"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="18"/>
+      <c r="F86" s="19"/>
+      <c r="G86" s="20"/>
+      <c r="H86" s="21"/>
+      <c r="I86" s="21"/>
+      <c r="J86" s="22"/>
+      <c r="K86" s="18"/>
+      <c r="L86" s="21"/>
+      <c r="M86" s="21"/>
+      <c r="N86" s="21"/>
+      <c r="O86" s="26"/>
+    </row>
+    <row r="87" spans="3:15" ht="18" customHeight="1">
+      <c r="C87" s="52"/>
+      <c r="D87" s="17"/>
+      <c r="E87" s="13"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="15"/>
+      <c r="H87" s="16"/>
+      <c r="I87" s="16"/>
+      <c r="J87" s="17"/>
+      <c r="K87" s="13"/>
+      <c r="L87" s="16"/>
+      <c r="M87" s="16"/>
+      <c r="N87" s="16"/>
+      <c r="O87" s="27"/>
+    </row>
+    <row r="88" spans="3:15" ht="18" customHeight="1">
+      <c r="C88" s="53"/>
+      <c r="D88" s="22"/>
+      <c r="E88" s="18"/>
+      <c r="F88" s="19"/>
+      <c r="G88" s="20"/>
+      <c r="H88" s="21"/>
+      <c r="I88" s="21"/>
+      <c r="J88" s="22"/>
+      <c r="K88" s="18"/>
+      <c r="L88" s="21"/>
+      <c r="M88" s="21"/>
+      <c r="N88" s="21"/>
+      <c r="O88" s="26"/>
+    </row>
+    <row r="89" spans="3:15" ht="18" customHeight="1">
+      <c r="C89" s="52"/>
+      <c r="D89" s="17"/>
+      <c r="E89" s="13"/>
+      <c r="F89" s="14"/>
+      <c r="G89" s="15"/>
+      <c r="H89" s="16"/>
+      <c r="I89" s="16"/>
+      <c r="J89" s="17"/>
+      <c r="K89" s="13"/>
+      <c r="L89" s="16"/>
+      <c r="M89" s="16"/>
+      <c r="N89" s="16"/>
+      <c r="O89" s="27"/>
+    </row>
+    <row r="90" spans="3:15" ht="18" customHeight="1">
+      <c r="C90" s="53"/>
+      <c r="D90" s="22"/>
+      <c r="E90" s="18"/>
+      <c r="F90" s="19"/>
+      <c r="G90" s="20"/>
+      <c r="H90" s="21"/>
+      <c r="I90" s="21"/>
+      <c r="J90" s="22"/>
+      <c r="K90" s="18"/>
+      <c r="L90" s="21"/>
+      <c r="M90" s="21"/>
+      <c r="N90" s="21"/>
+      <c r="O90" s="26"/>
+    </row>
+    <row r="91" spans="3:15" ht="18" customHeight="1">
+      <c r="C91" s="52"/>
+      <c r="D91" s="17"/>
+      <c r="E91" s="13"/>
+      <c r="F91" s="14"/>
+      <c r="G91" s="15"/>
+      <c r="H91" s="16"/>
+      <c r="I91" s="16"/>
+      <c r="J91" s="17"/>
+      <c r="K91" s="13"/>
+      <c r="L91" s="16"/>
+      <c r="M91" s="16"/>
+      <c r="N91" s="16"/>
+      <c r="O91" s="27"/>
+    </row>
+    <row r="92" spans="3:15" ht="18" customHeight="1">
+      <c r="C92" s="53"/>
+      <c r="D92" s="22"/>
+      <c r="E92" s="18"/>
+      <c r="F92" s="19"/>
+      <c r="G92" s="20"/>
+      <c r="H92" s="21"/>
+      <c r="I92" s="21"/>
+      <c r="J92" s="22"/>
+      <c r="K92" s="18"/>
+      <c r="L92" s="21"/>
+      <c r="M92" s="21"/>
+      <c r="N92" s="21"/>
+      <c r="O92" s="26"/>
+    </row>
+    <row r="93" spans="3:15" ht="18" customHeight="1">
+      <c r="C93" s="52"/>
+      <c r="D93" s="17"/>
+      <c r="E93" s="13"/>
+      <c r="F93" s="14"/>
+      <c r="G93" s="15"/>
+      <c r="H93" s="16"/>
+      <c r="I93" s="16"/>
+      <c r="J93" s="17"/>
+      <c r="K93" s="13"/>
+      <c r="L93" s="16"/>
+      <c r="M93" s="16"/>
+      <c r="N93" s="16"/>
+      <c r="O93" s="27"/>
+    </row>
+    <row r="94" spans="3:15" ht="18" customHeight="1">
+      <c r="C94" s="53"/>
+      <c r="D94" s="22"/>
+      <c r="E94" s="18"/>
+      <c r="F94" s="19"/>
+      <c r="G94" s="20"/>
+      <c r="H94" s="21"/>
+      <c r="I94" s="21"/>
+      <c r="J94" s="22"/>
+      <c r="K94" s="18"/>
+      <c r="L94" s="21"/>
+      <c r="M94" s="21"/>
+      <c r="N94" s="21"/>
+      <c r="O94" s="26"/>
+    </row>
+    <row r="95" spans="3:15" ht="18" customHeight="1">
+      <c r="C95" s="52"/>
+      <c r="D95" s="17"/>
+      <c r="E95" s="13"/>
+      <c r="F95" s="14"/>
+      <c r="G95" s="15"/>
+      <c r="H95" s="16"/>
+      <c r="I95" s="16"/>
+      <c r="J95" s="17"/>
+      <c r="K95" s="13"/>
+      <c r="L95" s="16"/>
+      <c r="M95" s="16"/>
+      <c r="N95" s="16"/>
+      <c r="O95" s="27"/>
+    </row>
+    <row r="96" spans="3:15" ht="18" customHeight="1">
+      <c r="C96" s="53"/>
+      <c r="D96" s="22"/>
+      <c r="E96" s="18"/>
+      <c r="F96" s="19"/>
+      <c r="G96" s="20"/>
+      <c r="H96" s="21"/>
+      <c r="I96" s="21"/>
+      <c r="J96" s="22"/>
+      <c r="K96" s="18"/>
+      <c r="L96" s="21"/>
+      <c r="M96" s="21"/>
+      <c r="N96" s="21"/>
+      <c r="O96" s="26"/>
+    </row>
+    <row r="97" spans="3:15" ht="18" customHeight="1">
+      <c r="C97" s="52"/>
+      <c r="D97" s="17"/>
+      <c r="E97" s="13"/>
+      <c r="F97" s="14"/>
+      <c r="G97" s="15"/>
+      <c r="H97" s="16"/>
+      <c r="I97" s="16"/>
+      <c r="J97" s="17"/>
+      <c r="K97" s="13"/>
+      <c r="L97" s="16"/>
+      <c r="M97" s="16"/>
+      <c r="N97" s="16"/>
+      <c r="O97" s="27"/>
+    </row>
+    <row r="98" spans="3:15" ht="18" customHeight="1">
+      <c r="C98" s="53"/>
+      <c r="D98" s="22"/>
+      <c r="E98" s="18"/>
+      <c r="F98" s="19"/>
+      <c r="G98" s="20"/>
+      <c r="H98" s="21"/>
+      <c r="I98" s="21"/>
+      <c r="J98" s="22"/>
+      <c r="K98" s="18"/>
+      <c r="L98" s="21"/>
+      <c r="M98" s="21"/>
+      <c r="N98" s="21"/>
+      <c r="O98" s="26"/>
+    </row>
+    <row r="99" spans="3:15" ht="18" customHeight="1">
+      <c r="C99" s="52"/>
+      <c r="D99" s="17"/>
+      <c r="E99" s="13"/>
+      <c r="F99" s="14"/>
+      <c r="G99" s="15"/>
+      <c r="H99" s="16"/>
+      <c r="I99" s="16"/>
+      <c r="J99" s="17"/>
+      <c r="K99" s="13"/>
+      <c r="L99" s="16"/>
+      <c r="M99" s="16"/>
+      <c r="N99" s="16"/>
+      <c r="O99" s="27"/>
+    </row>
+    <row r="100" spans="3:15" ht="18" customHeight="1">
+      <c r="C100" s="53"/>
+      <c r="D100" s="22"/>
+      <c r="E100" s="18"/>
+      <c r="F100" s="19"/>
+      <c r="G100" s="20"/>
+      <c r="H100" s="21"/>
+      <c r="I100" s="21"/>
+      <c r="J100" s="22"/>
+      <c r="K100" s="18"/>
+      <c r="L100" s="21"/>
+      <c r="M100" s="21"/>
+      <c r="N100" s="21"/>
+      <c r="O100" s="26"/>
+    </row>
+    <row r="101" spans="3:15" ht="18" customHeight="1">
+      <c r="C101" s="52"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="13"/>
+      <c r="F101" s="14"/>
+      <c r="G101" s="15"/>
+      <c r="H101" s="16"/>
+      <c r="I101" s="16"/>
+      <c r="J101" s="17"/>
+      <c r="K101" s="13"/>
+      <c r="L101" s="16"/>
+      <c r="M101" s="16"/>
+      <c r="N101" s="16"/>
+      <c r="O101" s="27"/>
+    </row>
+    <row r="102" spans="3:15" ht="18" customHeight="1">
+      <c r="C102" s="53"/>
+      <c r="D102" s="22"/>
+      <c r="E102" s="18"/>
+      <c r="F102" s="19"/>
+      <c r="G102" s="20"/>
+      <c r="H102" s="21"/>
+      <c r="I102" s="21"/>
+      <c r="J102" s="22"/>
+      <c r="K102" s="18"/>
+      <c r="L102" s="21"/>
+      <c r="M102" s="21"/>
+      <c r="N102" s="21"/>
+      <c r="O102" s="26"/>
+    </row>
+    <row r="103" spans="3:15" ht="18" customHeight="1">
+      <c r="C103" s="52"/>
+      <c r="D103" s="17"/>
+      <c r="E103" s="13"/>
+      <c r="F103" s="14"/>
+      <c r="G103" s="15"/>
+      <c r="H103" s="16"/>
+      <c r="I103" s="16"/>
+      <c r="J103" s="17"/>
+      <c r="K103" s="13"/>
+      <c r="L103" s="16"/>
+      <c r="M103" s="16"/>
+      <c r="N103" s="16"/>
+      <c r="O103" s="27"/>
+    </row>
+    <row r="104" spans="3:15" ht="18" customHeight="1">
+      <c r="C104" s="53"/>
+      <c r="D104" s="22"/>
+      <c r="E104" s="18"/>
+      <c r="F104" s="19"/>
+      <c r="G104" s="20"/>
+      <c r="H104" s="21"/>
+      <c r="I104" s="21"/>
+      <c r="J104" s="22"/>
+      <c r="K104" s="18"/>
+      <c r="L104" s="21"/>
+      <c r="M104" s="21"/>
+      <c r="N104" s="21"/>
+      <c r="O104" s="26"/>
+    </row>
+    <row r="105" spans="3:15" ht="18" customHeight="1">
+      <c r="C105" s="52"/>
+      <c r="D105" s="17"/>
+      <c r="E105" s="13"/>
+      <c r="F105" s="14"/>
+      <c r="G105" s="15"/>
+      <c r="H105" s="16"/>
+      <c r="I105" s="16"/>
+      <c r="J105" s="17"/>
+      <c r="K105" s="13"/>
+      <c r="L105" s="16"/>
+      <c r="M105" s="16"/>
+      <c r="N105" s="16"/>
+      <c r="O105" s="27"/>
+    </row>
+    <row r="106" spans="3:15" ht="18" customHeight="1">
+      <c r="C106" s="51"/>
+      <c r="D106" s="32"/>
+      <c r="E106" s="35"/>
+      <c r="F106" s="36"/>
+      <c r="G106" s="28"/>
+      <c r="H106" s="29"/>
+      <c r="I106" s="29"/>
+      <c r="J106" s="30"/>
+      <c r="K106" s="37"/>
+      <c r="L106" s="29"/>
+      <c r="M106" s="29"/>
+      <c r="N106" s="29"/>
+      <c r="O106" s="26"/>
+    </row>
+    <row r="107" spans="3:15" ht="18" customHeight="1">
+      <c r="C107" s="52"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="13"/>
+      <c r="F107" s="14"/>
+      <c r="G107" s="15"/>
+      <c r="H107" s="16"/>
+      <c r="I107" s="16"/>
+      <c r="J107" s="17"/>
+      <c r="K107" s="13"/>
+      <c r="L107" s="16"/>
+      <c r="M107" s="16"/>
+      <c r="N107" s="16"/>
+      <c r="O107" s="27"/>
+    </row>
+    <row r="108" spans="3:15" ht="18" customHeight="1">
+      <c r="C108" s="53"/>
+      <c r="D108" s="22"/>
+      <c r="E108" s="18"/>
+      <c r="F108" s="19"/>
+      <c r="G108" s="20"/>
+      <c r="H108" s="21"/>
+      <c r="I108" s="21"/>
+      <c r="J108" s="22"/>
+      <c r="K108" s="18"/>
+      <c r="L108" s="21"/>
+      <c r="M108" s="21"/>
+      <c r="N108" s="21"/>
+      <c r="O108" s="26"/>
+    </row>
+    <row r="109" spans="3:15" ht="18" customHeight="1">
+      <c r="C109" s="52"/>
+      <c r="D109" s="17"/>
+      <c r="E109" s="13"/>
+      <c r="F109" s="14"/>
+      <c r="G109" s="15"/>
+      <c r="H109" s="16"/>
+      <c r="I109" s="16"/>
+      <c r="J109" s="17"/>
+      <c r="K109" s="13"/>
+      <c r="L109" s="16"/>
+      <c r="M109" s="16"/>
+      <c r="N109" s="16"/>
+      <c r="O109" s="27"/>
+    </row>
+    <row r="110" spans="3:15" ht="18" customHeight="1">
+      <c r="C110" s="53"/>
+      <c r="D110" s="22"/>
+      <c r="E110" s="18"/>
+      <c r="F110" s="19"/>
+      <c r="G110" s="20"/>
+      <c r="H110" s="21"/>
+      <c r="I110" s="21"/>
+      <c r="J110" s="22"/>
+      <c r="K110" s="18"/>
+      <c r="L110" s="21"/>
+      <c r="M110" s="21"/>
+      <c r="N110" s="21"/>
+      <c r="O110" s="26"/>
+    </row>
+    <row r="111" spans="3:15" ht="18" customHeight="1">
+      <c r="C111" s="52"/>
+      <c r="D111" s="17"/>
+      <c r="E111" s="13"/>
+      <c r="F111" s="14"/>
+      <c r="G111" s="15"/>
+      <c r="H111" s="16"/>
+      <c r="I111" s="16"/>
+      <c r="J111" s="17"/>
+      <c r="K111" s="13"/>
+      <c r="L111" s="16"/>
+      <c r="M111" s="16"/>
+      <c r="N111" s="16"/>
+      <c r="O111" s="27"/>
+    </row>
+    <row r="112" spans="3:15" ht="18" customHeight="1">
+      <c r="C112" s="53"/>
+      <c r="D112" s="22"/>
+      <c r="E112" s="18"/>
+      <c r="F112" s="19"/>
+      <c r="G112" s="20"/>
+      <c r="H112" s="21"/>
+      <c r="I112" s="21"/>
+      <c r="J112" s="22"/>
+      <c r="K112" s="18"/>
+      <c r="L112" s="21"/>
+      <c r="M112" s="21"/>
+      <c r="N112" s="21"/>
+      <c r="O112" s="26"/>
+    </row>
+    <row r="113" spans="3:15" ht="18" customHeight="1">
+      <c r="C113" s="52"/>
+      <c r="D113" s="17"/>
+      <c r="E113" s="13"/>
+      <c r="F113" s="14"/>
+      <c r="G113" s="15"/>
+      <c r="H113" s="16"/>
+      <c r="I113" s="16"/>
+      <c r="J113" s="17"/>
+      <c r="K113" s="13"/>
+      <c r="L113" s="16"/>
+      <c r="M113" s="16"/>
+      <c r="N113" s="16"/>
+      <c r="O113" s="27"/>
+    </row>
+    <row r="114" spans="3:15" ht="18" customHeight="1">
+      <c r="C114" s="53"/>
+      <c r="D114" s="22"/>
+      <c r="E114" s="18"/>
+      <c r="F114" s="19"/>
+      <c r="G114" s="20"/>
+      <c r="H114" s="21"/>
+      <c r="I114" s="21"/>
+      <c r="J114" s="22"/>
+      <c r="K114" s="18"/>
+      <c r="L114" s="21"/>
+      <c r="M114" s="21"/>
+      <c r="N114" s="21"/>
+      <c r="O114" s="26"/>
+    </row>
+    <row r="115" spans="3:15" ht="18" customHeight="1">
+      <c r="C115" s="52"/>
+      <c r="D115" s="17"/>
+      <c r="E115" s="13"/>
+      <c r="F115" s="14"/>
+      <c r="G115" s="15"/>
+      <c r="H115" s="16"/>
+      <c r="I115" s="16"/>
+      <c r="J115" s="17"/>
+      <c r="K115" s="13"/>
+      <c r="L115" s="16"/>
+      <c r="M115" s="16"/>
+      <c r="N115" s="16"/>
+      <c r="O115" s="27"/>
+    </row>
+    <row r="116" spans="3:15" ht="18" customHeight="1">
+      <c r="C116" s="53"/>
+      <c r="D116" s="22"/>
+      <c r="E116" s="18"/>
+      <c r="F116" s="19"/>
+      <c r="G116" s="20"/>
+      <c r="H116" s="21"/>
+      <c r="I116" s="21"/>
+      <c r="J116" s="22"/>
+      <c r="K116" s="18"/>
+      <c r="L116" s="21"/>
+      <c r="M116" s="21"/>
+      <c r="N116" s="21"/>
+      <c r="O116" s="26"/>
+    </row>
+    <row r="117" spans="3:15" ht="18" customHeight="1">
+      <c r="C117" s="52"/>
+      <c r="D117" s="17"/>
+      <c r="E117" s="13"/>
+      <c r="F117" s="14"/>
+      <c r="G117" s="15"/>
+      <c r="H117" s="16"/>
+      <c r="I117" s="16"/>
+      <c r="J117" s="17"/>
+      <c r="K117" s="13"/>
+      <c r="L117" s="16"/>
+      <c r="M117" s="16"/>
+      <c r="N117" s="16"/>
+      <c r="O117" s="27"/>
+    </row>
+    <row r="118" spans="3:15" ht="18" customHeight="1">
+      <c r="C118" s="53"/>
+      <c r="D118" s="22"/>
+      <c r="E118" s="18"/>
+      <c r="F118" s="19"/>
+      <c r="G118" s="20"/>
+      <c r="H118" s="21"/>
+      <c r="I118" s="21"/>
+      <c r="J118" s="22"/>
+      <c r="K118" s="18"/>
+      <c r="L118" s="21"/>
+      <c r="M118" s="21"/>
+      <c r="N118" s="21"/>
+      <c r="O118" s="26"/>
+    </row>
+    <row r="119" spans="3:15" ht="18" customHeight="1">
+      <c r="C119" s="52"/>
+      <c r="D119" s="17"/>
+      <c r="E119" s="13"/>
+      <c r="F119" s="14"/>
+      <c r="G119" s="15"/>
+      <c r="H119" s="16"/>
+      <c r="I119" s="16"/>
+      <c r="J119" s="17"/>
+      <c r="K119" s="13"/>
+      <c r="L119" s="16"/>
+      <c r="M119" s="16"/>
+      <c r="N119" s="16"/>
+      <c r="O119" s="27"/>
+    </row>
+    <row r="120" spans="3:15" ht="18" customHeight="1">
+      <c r="C120" s="53"/>
+      <c r="D120" s="22"/>
+      <c r="E120" s="18"/>
+      <c r="F120" s="19"/>
+      <c r="G120" s="20"/>
+      <c r="H120" s="21"/>
+      <c r="I120" s="21"/>
+      <c r="J120" s="22"/>
+      <c r="K120" s="18"/>
+      <c r="L120" s="21"/>
+      <c r="M120" s="21"/>
+      <c r="N120" s="21"/>
+      <c r="O120" s="26"/>
+    </row>
+    <row r="121" spans="3:15" ht="18" customHeight="1">
+      <c r="C121" s="52"/>
+      <c r="D121" s="17"/>
+      <c r="E121" s="13"/>
+      <c r="F121" s="14"/>
+      <c r="G121" s="15"/>
+      <c r="H121" s="16"/>
+      <c r="I121" s="16"/>
+      <c r="J121" s="17"/>
+      <c r="K121" s="13"/>
+      <c r="L121" s="16"/>
+      <c r="M121" s="16"/>
+      <c r="N121" s="16"/>
+      <c r="O121" s="27"/>
+    </row>
+    <row r="122" spans="3:15" ht="18" customHeight="1">
+      <c r="C122" s="53"/>
+      <c r="D122" s="22"/>
+      <c r="E122" s="18"/>
+      <c r="F122" s="19"/>
+      <c r="G122" s="20"/>
+      <c r="H122" s="21"/>
+      <c r="I122" s="21"/>
+      <c r="J122" s="22"/>
+      <c r="K122" s="18"/>
+      <c r="L122" s="21"/>
+      <c r="M122" s="21"/>
+      <c r="N122" s="21"/>
+      <c r="O122" s="26"/>
+    </row>
+    <row r="123" spans="3:15" ht="18" customHeight="1">
+      <c r="C123" s="52"/>
+      <c r="D123" s="17"/>
+      <c r="E123" s="13"/>
+      <c r="F123" s="14"/>
+      <c r="G123" s="15"/>
+      <c r="H123" s="16"/>
+      <c r="I123" s="16"/>
+      <c r="J123" s="17"/>
+      <c r="K123" s="13"/>
+      <c r="L123" s="16"/>
+      <c r="M123" s="16"/>
+      <c r="N123" s="16"/>
+      <c r="O123" s="27"/>
+    </row>
+    <row r="124" spans="3:15" ht="18" customHeight="1">
+      <c r="C124" s="53"/>
+      <c r="D124" s="22"/>
+      <c r="E124" s="18"/>
+      <c r="F124" s="19"/>
+      <c r="G124" s="20"/>
+      <c r="H124" s="21"/>
+      <c r="I124" s="21"/>
+      <c r="J124" s="22"/>
+      <c r="K124" s="18"/>
+      <c r="L124" s="21"/>
+      <c r="M124" s="21"/>
+      <c r="N124" s="21"/>
+      <c r="O124" s="26"/>
+    </row>
+    <row r="125" spans="3:15" ht="18" customHeight="1">
+      <c r="C125" s="52"/>
+      <c r="D125" s="17"/>
+      <c r="E125" s="13"/>
+      <c r="F125" s="14"/>
+      <c r="G125" s="15"/>
+      <c r="H125" s="16"/>
+      <c r="I125" s="16"/>
+      <c r="J125" s="17"/>
+      <c r="K125" s="13"/>
+      <c r="L125" s="16"/>
+      <c r="M125" s="16"/>
+      <c r="N125" s="16"/>
+      <c r="O125" s="27"/>
+    </row>
+    <row r="126" spans="3:15" ht="18" customHeight="1">
+      <c r="C126" s="53"/>
+      <c r="D126" s="22"/>
+      <c r="E126" s="18"/>
+      <c r="F126" s="19"/>
+      <c r="G126" s="20"/>
+      <c r="H126" s="21"/>
+      <c r="I126" s="21"/>
+      <c r="J126" s="22"/>
+      <c r="K126" s="18"/>
+      <c r="L126" s="21"/>
+      <c r="M126" s="21"/>
+      <c r="N126" s="21"/>
+      <c r="O126" s="26"/>
+    </row>
+    <row r="127" spans="3:15" ht="18" customHeight="1">
+      <c r="C127" s="52"/>
+      <c r="D127" s="17"/>
+      <c r="E127" s="13"/>
+      <c r="F127" s="14"/>
+      <c r="G127" s="15"/>
+      <c r="H127" s="16"/>
+      <c r="I127" s="16"/>
+      <c r="J127" s="17"/>
+      <c r="K127" s="13"/>
+      <c r="L127" s="16"/>
+      <c r="M127" s="16"/>
+      <c r="N127" s="16"/>
+      <c r="O127" s="27"/>
+    </row>
+    <row r="128" spans="3:15" ht="18" customHeight="1">
+      <c r="C128" s="53"/>
+      <c r="D128" s="22"/>
+      <c r="E128" s="18"/>
+      <c r="F128" s="19"/>
+      <c r="G128" s="20"/>
+      <c r="H128" s="21"/>
+      <c r="I128" s="21"/>
+      <c r="J128" s="22"/>
+      <c r="K128" s="18"/>
+      <c r="L128" s="21"/>
+      <c r="M128" s="21"/>
+      <c r="N128" s="21"/>
+      <c r="O128" s="26"/>
+    </row>
+    <row r="129" spans="3:15" ht="18" customHeight="1">
+      <c r="C129" s="52"/>
+      <c r="D129" s="17"/>
+      <c r="E129" s="13"/>
+      <c r="F129" s="14"/>
+      <c r="G129" s="15"/>
+      <c r="H129" s="16"/>
+      <c r="I129" s="16"/>
+      <c r="J129" s="17"/>
+      <c r="K129" s="13"/>
+      <c r="L129" s="16"/>
+      <c r="M129" s="16"/>
+      <c r="N129" s="16"/>
+      <c r="O129" s="27"/>
+    </row>
+    <row r="130" spans="3:15" ht="18" customHeight="1">
+      <c r="C130" s="53"/>
+      <c r="D130" s="22"/>
+      <c r="E130" s="18"/>
+      <c r="F130" s="19"/>
+      <c r="G130" s="20"/>
+      <c r="H130" s="21"/>
+      <c r="I130" s="21"/>
+      <c r="J130" s="22"/>
+      <c r="K130" s="18"/>
+      <c r="L130" s="21"/>
+      <c r="M130" s="21"/>
+      <c r="N130" s="21"/>
+      <c r="O130" s="26"/>
+    </row>
+    <row r="131" spans="3:15" ht="18" customHeight="1">
+      <c r="C131" s="52"/>
+      <c r="D131" s="17"/>
+      <c r="E131" s="13"/>
+      <c r="F131" s="14"/>
+      <c r="G131" s="15"/>
+      <c r="H131" s="16"/>
+      <c r="I131" s="16"/>
+      <c r="J131" s="17"/>
+      <c r="K131" s="13"/>
+      <c r="L131" s="16"/>
+      <c r="M131" s="16"/>
+      <c r="N131" s="16"/>
+      <c r="O131" s="27"/>
+    </row>
+    <row r="132" spans="3:15" ht="18" customHeight="1">
+      <c r="C132" s="53"/>
+      <c r="D132" s="22"/>
+      <c r="E132" s="18"/>
+      <c r="F132" s="19"/>
+      <c r="G132" s="20"/>
+      <c r="H132" s="21"/>
+      <c r="I132" s="21"/>
+      <c r="J132" s="22"/>
+      <c r="K132" s="18"/>
+      <c r="L132" s="21"/>
+      <c r="M132" s="21"/>
+      <c r="N132" s="21"/>
+      <c r="O132" s="26"/>
+    </row>
+    <row r="133" spans="3:15" ht="18" customHeight="1">
+      <c r="C133" s="52"/>
+      <c r="D133" s="17"/>
+      <c r="E133" s="13"/>
+      <c r="F133" s="14"/>
+      <c r="G133" s="15"/>
+      <c r="H133" s="16"/>
+      <c r="I133" s="16"/>
+      <c r="J133" s="17"/>
+      <c r="K133" s="13"/>
+      <c r="L133" s="16"/>
+      <c r="M133" s="16"/>
+      <c r="N133" s="16"/>
+      <c r="O133" s="27"/>
+    </row>
+    <row r="134" spans="3:15" ht="18" customHeight="1">
+      <c r="C134" s="53"/>
+      <c r="D134" s="22"/>
+      <c r="E134" s="18"/>
+      <c r="F134" s="19"/>
+      <c r="G134" s="20"/>
+      <c r="H134" s="21"/>
+      <c r="I134" s="21"/>
+      <c r="J134" s="22"/>
+      <c r="K134" s="18"/>
+      <c r="L134" s="21"/>
+      <c r="M134" s="21"/>
+      <c r="N134" s="21"/>
+      <c r="O134" s="26"/>
+    </row>
+    <row r="135" spans="3:15" ht="18" customHeight="1">
+      <c r="C135" s="52"/>
+      <c r="D135" s="17"/>
+      <c r="E135" s="13"/>
+      <c r="F135" s="14"/>
+      <c r="G135" s="15"/>
+      <c r="H135" s="16"/>
+      <c r="I135" s="16"/>
+      <c r="J135" s="17"/>
+      <c r="K135" s="13"/>
+      <c r="L135" s="16"/>
+      <c r="M135" s="16"/>
+      <c r="N135" s="16"/>
+      <c r="O135" s="27"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="18">
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="G71:J71"/>
+    <mergeCell ref="K71:N71"/>
+    <mergeCell ref="O71:O73"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="K72:L72"/>
+    <mergeCell ref="M72:N72"/>
     <mergeCell ref="O3:O5"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
@@ -45610,11 +46717,14 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="64" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="32" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;10日通システム株式会社 &amp;C&amp;"ＭＳ ゴシック,Regular"&amp;16標準報酬月額表（厚生年金）&amp;R&amp;"ＭＳ ゴシック,Regular"&amp;10&amp;KFF0000 &amp;K01+000&amp;D　&amp;T　
 &amp;KFF0000 &amp;K01+000page&amp;P</oddHeader>
   </headerFooter>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="68" max="16383" man="1"/>
+  </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[SMAL] Change the file output format to pdf instead of xlsx QMM007 + QMM008 Screen F
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_標準報酬月額表（厚生年金).xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_標準報酬月額表（厚生年金).xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="マスタリスト" sheetId="11" r:id="rId1"/>
+    <sheet name="マスタリスト (2)" sheetId="12" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
@@ -26,18 +26,29 @@
     <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
     <externalReference r:id="rId12"/>
+    <externalReference r:id="rId13"/>
   </externalReferences>
   <definedNames>
+    <definedName name="_Fill" localSheetId="1" hidden="1">#REF!</definedName>
     <definedName name="_Fill" hidden="1">#REF!</definedName>
+    <definedName name="_Key1" localSheetId="1" hidden="1">#REF!</definedName>
     <definedName name="_Key1" hidden="1">#REF!</definedName>
     <definedName name="_Order1" hidden="1">255</definedName>
+    <definedName name="_Parse_In" localSheetId="1" hidden="1">#REF!</definedName>
     <definedName name="_Parse_In" hidden="1">#REF!</definedName>
+    <definedName name="_Parse_Out" localSheetId="1" hidden="1">#REF!</definedName>
     <definedName name="_Parse_Out" hidden="1">#REF!</definedName>
+    <definedName name="_Regression_X" localSheetId="1" hidden="1">#REF!</definedName>
     <definedName name="_Regression_X" hidden="1">#REF!</definedName>
+    <definedName name="_Sort" localSheetId="1" hidden="1">#REF!</definedName>
     <definedName name="_Sort" hidden="1">#REF!</definedName>
+    <definedName name="_面接から採用に至るまでの情報管理とする_____アウトソーシングにて_採用された情報を_ファイ__ルにて取込を行う_" localSheetId="1">#REF!</definedName>
     <definedName name="_面接から採用に至るまでの情報管理とする_____アウトソーシングにて_採用された情報を_ファイ__ルにて取込を行う_">#REF!</definedName>
+    <definedName name="・面接から採用に至るまでの情報管理とする。___・アウトソーシングにて_採用された情報を_ファイ__ルにて取込を行う。" localSheetId="1">#REF!</definedName>
     <definedName name="・面接から採用に至るまでの情報管理とする。___・アウトソーシングにて_採用された情報を_ファイ__ルにて取込を行う。">#REF!</definedName>
+    <definedName name="a" localSheetId="1">[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
     <definedName name="a">[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="AAA" localSheetId="1">#REF!</definedName>
     <definedName name="AAA">#REF!</definedName>
     <definedName name="AAAA" hidden="1">{"VIEW1",#N/A,FALSE,"懸案事項";"VIEW2",#N/A,FALSE,"懸案事項"}</definedName>
     <definedName name="abc" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
@@ -45,120 +56,211 @@
     <definedName name="ｂｂｂ" hidden="1">{"VIEW1",#N/A,FALSE,"懸案事項";"VIEW2",#N/A,FALSE,"懸案事項"}</definedName>
     <definedName name="ｂｂｂｂ" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="ｃｃｃｃ" hidden="1">{"VIEW1",#N/A,FALSE,"懸案事項";"VIEW2",#N/A,FALSE,"懸案事項"}</definedName>
+    <definedName name="C保守単価" localSheetId="1">'[2]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="C保守単価">'[2]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="C保守委託単価" localSheetId="1">'[2]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="C保守委託単価">'[2]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="C保守支援単価" localSheetId="1">'[2]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="C保守支援単価">'[2]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="DDDD" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="def" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="e" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
+    <definedName name="ｈｈｈ" localSheetId="1">#REF!</definedName>
     <definedName name="ｈｈｈ">#REF!</definedName>
     <definedName name="HW9707K">[3]仕切価格!$B$1:$BD$231</definedName>
+    <definedName name="ＩＨ" localSheetId="1">#REF!</definedName>
     <definedName name="ＩＨ">#REF!</definedName>
+    <definedName name="item1" localSheetId="1">#REF!</definedName>
     <definedName name="item1">#REF!</definedName>
+    <definedName name="Ｉホ" localSheetId="1">#REF!</definedName>
     <definedName name="Ｉホ">#REF!</definedName>
     <definedName name="k" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
+    <definedName name="kkkk" localSheetId="1" hidden="1">#REF!</definedName>
     <definedName name="kkkk" hidden="1">#REF!</definedName>
     <definedName name="ｌ" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
+    <definedName name="ＬＨ" localSheetId="1">#REF!</definedName>
     <definedName name="ＬＨ">#REF!</definedName>
+    <definedName name="ＬサＨ" localSheetId="1">#REF!</definedName>
     <definedName name="ＬサＨ">#REF!</definedName>
+    <definedName name="Ｌサホ" localSheetId="1">#REF!</definedName>
     <definedName name="Ｌサホ">#REF!</definedName>
+    <definedName name="ＬニＨ" localSheetId="1">#REF!</definedName>
     <definedName name="ＬニＨ">#REF!</definedName>
+    <definedName name="Ｌニホ" localSheetId="1">#REF!</definedName>
     <definedName name="Ｌニホ">#REF!</definedName>
+    <definedName name="Ｌホ" localSheetId="1">#REF!</definedName>
     <definedName name="Ｌホ">#REF!</definedName>
+    <definedName name="ＭＨ" localSheetId="1">#REF!</definedName>
     <definedName name="ＭＨ">#REF!</definedName>
+    <definedName name="Ｍホ" localSheetId="1">#REF!</definedName>
     <definedName name="Ｍホ">#REF!</definedName>
+    <definedName name="ｎ" localSheetId="1">[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
     <definedName name="ｎ">[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="ＯＨ" localSheetId="1">#REF!</definedName>
     <definedName name="ＯＨ">#REF!</definedName>
+    <definedName name="OPT_NO" localSheetId="1">[5]!OPT_NO</definedName>
     <definedName name="OPT_NO">[5]!OPT_NO</definedName>
+    <definedName name="OPT_YES" localSheetId="1">[5]!OPT_YES</definedName>
     <definedName name="OPT_YES">[5]!OPT_YES</definedName>
+    <definedName name="Ｏホ" localSheetId="1">#REF!</definedName>
     <definedName name="Ｏホ">#REF!</definedName>
+    <definedName name="PG単価" localSheetId="1">[6]明細合計!#REF!</definedName>
     <definedName name="PG単価">[6]明細合計!#REF!</definedName>
+    <definedName name="PG田中" localSheetId="1">#REF!</definedName>
     <definedName name="PG田中">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">マスタリスト!$A$1:$P$67</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'マスタリスト (2)'!$A$1:$P$67</definedName>
+    <definedName name="PrintDaicho" localSheetId="1">[7]!PrintDaicho</definedName>
     <definedName name="PrintDaicho">[7]!PrintDaicho</definedName>
+    <definedName name="QuitDaicho" localSheetId="1">[7]!QuitDaicho</definedName>
     <definedName name="QuitDaicho">[7]!QuitDaicho</definedName>
+    <definedName name="SE単価" localSheetId="1">[6]明細合計!#REF!</definedName>
     <definedName name="SE単価">[6]明細合計!#REF!</definedName>
+    <definedName name="sss" localSheetId="1" hidden="1">#REF!</definedName>
     <definedName name="sss" hidden="1">#REF!</definedName>
+    <definedName name="SS単価" localSheetId="1">#REF!</definedName>
     <definedName name="SS単価">#REF!</definedName>
+    <definedName name="STEP概算" localSheetId="1">#REF!</definedName>
     <definedName name="STEP概算">#REF!</definedName>
+    <definedName name="ＳＷ" localSheetId="1">#REF!</definedName>
     <definedName name="ＳＷ">#REF!</definedName>
+    <definedName name="Ver002001006特休残管理対応" localSheetId="1" hidden="1">#REF!</definedName>
     <definedName name="Ver002001006特休残管理対応" hidden="1">#REF!</definedName>
+    <definedName name="ｗ" localSheetId="1">'[2]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="ｗ">'[2]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="WC単価">'[2]見積明細(ハードのみ）'!$X$5:$X$34</definedName>
     <definedName name="wrn.MIND." hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="wrn.PRINT_ALL." hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="wrn.REPORT1." hidden="1">{"VIEW1",#N/A,FALSE,"懸案事項";"VIEW2",#N/A,FALSE,"懸案事項"}</definedName>
+    <definedName name="あ" localSheetId="1">#REF!</definedName>
     <definedName name="あ">#REF!</definedName>
+    <definedName name="あ１" localSheetId="1">#REF!</definedName>
     <definedName name="あ１">#REF!</definedName>
     <definedName name="あああ" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
+    <definedName name="ああああああああああ" localSheetId="1">#REF!</definedName>
     <definedName name="ああああああああああ">#REF!</definedName>
+    <definedName name="い" localSheetId="1" hidden="1">#REF!</definedName>
     <definedName name="い" hidden="1">#REF!</definedName>
+    <definedName name="クＨ" localSheetId="1">#REF!</definedName>
     <definedName name="クＨ">#REF!</definedName>
+    <definedName name="クサＨ" localSheetId="1">#REF!</definedName>
     <definedName name="クサＨ">#REF!</definedName>
+    <definedName name="クサホ" localSheetId="1">#REF!</definedName>
     <definedName name="クサホ">#REF!</definedName>
+    <definedName name="クにＨ" localSheetId="1">#REF!</definedName>
     <definedName name="クにＨ">#REF!</definedName>
+    <definedName name="クニホ" localSheetId="1">#REF!</definedName>
     <definedName name="クニホ">#REF!</definedName>
+    <definedName name="クホ" localSheetId="1">#REF!</definedName>
     <definedName name="クホ">#REF!</definedName>
+    <definedName name="サＨ" localSheetId="1">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
     <definedName name="サＨ">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サホ" localSheetId="1">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
     <definedName name="サホ">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サホ1" localSheetId="1">#REF!</definedName>
     <definedName name="サホ1">#REF!</definedName>
+    <definedName name="ツール別見積工数" localSheetId="1">#REF!</definedName>
     <definedName name="ツール別見積工数">#REF!</definedName>
     <definedName name="テーブル項目">[9]項目定義書!$A$3:$E$364</definedName>
+    <definedName name="ハ１" localSheetId="1">#REF!</definedName>
     <definedName name="ハ１">#REF!</definedName>
+    <definedName name="は２" localSheetId="1">#REF!</definedName>
     <definedName name="は２">#REF!</definedName>
+    <definedName name="ハ２ホ" localSheetId="1">#REF!</definedName>
     <definedName name="ハ２ホ">#REF!</definedName>
+    <definedName name="は３" localSheetId="1">#REF!</definedName>
     <definedName name="は３">#REF!</definedName>
+    <definedName name="ハサホ" localSheetId="1">#REF!</definedName>
     <definedName name="ハサホ">#REF!</definedName>
+    <definedName name="ﾊﾞｽ･ﾀｸｼｰ" localSheetId="1">#REF!</definedName>
     <definedName name="ﾊﾞｽ･ﾀｸｼｰ">#REF!</definedName>
+    <definedName name="ハホ" localSheetId="1">#REF!</definedName>
     <definedName name="ハホ">#REF!</definedName>
+    <definedName name="ヘッダー" localSheetId="1">#REF!</definedName>
     <definedName name="ヘッダー">#REF!</definedName>
+    <definedName name="ユーザー一覧" localSheetId="1">'[10]工数計算(ﾈｯﾄﾜｰｸ）'!#REF!</definedName>
     <definedName name="ユーザー一覧">'[10]工数計算(ﾈｯﾄﾜｰｸ）'!#REF!</definedName>
+    <definedName name="一般社員時間外労働手当部門別集計ｸｴﾘｰ" localSheetId="1">#REF!</definedName>
     <definedName name="一般社員時間外労働手当部門別集計ｸｴﾘｰ">#REF!</definedName>
+    <definedName name="人日原価" localSheetId="1">#REF!</definedName>
     <definedName name="人日原価">#REF!</definedName>
     <definedName name="仕切り">'[2]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
     <definedName name="仕切単価">'[2]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
+    <definedName name="住民税115" localSheetId="1">#REF!</definedName>
     <definedName name="住民税115">#REF!</definedName>
+    <definedName name="住民税96" localSheetId="1">#REF!</definedName>
     <definedName name="住民税96">#REF!</definedName>
+    <definedName name="住民税納付先の登録7" localSheetId="1">#REF!</definedName>
     <definedName name="住民税納付先の登録7">#REF!</definedName>
+    <definedName name="価格表" localSheetId="1">#REF!</definedName>
     <definedName name="価格表">#REF!</definedName>
     <definedName name="保守単価">'[2]見積明細(ハードのみ）'!$L$5:$L$34</definedName>
     <definedName name="保守委託単価">'[2]見積明細(ハードのみ）'!$N$5:$N$34</definedName>
     <definedName name="保守支援単価">'[2]見積明細(ハードのみ）'!$P$5:$P$34</definedName>
     <definedName name="値引単価">'[2]見積明細(ハードのみ）'!$J$5:$J$34</definedName>
     <definedName name="備考">'[2]見積明細(ハードのみ）'!$AA$5:$AA$34</definedName>
+    <definedName name="単価" localSheetId="1">#REF!</definedName>
     <definedName name="単価">#REF!</definedName>
+    <definedName name="単価種別" localSheetId="1">#REF!</definedName>
     <definedName name="単価種別">#REF!</definedName>
+    <definedName name="原価" localSheetId="1">#REF!</definedName>
     <definedName name="原価">#REF!</definedName>
+    <definedName name="売値" localSheetId="1">#REF!</definedName>
     <definedName name="売値">#REF!</definedName>
+    <definedName name="定価" localSheetId="1">#REF!</definedName>
     <definedName name="定価">#REF!</definedName>
+    <definedName name="宿泊" localSheetId="1">#REF!</definedName>
     <definedName name="宿泊">#REF!</definedName>
+    <definedName name="宿泊単金" localSheetId="1">#REF!</definedName>
     <definedName name="宿泊単金">#REF!</definedName>
+    <definedName name="工程別生産性" localSheetId="1">#REF!</definedName>
     <definedName name="工程別生産性">#REF!</definedName>
+    <definedName name="日帰り" localSheetId="1">#REF!</definedName>
     <definedName name="日帰り">#REF!</definedName>
+    <definedName name="日帰り単金" localSheetId="1">#REF!</definedName>
     <definedName name="日帰り単金">#REF!</definedName>
+    <definedName name="概要_基準日設定" localSheetId="1" hidden="1">#REF!</definedName>
     <definedName name="概要_基準日設定" hidden="1">#REF!</definedName>
     <definedName name="標準価格">'[2]見積明細(ハードのみ）'!$C$5:$H$34</definedName>
     <definedName name="機種SORT">[11]!機種SORT</definedName>
+    <definedName name="機能別原価" localSheetId="1">#REF!</definedName>
     <definedName name="機能別原価">#REF!</definedName>
     <definedName name="直扱単価">'[2]見積明細(ハードのみ）'!$V$5:$V$34</definedName>
     <definedName name="社共単価">'[2]見積明細(ハードのみ）'!$T$5:$T$34</definedName>
+    <definedName name="種別" localSheetId="1">#REF!</definedName>
     <definedName name="種別">#REF!</definedName>
+    <definedName name="見積工数" localSheetId="1">#REF!</definedName>
     <definedName name="見積工数">#REF!</definedName>
     <definedName name="部">'[2]見積明細(ハードのみ）'!$Z$5:$Z$34</definedName>
+    <definedName name="部門別時間外労働手当状況" localSheetId="1">#REF!</definedName>
     <definedName name="部門別時間外労働手当状況">#REF!</definedName>
+    <definedName name="銀行の登録48" localSheetId="1">#REF!</definedName>
     <definedName name="銀行の登録48">#REF!</definedName>
+    <definedName name="銀行の登録67" localSheetId="1">#REF!</definedName>
     <definedName name="銀行の登録67">#REF!</definedName>
+    <definedName name="銀行の登録7" localSheetId="1">#REF!</definedName>
     <definedName name="銀行の登録7">#REF!</definedName>
+    <definedName name="関連表" localSheetId="1" hidden="1">#REF!</definedName>
     <definedName name="関連表" hidden="1">#REF!</definedName>
+    <definedName name="電車" localSheetId="1">#REF!</definedName>
     <definedName name="電車">#REF!</definedName>
+    <definedName name="項目名の登録1" localSheetId="1">#REF!</definedName>
     <definedName name="項目名の登録1">#REF!</definedName>
+    <definedName name="項目名の登録2" localSheetId="1">#REF!</definedName>
     <definedName name="項目名の登録2">#REF!</definedName>
+    <definedName name="項目名の登録3" localSheetId="1">#REF!</definedName>
     <definedName name="項目名の登録3">#REF!</definedName>
+    <definedName name="項目名の登録4" localSheetId="1">#REF!</definedName>
     <definedName name="項目名の登録4">#REF!</definedName>
+    <definedName name="項目名の登録5" localSheetId="1">#REF!</definedName>
     <definedName name="項目名の登録5">#REF!</definedName>
+    <definedName name="項目名の登録6" localSheetId="1">#REF!</definedName>
     <definedName name="項目名の登録6">#REF!</definedName>
+    <definedName name="項目名の登録7" localSheetId="1">#REF!</definedName>
     <definedName name="項目名の登録7">#REF!</definedName>
+    <definedName name="項目名の登録8" localSheetId="1">#REF!</definedName>
     <definedName name="項目名の登録8">#REF!</definedName>
+    <definedName name="飛行機" localSheetId="1">#REF!</definedName>
     <definedName name="飛行機">#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -838,6 +940,15 @@
     <xf numFmtId="40" fontId="4" fillId="0" borderId="30" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -876,15 +987,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -977,28 +1079,33 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>173212</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>5281</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>17518</xdr:colOff>
-      <xdr:row>135</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="角丸四角形 1"/>
+        <xdr:cNvPr id="2" name="角丸四角形 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="285271" y="218193"/>
-          <a:ext cx="9862365" cy="14562366"/>
+          <a:off x="287512" y="214831"/>
+          <a:ext cx="9855081" cy="14853719"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -44607,7 +44714,7 @@
   <sheetPr codeName="Sheet7">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:O135"/>
+  <dimension ref="B1:O67"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="85" workbookViewId="0"/>
   </sheetViews>
@@ -44642,27 +44749,27 @@
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="2:15" ht="18" customHeight="1">
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="41" t="s">
+      <c r="D3" s="43"/>
+      <c r="E3" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="42"/>
-      <c r="G3" s="43" t="s">
+      <c r="F3" s="45"/>
+      <c r="G3" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="43" t="s">
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="38" t="s">
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="41" t="s">
         <v>8</v>
       </c>
     </row>
@@ -44671,23 +44778,23 @@
       <c r="D4" s="23"/>
       <c r="E4" s="24"/>
       <c r="F4" s="25"/>
-      <c r="G4" s="47" t="s">
+      <c r="G4" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="48"/>
-      <c r="I4" s="49" t="s">
+      <c r="H4" s="51"/>
+      <c r="I4" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="50"/>
-      <c r="K4" s="47" t="s">
+      <c r="J4" s="53"/>
+      <c r="K4" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="48"/>
-      <c r="M4" s="49" t="s">
+      <c r="L4" s="51"/>
+      <c r="M4" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="50"/>
-      <c r="O4" s="38"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="41"/>
     </row>
     <row r="5" spans="2:15" ht="18" customHeight="1" thickBot="1">
       <c r="C5" s="5" t="s">
@@ -44726,10 +44833,10 @@
       <c r="N5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="38"/>
+      <c r="O5" s="41"/>
     </row>
     <row r="6" spans="2:15" ht="18" customHeight="1" thickTop="1">
-      <c r="C6" s="51"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="32"/>
       <c r="E6" s="11"/>
       <c r="F6" s="12"/>
@@ -44744,7 +44851,7 @@
       <c r="O6" s="26"/>
     </row>
     <row r="7" spans="2:15" ht="18" customHeight="1">
-      <c r="C7" s="52"/>
+      <c r="C7" s="39"/>
       <c r="D7" s="17"/>
       <c r="E7" s="13"/>
       <c r="F7" s="14"/>
@@ -44759,7 +44866,7 @@
       <c r="O7" s="27"/>
     </row>
     <row r="8" spans="2:15" ht="18" customHeight="1">
-      <c r="C8" s="53"/>
+      <c r="C8" s="40"/>
       <c r="D8" s="22"/>
       <c r="E8" s="18"/>
       <c r="F8" s="19"/>
@@ -44774,7 +44881,7 @@
       <c r="O8" s="26"/>
     </row>
     <row r="9" spans="2:15" ht="18" customHeight="1">
-      <c r="C9" s="52"/>
+      <c r="C9" s="39"/>
       <c r="D9" s="17"/>
       <c r="E9" s="13"/>
       <c r="F9" s="14"/>
@@ -44789,7 +44896,7 @@
       <c r="O9" s="27"/>
     </row>
     <row r="10" spans="2:15" ht="18" customHeight="1">
-      <c r="C10" s="53"/>
+      <c r="C10" s="40"/>
       <c r="D10" s="22"/>
       <c r="E10" s="18"/>
       <c r="F10" s="19"/>
@@ -44804,7 +44911,7 @@
       <c r="O10" s="26"/>
     </row>
     <row r="11" spans="2:15" ht="18" customHeight="1">
-      <c r="C11" s="52"/>
+      <c r="C11" s="39"/>
       <c r="D11" s="17"/>
       <c r="E11" s="13"/>
       <c r="F11" s="14"/>
@@ -44819,7 +44926,7 @@
       <c r="O11" s="27"/>
     </row>
     <row r="12" spans="2:15" ht="18" customHeight="1">
-      <c r="C12" s="53"/>
+      <c r="C12" s="40"/>
       <c r="D12" s="22"/>
       <c r="E12" s="18"/>
       <c r="F12" s="19"/>
@@ -44834,7 +44941,7 @@
       <c r="O12" s="26"/>
     </row>
     <row r="13" spans="2:15" ht="18" customHeight="1">
-      <c r="C13" s="52"/>
+      <c r="C13" s="39"/>
       <c r="D13" s="17"/>
       <c r="E13" s="13"/>
       <c r="F13" s="14"/>
@@ -44849,7 +44956,7 @@
       <c r="O13" s="27"/>
     </row>
     <row r="14" spans="2:15" ht="18" customHeight="1">
-      <c r="C14" s="53"/>
+      <c r="C14" s="40"/>
       <c r="D14" s="22"/>
       <c r="E14" s="18"/>
       <c r="F14" s="19"/>
@@ -44864,7 +44971,7 @@
       <c r="O14" s="26"/>
     </row>
     <row r="15" spans="2:15" ht="18" customHeight="1">
-      <c r="C15" s="52"/>
+      <c r="C15" s="39"/>
       <c r="D15" s="17"/>
       <c r="E15" s="13"/>
       <c r="F15" s="14"/>
@@ -44879,7 +44986,7 @@
       <c r="O15" s="27"/>
     </row>
     <row r="16" spans="2:15" ht="18" customHeight="1">
-      <c r="C16" s="53"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="22"/>
       <c r="E16" s="18"/>
       <c r="F16" s="19"/>
@@ -44894,7 +45001,7 @@
       <c r="O16" s="26"/>
     </row>
     <row r="17" spans="3:15" ht="18" customHeight="1">
-      <c r="C17" s="52"/>
+      <c r="C17" s="39"/>
       <c r="D17" s="17"/>
       <c r="E17" s="13"/>
       <c r="F17" s="14"/>
@@ -44909,7 +45016,7 @@
       <c r="O17" s="27"/>
     </row>
     <row r="18" spans="3:15" ht="18" customHeight="1">
-      <c r="C18" s="53"/>
+      <c r="C18" s="40"/>
       <c r="D18" s="22"/>
       <c r="E18" s="18"/>
       <c r="F18" s="19"/>
@@ -44924,7 +45031,7 @@
       <c r="O18" s="26"/>
     </row>
     <row r="19" spans="3:15" ht="18" customHeight="1">
-      <c r="C19" s="52"/>
+      <c r="C19" s="39"/>
       <c r="D19" s="17"/>
       <c r="E19" s="13"/>
       <c r="F19" s="14"/>
@@ -44939,7 +45046,7 @@
       <c r="O19" s="27"/>
     </row>
     <row r="20" spans="3:15" ht="18" customHeight="1">
-      <c r="C20" s="53"/>
+      <c r="C20" s="40"/>
       <c r="D20" s="22"/>
       <c r="E20" s="18"/>
       <c r="F20" s="19"/>
@@ -44954,7 +45061,7 @@
       <c r="O20" s="26"/>
     </row>
     <row r="21" spans="3:15" ht="18" customHeight="1">
-      <c r="C21" s="52"/>
+      <c r="C21" s="39"/>
       <c r="D21" s="17"/>
       <c r="E21" s="13"/>
       <c r="F21" s="14"/>
@@ -44969,7 +45076,7 @@
       <c r="O21" s="27"/>
     </row>
     <row r="22" spans="3:15" ht="18" customHeight="1">
-      <c r="C22" s="53"/>
+      <c r="C22" s="40"/>
       <c r="D22" s="22"/>
       <c r="E22" s="18"/>
       <c r="F22" s="19"/>
@@ -44984,7 +45091,7 @@
       <c r="O22" s="26"/>
     </row>
     <row r="23" spans="3:15" ht="18" customHeight="1">
-      <c r="C23" s="52"/>
+      <c r="C23" s="39"/>
       <c r="D23" s="17"/>
       <c r="E23" s="13"/>
       <c r="F23" s="14"/>
@@ -44999,7 +45106,7 @@
       <c r="O23" s="27"/>
     </row>
     <row r="24" spans="3:15" ht="18" customHeight="1">
-      <c r="C24" s="53"/>
+      <c r="C24" s="40"/>
       <c r="D24" s="22"/>
       <c r="E24" s="18"/>
       <c r="F24" s="19"/>
@@ -45014,7 +45121,7 @@
       <c r="O24" s="26"/>
     </row>
     <row r="25" spans="3:15" ht="18" customHeight="1">
-      <c r="C25" s="52"/>
+      <c r="C25" s="39"/>
       <c r="D25" s="17"/>
       <c r="E25" s="13"/>
       <c r="F25" s="14"/>
@@ -45029,7 +45136,7 @@
       <c r="O25" s="27"/>
     </row>
     <row r="26" spans="3:15" ht="18" customHeight="1">
-      <c r="C26" s="53"/>
+      <c r="C26" s="40"/>
       <c r="D26" s="22"/>
       <c r="E26" s="18"/>
       <c r="F26" s="19"/>
@@ -45044,7 +45151,7 @@
       <c r="O26" s="26"/>
     </row>
     <row r="27" spans="3:15" ht="18" customHeight="1">
-      <c r="C27" s="52"/>
+      <c r="C27" s="39"/>
       <c r="D27" s="17"/>
       <c r="E27" s="13"/>
       <c r="F27" s="14"/>
@@ -45059,7 +45166,7 @@
       <c r="O27" s="27"/>
     </row>
     <row r="28" spans="3:15" ht="18" customHeight="1">
-      <c r="C28" s="53"/>
+      <c r="C28" s="40"/>
       <c r="D28" s="22"/>
       <c r="E28" s="18"/>
       <c r="F28" s="19"/>
@@ -45074,7 +45181,7 @@
       <c r="O28" s="26"/>
     </row>
     <row r="29" spans="3:15" ht="18" customHeight="1">
-      <c r="C29" s="52"/>
+      <c r="C29" s="39"/>
       <c r="D29" s="17"/>
       <c r="E29" s="13"/>
       <c r="F29" s="14"/>
@@ -45089,7 +45196,7 @@
       <c r="O29" s="27"/>
     </row>
     <row r="30" spans="3:15" ht="18" customHeight="1">
-      <c r="C30" s="53"/>
+      <c r="C30" s="40"/>
       <c r="D30" s="22"/>
       <c r="E30" s="18"/>
       <c r="F30" s="19"/>
@@ -45104,7 +45211,7 @@
       <c r="O30" s="26"/>
     </row>
     <row r="31" spans="3:15" ht="18" customHeight="1">
-      <c r="C31" s="52"/>
+      <c r="C31" s="39"/>
       <c r="D31" s="17"/>
       <c r="E31" s="13"/>
       <c r="F31" s="14"/>
@@ -45119,7 +45226,7 @@
       <c r="O31" s="27"/>
     </row>
     <row r="32" spans="3:15" ht="18" customHeight="1">
-      <c r="C32" s="53"/>
+      <c r="C32" s="40"/>
       <c r="D32" s="22"/>
       <c r="E32" s="18"/>
       <c r="F32" s="19"/>
@@ -45134,7 +45241,7 @@
       <c r="O32" s="26"/>
     </row>
     <row r="33" spans="3:15" ht="18" customHeight="1">
-      <c r="C33" s="52"/>
+      <c r="C33" s="39"/>
       <c r="D33" s="17"/>
       <c r="E33" s="13"/>
       <c r="F33" s="14"/>
@@ -45149,7 +45256,7 @@
       <c r="O33" s="27"/>
     </row>
     <row r="34" spans="3:15" ht="18" customHeight="1">
-      <c r="C34" s="53"/>
+      <c r="C34" s="40"/>
       <c r="D34" s="22"/>
       <c r="E34" s="18"/>
       <c r="F34" s="19"/>
@@ -45164,7 +45271,7 @@
       <c r="O34" s="26"/>
     </row>
     <row r="35" spans="3:15" ht="18" customHeight="1">
-      <c r="C35" s="52"/>
+      <c r="C35" s="39"/>
       <c r="D35" s="17"/>
       <c r="E35" s="13"/>
       <c r="F35" s="14"/>
@@ -45179,7 +45286,7 @@
       <c r="O35" s="27"/>
     </row>
     <row r="36" spans="3:15" ht="18" customHeight="1">
-      <c r="C36" s="53"/>
+      <c r="C36" s="40"/>
       <c r="D36" s="22"/>
       <c r="E36" s="18"/>
       <c r="F36" s="19"/>
@@ -45194,7 +45301,7 @@
       <c r="O36" s="26"/>
     </row>
     <row r="37" spans="3:15" ht="18" customHeight="1">
-      <c r="C37" s="52"/>
+      <c r="C37" s="39"/>
       <c r="D37" s="17"/>
       <c r="E37" s="13"/>
       <c r="F37" s="14"/>
@@ -45209,7 +45316,7 @@
       <c r="O37" s="27"/>
     </row>
     <row r="38" spans="3:15" ht="18" customHeight="1">
-      <c r="C38" s="51"/>
+      <c r="C38" s="38"/>
       <c r="D38" s="32"/>
       <c r="E38" s="35"/>
       <c r="F38" s="36"/>
@@ -45224,7 +45331,7 @@
       <c r="O38" s="26"/>
     </row>
     <row r="39" spans="3:15" ht="18" customHeight="1">
-      <c r="C39" s="52"/>
+      <c r="C39" s="39"/>
       <c r="D39" s="17"/>
       <c r="E39" s="13"/>
       <c r="F39" s="14"/>
@@ -45239,7 +45346,7 @@
       <c r="O39" s="27"/>
     </row>
     <row r="40" spans="3:15" ht="18" customHeight="1">
-      <c r="C40" s="53"/>
+      <c r="C40" s="40"/>
       <c r="D40" s="22"/>
       <c r="E40" s="18"/>
       <c r="F40" s="19"/>
@@ -45254,7 +45361,7 @@
       <c r="O40" s="26"/>
     </row>
     <row r="41" spans="3:15" ht="18" customHeight="1">
-      <c r="C41" s="52"/>
+      <c r="C41" s="39"/>
       <c r="D41" s="17"/>
       <c r="E41" s="13"/>
       <c r="F41" s="14"/>
@@ -45269,7 +45376,7 @@
       <c r="O41" s="27"/>
     </row>
     <row r="42" spans="3:15" ht="18" customHeight="1">
-      <c r="C42" s="53"/>
+      <c r="C42" s="40"/>
       <c r="D42" s="22"/>
       <c r="E42" s="18"/>
       <c r="F42" s="19"/>
@@ -45284,7 +45391,7 @@
       <c r="O42" s="26"/>
     </row>
     <row r="43" spans="3:15" ht="18" customHeight="1">
-      <c r="C43" s="52"/>
+      <c r="C43" s="39"/>
       <c r="D43" s="17"/>
       <c r="E43" s="13"/>
       <c r="F43" s="14"/>
@@ -45299,7 +45406,7 @@
       <c r="O43" s="27"/>
     </row>
     <row r="44" spans="3:15" ht="18" customHeight="1">
-      <c r="C44" s="53"/>
+      <c r="C44" s="40"/>
       <c r="D44" s="22"/>
       <c r="E44" s="18"/>
       <c r="F44" s="19"/>
@@ -45314,7 +45421,7 @@
       <c r="O44" s="26"/>
     </row>
     <row r="45" spans="3:15" ht="18" customHeight="1">
-      <c r="C45" s="52"/>
+      <c r="C45" s="39"/>
       <c r="D45" s="17"/>
       <c r="E45" s="13"/>
       <c r="F45" s="14"/>
@@ -45329,7 +45436,7 @@
       <c r="O45" s="27"/>
     </row>
     <row r="46" spans="3:15" ht="18" customHeight="1">
-      <c r="C46" s="53"/>
+      <c r="C46" s="40"/>
       <c r="D46" s="22"/>
       <c r="E46" s="18"/>
       <c r="F46" s="19"/>
@@ -45344,7 +45451,7 @@
       <c r="O46" s="26"/>
     </row>
     <row r="47" spans="3:15" ht="18" customHeight="1">
-      <c r="C47" s="52"/>
+      <c r="C47" s="39"/>
       <c r="D47" s="17"/>
       <c r="E47" s="13"/>
       <c r="F47" s="14"/>
@@ -45359,7 +45466,7 @@
       <c r="O47" s="27"/>
     </row>
     <row r="48" spans="3:15" ht="18" customHeight="1">
-      <c r="C48" s="53"/>
+      <c r="C48" s="40"/>
       <c r="D48" s="22"/>
       <c r="E48" s="18"/>
       <c r="F48" s="19"/>
@@ -45374,7 +45481,7 @@
       <c r="O48" s="26"/>
     </row>
     <row r="49" spans="3:15" ht="18" customHeight="1">
-      <c r="C49" s="52"/>
+      <c r="C49" s="39"/>
       <c r="D49" s="17"/>
       <c r="E49" s="13"/>
       <c r="F49" s="14"/>
@@ -45389,7 +45496,7 @@
       <c r="O49" s="27"/>
     </row>
     <row r="50" spans="3:15" ht="18" customHeight="1">
-      <c r="C50" s="53"/>
+      <c r="C50" s="40"/>
       <c r="D50" s="22"/>
       <c r="E50" s="18"/>
       <c r="F50" s="19"/>
@@ -45404,7 +45511,7 @@
       <c r="O50" s="26"/>
     </row>
     <row r="51" spans="3:15" ht="18" customHeight="1">
-      <c r="C51" s="52"/>
+      <c r="C51" s="39"/>
       <c r="D51" s="17"/>
       <c r="E51" s="13"/>
       <c r="F51" s="14"/>
@@ -45419,7 +45526,7 @@
       <c r="O51" s="27"/>
     </row>
     <row r="52" spans="3:15" ht="18" customHeight="1">
-      <c r="C52" s="53"/>
+      <c r="C52" s="40"/>
       <c r="D52" s="22"/>
       <c r="E52" s="18"/>
       <c r="F52" s="19"/>
@@ -45434,7 +45541,7 @@
       <c r="O52" s="26"/>
     </row>
     <row r="53" spans="3:15" ht="18" customHeight="1">
-      <c r="C53" s="52"/>
+      <c r="C53" s="39"/>
       <c r="D53" s="17"/>
       <c r="E53" s="13"/>
       <c r="F53" s="14"/>
@@ -45449,7 +45556,7 @@
       <c r="O53" s="27"/>
     </row>
     <row r="54" spans="3:15" ht="18" customHeight="1">
-      <c r="C54" s="53"/>
+      <c r="C54" s="40"/>
       <c r="D54" s="22"/>
       <c r="E54" s="18"/>
       <c r="F54" s="19"/>
@@ -45464,7 +45571,7 @@
       <c r="O54" s="26"/>
     </row>
     <row r="55" spans="3:15" ht="18" customHeight="1">
-      <c r="C55" s="52"/>
+      <c r="C55" s="39"/>
       <c r="D55" s="17"/>
       <c r="E55" s="13"/>
       <c r="F55" s="14"/>
@@ -45479,7 +45586,7 @@
       <c r="O55" s="27"/>
     </row>
     <row r="56" spans="3:15" ht="18" customHeight="1">
-      <c r="C56" s="53"/>
+      <c r="C56" s="40"/>
       <c r="D56" s="22"/>
       <c r="E56" s="18"/>
       <c r="F56" s="19"/>
@@ -45494,7 +45601,7 @@
       <c r="O56" s="26"/>
     </row>
     <row r="57" spans="3:15" ht="18" customHeight="1">
-      <c r="C57" s="52"/>
+      <c r="C57" s="39"/>
       <c r="D57" s="17"/>
       <c r="E57" s="13"/>
       <c r="F57" s="14"/>
@@ -45509,7 +45616,7 @@
       <c r="O57" s="27"/>
     </row>
     <row r="58" spans="3:15" ht="18" customHeight="1">
-      <c r="C58" s="53"/>
+      <c r="C58" s="40"/>
       <c r="D58" s="22"/>
       <c r="E58" s="18"/>
       <c r="F58" s="19"/>
@@ -45524,7 +45631,7 @@
       <c r="O58" s="26"/>
     </row>
     <row r="59" spans="3:15" ht="18" customHeight="1">
-      <c r="C59" s="52"/>
+      <c r="C59" s="39"/>
       <c r="D59" s="17"/>
       <c r="E59" s="13"/>
       <c r="F59" s="14"/>
@@ -45539,7 +45646,7 @@
       <c r="O59" s="27"/>
     </row>
     <row r="60" spans="3:15" ht="18" customHeight="1">
-      <c r="C60" s="53"/>
+      <c r="C60" s="40"/>
       <c r="D60" s="22"/>
       <c r="E60" s="18"/>
       <c r="F60" s="19"/>
@@ -45554,7 +45661,7 @@
       <c r="O60" s="26"/>
     </row>
     <row r="61" spans="3:15" ht="18" customHeight="1">
-      <c r="C61" s="52"/>
+      <c r="C61" s="39"/>
       <c r="D61" s="17"/>
       <c r="E61" s="13"/>
       <c r="F61" s="14"/>
@@ -45569,7 +45676,7 @@
       <c r="O61" s="27"/>
     </row>
     <row r="62" spans="3:15" ht="18" customHeight="1">
-      <c r="C62" s="53"/>
+      <c r="C62" s="40"/>
       <c r="D62" s="22"/>
       <c r="E62" s="18"/>
       <c r="F62" s="19"/>
@@ -45584,7 +45691,7 @@
       <c r="O62" s="26"/>
     </row>
     <row r="63" spans="3:15" ht="18" customHeight="1">
-      <c r="C63" s="52"/>
+      <c r="C63" s="39"/>
       <c r="D63" s="17"/>
       <c r="E63" s="13"/>
       <c r="F63" s="14"/>
@@ -45599,7 +45706,7 @@
       <c r="O63" s="27"/>
     </row>
     <row r="64" spans="3:15" ht="18" customHeight="1">
-      <c r="C64" s="53"/>
+      <c r="C64" s="40"/>
       <c r="D64" s="22"/>
       <c r="E64" s="18"/>
       <c r="F64" s="19"/>
@@ -45613,8 +45720,8 @@
       <c r="N64" s="21"/>
       <c r="O64" s="26"/>
     </row>
-    <row r="65" spans="2:15" ht="18" customHeight="1">
-      <c r="C65" s="52"/>
+    <row r="65" spans="3:15" ht="18" customHeight="1">
+      <c r="C65" s="39"/>
       <c r="D65" s="17"/>
       <c r="E65" s="13"/>
       <c r="F65" s="14"/>
@@ -45628,8 +45735,8 @@
       <c r="N65" s="16"/>
       <c r="O65" s="27"/>
     </row>
-    <row r="66" spans="2:15" ht="18" customHeight="1">
-      <c r="C66" s="53"/>
+    <row r="66" spans="3:15" ht="18" customHeight="1">
+      <c r="C66" s="40"/>
       <c r="D66" s="22"/>
       <c r="E66" s="18"/>
       <c r="F66" s="19"/>
@@ -45643,8 +45750,8 @@
       <c r="N66" s="21"/>
       <c r="O66" s="26"/>
     </row>
-    <row r="67" spans="2:15" ht="18" customHeight="1">
-      <c r="C67" s="52"/>
+    <row r="67" spans="3:15" ht="18" customHeight="1">
+      <c r="C67" s="39"/>
       <c r="D67" s="17"/>
       <c r="E67" s="13"/>
       <c r="F67" s="14"/>
@@ -45658,1053 +45765,8 @@
       <c r="N67" s="16"/>
       <c r="O67" s="27"/>
     </row>
-    <row r="69" spans="2:15">
-      <c r="B69" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="70" spans="2:15" ht="4.9000000000000004" customHeight="1">
-      <c r="D70" s="2"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="4"/>
-    </row>
-    <row r="71" spans="2:15" ht="18" customHeight="1">
-      <c r="C71" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="D71" s="40"/>
-      <c r="E71" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="F71" s="42"/>
-      <c r="G71" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="H71" s="44"/>
-      <c r="I71" s="44"/>
-      <c r="J71" s="45"/>
-      <c r="K71" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="L71" s="44"/>
-      <c r="M71" s="44"/>
-      <c r="N71" s="46"/>
-      <c r="O71" s="38" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="72" spans="2:15" ht="18" customHeight="1">
-      <c r="C72" s="34"/>
-      <c r="D72" s="23"/>
-      <c r="E72" s="24"/>
-      <c r="F72" s="25"/>
-      <c r="G72" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="H72" s="48"/>
-      <c r="I72" s="49" t="s">
-        <v>10</v>
-      </c>
-      <c r="J72" s="50"/>
-      <c r="K72" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="L72" s="48"/>
-      <c r="M72" s="49" t="s">
-        <v>10</v>
-      </c>
-      <c r="N72" s="50"/>
-      <c r="O72" s="38"/>
-    </row>
-    <row r="73" spans="2:15" ht="18" customHeight="1" thickBot="1">
-      <c r="C73" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E73" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F73" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G73" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H73" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I73" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J73" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="K73" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L73" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="M73" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N73" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="O73" s="38"/>
-    </row>
-    <row r="74" spans="2:15" ht="18" customHeight="1" thickTop="1">
-      <c r="C74" s="51"/>
-      <c r="D74" s="32"/>
-      <c r="E74" s="11"/>
-      <c r="F74" s="12"/>
-      <c r="G74" s="28"/>
-      <c r="H74" s="29"/>
-      <c r="I74" s="29"/>
-      <c r="J74" s="30"/>
-      <c r="K74" s="31"/>
-      <c r="L74" s="29"/>
-      <c r="M74" s="29"/>
-      <c r="N74" s="29"/>
-      <c r="O74" s="26"/>
-    </row>
-    <row r="75" spans="2:15" ht="18" customHeight="1">
-      <c r="C75" s="52"/>
-      <c r="D75" s="17"/>
-      <c r="E75" s="13"/>
-      <c r="F75" s="14"/>
-      <c r="G75" s="15"/>
-      <c r="H75" s="16"/>
-      <c r="I75" s="16"/>
-      <c r="J75" s="17"/>
-      <c r="K75" s="13"/>
-      <c r="L75" s="16"/>
-      <c r="M75" s="16"/>
-      <c r="N75" s="16"/>
-      <c r="O75" s="27"/>
-    </row>
-    <row r="76" spans="2:15" ht="18" customHeight="1">
-      <c r="C76" s="53"/>
-      <c r="D76" s="22"/>
-      <c r="E76" s="18"/>
-      <c r="F76" s="19"/>
-      <c r="G76" s="20"/>
-      <c r="H76" s="21"/>
-      <c r="I76" s="21"/>
-      <c r="J76" s="22"/>
-      <c r="K76" s="18"/>
-      <c r="L76" s="21"/>
-      <c r="M76" s="21"/>
-      <c r="N76" s="21"/>
-      <c r="O76" s="26"/>
-    </row>
-    <row r="77" spans="2:15" ht="18" customHeight="1">
-      <c r="C77" s="52"/>
-      <c r="D77" s="17"/>
-      <c r="E77" s="13"/>
-      <c r="F77" s="14"/>
-      <c r="G77" s="15"/>
-      <c r="H77" s="16"/>
-      <c r="I77" s="16"/>
-      <c r="J77" s="17"/>
-      <c r="K77" s="13"/>
-      <c r="L77" s="16"/>
-      <c r="M77" s="16"/>
-      <c r="N77" s="16"/>
-      <c r="O77" s="27"/>
-    </row>
-    <row r="78" spans="2:15" ht="18" customHeight="1">
-      <c r="C78" s="53"/>
-      <c r="D78" s="22"/>
-      <c r="E78" s="18"/>
-      <c r="F78" s="19"/>
-      <c r="G78" s="20"/>
-      <c r="H78" s="21"/>
-      <c r="I78" s="21"/>
-      <c r="J78" s="22"/>
-      <c r="K78" s="18"/>
-      <c r="L78" s="21"/>
-      <c r="M78" s="21"/>
-      <c r="N78" s="21"/>
-      <c r="O78" s="26"/>
-    </row>
-    <row r="79" spans="2:15" ht="18" customHeight="1">
-      <c r="C79" s="52"/>
-      <c r="D79" s="17"/>
-      <c r="E79" s="13"/>
-      <c r="F79" s="14"/>
-      <c r="G79" s="15"/>
-      <c r="H79" s="16"/>
-      <c r="I79" s="16"/>
-      <c r="J79" s="17"/>
-      <c r="K79" s="13"/>
-      <c r="L79" s="16"/>
-      <c r="M79" s="16"/>
-      <c r="N79" s="16"/>
-      <c r="O79" s="27"/>
-    </row>
-    <row r="80" spans="2:15" ht="18" customHeight="1">
-      <c r="C80" s="53"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="18"/>
-      <c r="F80" s="19"/>
-      <c r="G80" s="20"/>
-      <c r="H80" s="21"/>
-      <c r="I80" s="21"/>
-      <c r="J80" s="22"/>
-      <c r="K80" s="18"/>
-      <c r="L80" s="21"/>
-      <c r="M80" s="21"/>
-      <c r="N80" s="21"/>
-      <c r="O80" s="26"/>
-    </row>
-    <row r="81" spans="3:15" ht="18" customHeight="1">
-      <c r="C81" s="52"/>
-      <c r="D81" s="17"/>
-      <c r="E81" s="13"/>
-      <c r="F81" s="14"/>
-      <c r="G81" s="15"/>
-      <c r="H81" s="16"/>
-      <c r="I81" s="16"/>
-      <c r="J81" s="17"/>
-      <c r="K81" s="13"/>
-      <c r="L81" s="16"/>
-      <c r="M81" s="16"/>
-      <c r="N81" s="16"/>
-      <c r="O81" s="27"/>
-    </row>
-    <row r="82" spans="3:15" ht="18" customHeight="1">
-      <c r="C82" s="53"/>
-      <c r="D82" s="22"/>
-      <c r="E82" s="18"/>
-      <c r="F82" s="19"/>
-      <c r="G82" s="20"/>
-      <c r="H82" s="21"/>
-      <c r="I82" s="21"/>
-      <c r="J82" s="22"/>
-      <c r="K82" s="18"/>
-      <c r="L82" s="21"/>
-      <c r="M82" s="21"/>
-      <c r="N82" s="21"/>
-      <c r="O82" s="26"/>
-    </row>
-    <row r="83" spans="3:15" ht="18" customHeight="1">
-      <c r="C83" s="52"/>
-      <c r="D83" s="17"/>
-      <c r="E83" s="13"/>
-      <c r="F83" s="14"/>
-      <c r="G83" s="15"/>
-      <c r="H83" s="16"/>
-      <c r="I83" s="16"/>
-      <c r="J83" s="17"/>
-      <c r="K83" s="13"/>
-      <c r="L83" s="16"/>
-      <c r="M83" s="16"/>
-      <c r="N83" s="16"/>
-      <c r="O83" s="27"/>
-    </row>
-    <row r="84" spans="3:15" ht="18" customHeight="1">
-      <c r="C84" s="53"/>
-      <c r="D84" s="22"/>
-      <c r="E84" s="18"/>
-      <c r="F84" s="19"/>
-      <c r="G84" s="20"/>
-      <c r="H84" s="21"/>
-      <c r="I84" s="21"/>
-      <c r="J84" s="22"/>
-      <c r="K84" s="18"/>
-      <c r="L84" s="21"/>
-      <c r="M84" s="21"/>
-      <c r="N84" s="21"/>
-      <c r="O84" s="26"/>
-    </row>
-    <row r="85" spans="3:15" ht="18" customHeight="1">
-      <c r="C85" s="52"/>
-      <c r="D85" s="17"/>
-      <c r="E85" s="13"/>
-      <c r="F85" s="14"/>
-      <c r="G85" s="15"/>
-      <c r="H85" s="16"/>
-      <c r="I85" s="16"/>
-      <c r="J85" s="17"/>
-      <c r="K85" s="13"/>
-      <c r="L85" s="16"/>
-      <c r="M85" s="16"/>
-      <c r="N85" s="16"/>
-      <c r="O85" s="27"/>
-    </row>
-    <row r="86" spans="3:15" ht="18" customHeight="1">
-      <c r="C86" s="53"/>
-      <c r="D86" s="22"/>
-      <c r="E86" s="18"/>
-      <c r="F86" s="19"/>
-      <c r="G86" s="20"/>
-      <c r="H86" s="21"/>
-      <c r="I86" s="21"/>
-      <c r="J86" s="22"/>
-      <c r="K86" s="18"/>
-      <c r="L86" s="21"/>
-      <c r="M86" s="21"/>
-      <c r="N86" s="21"/>
-      <c r="O86" s="26"/>
-    </row>
-    <row r="87" spans="3:15" ht="18" customHeight="1">
-      <c r="C87" s="52"/>
-      <c r="D87" s="17"/>
-      <c r="E87" s="13"/>
-      <c r="F87" s="14"/>
-      <c r="G87" s="15"/>
-      <c r="H87" s="16"/>
-      <c r="I87" s="16"/>
-      <c r="J87" s="17"/>
-      <c r="K87" s="13"/>
-      <c r="L87" s="16"/>
-      <c r="M87" s="16"/>
-      <c r="N87" s="16"/>
-      <c r="O87" s="27"/>
-    </row>
-    <row r="88" spans="3:15" ht="18" customHeight="1">
-      <c r="C88" s="53"/>
-      <c r="D88" s="22"/>
-      <c r="E88" s="18"/>
-      <c r="F88" s="19"/>
-      <c r="G88" s="20"/>
-      <c r="H88" s="21"/>
-      <c r="I88" s="21"/>
-      <c r="J88" s="22"/>
-      <c r="K88" s="18"/>
-      <c r="L88" s="21"/>
-      <c r="M88" s="21"/>
-      <c r="N88" s="21"/>
-      <c r="O88" s="26"/>
-    </row>
-    <row r="89" spans="3:15" ht="18" customHeight="1">
-      <c r="C89" s="52"/>
-      <c r="D89" s="17"/>
-      <c r="E89" s="13"/>
-      <c r="F89" s="14"/>
-      <c r="G89" s="15"/>
-      <c r="H89" s="16"/>
-      <c r="I89" s="16"/>
-      <c r="J89" s="17"/>
-      <c r="K89" s="13"/>
-      <c r="L89" s="16"/>
-      <c r="M89" s="16"/>
-      <c r="N89" s="16"/>
-      <c r="O89" s="27"/>
-    </row>
-    <row r="90" spans="3:15" ht="18" customHeight="1">
-      <c r="C90" s="53"/>
-      <c r="D90" s="22"/>
-      <c r="E90" s="18"/>
-      <c r="F90" s="19"/>
-      <c r="G90" s="20"/>
-      <c r="H90" s="21"/>
-      <c r="I90" s="21"/>
-      <c r="J90" s="22"/>
-      <c r="K90" s="18"/>
-      <c r="L90" s="21"/>
-      <c r="M90" s="21"/>
-      <c r="N90" s="21"/>
-      <c r="O90" s="26"/>
-    </row>
-    <row r="91" spans="3:15" ht="18" customHeight="1">
-      <c r="C91" s="52"/>
-      <c r="D91" s="17"/>
-      <c r="E91" s="13"/>
-      <c r="F91" s="14"/>
-      <c r="G91" s="15"/>
-      <c r="H91" s="16"/>
-      <c r="I91" s="16"/>
-      <c r="J91" s="17"/>
-      <c r="K91" s="13"/>
-      <c r="L91" s="16"/>
-      <c r="M91" s="16"/>
-      <c r="N91" s="16"/>
-      <c r="O91" s="27"/>
-    </row>
-    <row r="92" spans="3:15" ht="18" customHeight="1">
-      <c r="C92" s="53"/>
-      <c r="D92" s="22"/>
-      <c r="E92" s="18"/>
-      <c r="F92" s="19"/>
-      <c r="G92" s="20"/>
-      <c r="H92" s="21"/>
-      <c r="I92" s="21"/>
-      <c r="J92" s="22"/>
-      <c r="K92" s="18"/>
-      <c r="L92" s="21"/>
-      <c r="M92" s="21"/>
-      <c r="N92" s="21"/>
-      <c r="O92" s="26"/>
-    </row>
-    <row r="93" spans="3:15" ht="18" customHeight="1">
-      <c r="C93" s="52"/>
-      <c r="D93" s="17"/>
-      <c r="E93" s="13"/>
-      <c r="F93" s="14"/>
-      <c r="G93" s="15"/>
-      <c r="H93" s="16"/>
-      <c r="I93" s="16"/>
-      <c r="J93" s="17"/>
-      <c r="K93" s="13"/>
-      <c r="L93" s="16"/>
-      <c r="M93" s="16"/>
-      <c r="N93" s="16"/>
-      <c r="O93" s="27"/>
-    </row>
-    <row r="94" spans="3:15" ht="18" customHeight="1">
-      <c r="C94" s="53"/>
-      <c r="D94" s="22"/>
-      <c r="E94" s="18"/>
-      <c r="F94" s="19"/>
-      <c r="G94" s="20"/>
-      <c r="H94" s="21"/>
-      <c r="I94" s="21"/>
-      <c r="J94" s="22"/>
-      <c r="K94" s="18"/>
-      <c r="L94" s="21"/>
-      <c r="M94" s="21"/>
-      <c r="N94" s="21"/>
-      <c r="O94" s="26"/>
-    </row>
-    <row r="95" spans="3:15" ht="18" customHeight="1">
-      <c r="C95" s="52"/>
-      <c r="D95" s="17"/>
-      <c r="E95" s="13"/>
-      <c r="F95" s="14"/>
-      <c r="G95" s="15"/>
-      <c r="H95" s="16"/>
-      <c r="I95" s="16"/>
-      <c r="J95" s="17"/>
-      <c r="K95" s="13"/>
-      <c r="L95" s="16"/>
-      <c r="M95" s="16"/>
-      <c r="N95" s="16"/>
-      <c r="O95" s="27"/>
-    </row>
-    <row r="96" spans="3:15" ht="18" customHeight="1">
-      <c r="C96" s="53"/>
-      <c r="D96" s="22"/>
-      <c r="E96" s="18"/>
-      <c r="F96" s="19"/>
-      <c r="G96" s="20"/>
-      <c r="H96" s="21"/>
-      <c r="I96" s="21"/>
-      <c r="J96" s="22"/>
-      <c r="K96" s="18"/>
-      <c r="L96" s="21"/>
-      <c r="M96" s="21"/>
-      <c r="N96" s="21"/>
-      <c r="O96" s="26"/>
-    </row>
-    <row r="97" spans="3:15" ht="18" customHeight="1">
-      <c r="C97" s="52"/>
-      <c r="D97" s="17"/>
-      <c r="E97" s="13"/>
-      <c r="F97" s="14"/>
-      <c r="G97" s="15"/>
-      <c r="H97" s="16"/>
-      <c r="I97" s="16"/>
-      <c r="J97" s="17"/>
-      <c r="K97" s="13"/>
-      <c r="L97" s="16"/>
-      <c r="M97" s="16"/>
-      <c r="N97" s="16"/>
-      <c r="O97" s="27"/>
-    </row>
-    <row r="98" spans="3:15" ht="18" customHeight="1">
-      <c r="C98" s="53"/>
-      <c r="D98" s="22"/>
-      <c r="E98" s="18"/>
-      <c r="F98" s="19"/>
-      <c r="G98" s="20"/>
-      <c r="H98" s="21"/>
-      <c r="I98" s="21"/>
-      <c r="J98" s="22"/>
-      <c r="K98" s="18"/>
-      <c r="L98" s="21"/>
-      <c r="M98" s="21"/>
-      <c r="N98" s="21"/>
-      <c r="O98" s="26"/>
-    </row>
-    <row r="99" spans="3:15" ht="18" customHeight="1">
-      <c r="C99" s="52"/>
-      <c r="D99" s="17"/>
-      <c r="E99" s="13"/>
-      <c r="F99" s="14"/>
-      <c r="G99" s="15"/>
-      <c r="H99" s="16"/>
-      <c r="I99" s="16"/>
-      <c r="J99" s="17"/>
-      <c r="K99" s="13"/>
-      <c r="L99" s="16"/>
-      <c r="M99" s="16"/>
-      <c r="N99" s="16"/>
-      <c r="O99" s="27"/>
-    </row>
-    <row r="100" spans="3:15" ht="18" customHeight="1">
-      <c r="C100" s="53"/>
-      <c r="D100" s="22"/>
-      <c r="E100" s="18"/>
-      <c r="F100" s="19"/>
-      <c r="G100" s="20"/>
-      <c r="H100" s="21"/>
-      <c r="I100" s="21"/>
-      <c r="J100" s="22"/>
-      <c r="K100" s="18"/>
-      <c r="L100" s="21"/>
-      <c r="M100" s="21"/>
-      <c r="N100" s="21"/>
-      <c r="O100" s="26"/>
-    </row>
-    <row r="101" spans="3:15" ht="18" customHeight="1">
-      <c r="C101" s="52"/>
-      <c r="D101" s="17"/>
-      <c r="E101" s="13"/>
-      <c r="F101" s="14"/>
-      <c r="G101" s="15"/>
-      <c r="H101" s="16"/>
-      <c r="I101" s="16"/>
-      <c r="J101" s="17"/>
-      <c r="K101" s="13"/>
-      <c r="L101" s="16"/>
-      <c r="M101" s="16"/>
-      <c r="N101" s="16"/>
-      <c r="O101" s="27"/>
-    </row>
-    <row r="102" spans="3:15" ht="18" customHeight="1">
-      <c r="C102" s="53"/>
-      <c r="D102" s="22"/>
-      <c r="E102" s="18"/>
-      <c r="F102" s="19"/>
-      <c r="G102" s="20"/>
-      <c r="H102" s="21"/>
-      <c r="I102" s="21"/>
-      <c r="J102" s="22"/>
-      <c r="K102" s="18"/>
-      <c r="L102" s="21"/>
-      <c r="M102" s="21"/>
-      <c r="N102" s="21"/>
-      <c r="O102" s="26"/>
-    </row>
-    <row r="103" spans="3:15" ht="18" customHeight="1">
-      <c r="C103" s="52"/>
-      <c r="D103" s="17"/>
-      <c r="E103" s="13"/>
-      <c r="F103" s="14"/>
-      <c r="G103" s="15"/>
-      <c r="H103" s="16"/>
-      <c r="I103" s="16"/>
-      <c r="J103" s="17"/>
-      <c r="K103" s="13"/>
-      <c r="L103" s="16"/>
-      <c r="M103" s="16"/>
-      <c r="N103" s="16"/>
-      <c r="O103" s="27"/>
-    </row>
-    <row r="104" spans="3:15" ht="18" customHeight="1">
-      <c r="C104" s="53"/>
-      <c r="D104" s="22"/>
-      <c r="E104" s="18"/>
-      <c r="F104" s="19"/>
-      <c r="G104" s="20"/>
-      <c r="H104" s="21"/>
-      <c r="I104" s="21"/>
-      <c r="J104" s="22"/>
-      <c r="K104" s="18"/>
-      <c r="L104" s="21"/>
-      <c r="M104" s="21"/>
-      <c r="N104" s="21"/>
-      <c r="O104" s="26"/>
-    </row>
-    <row r="105" spans="3:15" ht="18" customHeight="1">
-      <c r="C105" s="52"/>
-      <c r="D105" s="17"/>
-      <c r="E105" s="13"/>
-      <c r="F105" s="14"/>
-      <c r="G105" s="15"/>
-      <c r="H105" s="16"/>
-      <c r="I105" s="16"/>
-      <c r="J105" s="17"/>
-      <c r="K105" s="13"/>
-      <c r="L105" s="16"/>
-      <c r="M105" s="16"/>
-      <c r="N105" s="16"/>
-      <c r="O105" s="27"/>
-    </row>
-    <row r="106" spans="3:15" ht="18" customHeight="1">
-      <c r="C106" s="51"/>
-      <c r="D106" s="32"/>
-      <c r="E106" s="35"/>
-      <c r="F106" s="36"/>
-      <c r="G106" s="28"/>
-      <c r="H106" s="29"/>
-      <c r="I106" s="29"/>
-      <c r="J106" s="30"/>
-      <c r="K106" s="37"/>
-      <c r="L106" s="29"/>
-      <c r="M106" s="29"/>
-      <c r="N106" s="29"/>
-      <c r="O106" s="26"/>
-    </row>
-    <row r="107" spans="3:15" ht="18" customHeight="1">
-      <c r="C107" s="52"/>
-      <c r="D107" s="17"/>
-      <c r="E107" s="13"/>
-      <c r="F107" s="14"/>
-      <c r="G107" s="15"/>
-      <c r="H107" s="16"/>
-      <c r="I107" s="16"/>
-      <c r="J107" s="17"/>
-      <c r="K107" s="13"/>
-      <c r="L107" s="16"/>
-      <c r="M107" s="16"/>
-      <c r="N107" s="16"/>
-      <c r="O107" s="27"/>
-    </row>
-    <row r="108" spans="3:15" ht="18" customHeight="1">
-      <c r="C108" s="53"/>
-      <c r="D108" s="22"/>
-      <c r="E108" s="18"/>
-      <c r="F108" s="19"/>
-      <c r="G108" s="20"/>
-      <c r="H108" s="21"/>
-      <c r="I108" s="21"/>
-      <c r="J108" s="22"/>
-      <c r="K108" s="18"/>
-      <c r="L108" s="21"/>
-      <c r="M108" s="21"/>
-      <c r="N108" s="21"/>
-      <c r="O108" s="26"/>
-    </row>
-    <row r="109" spans="3:15" ht="18" customHeight="1">
-      <c r="C109" s="52"/>
-      <c r="D109" s="17"/>
-      <c r="E109" s="13"/>
-      <c r="F109" s="14"/>
-      <c r="G109" s="15"/>
-      <c r="H109" s="16"/>
-      <c r="I109" s="16"/>
-      <c r="J109" s="17"/>
-      <c r="K109" s="13"/>
-      <c r="L109" s="16"/>
-      <c r="M109" s="16"/>
-      <c r="N109" s="16"/>
-      <c r="O109" s="27"/>
-    </row>
-    <row r="110" spans="3:15" ht="18" customHeight="1">
-      <c r="C110" s="53"/>
-      <c r="D110" s="22"/>
-      <c r="E110" s="18"/>
-      <c r="F110" s="19"/>
-      <c r="G110" s="20"/>
-      <c r="H110" s="21"/>
-      <c r="I110" s="21"/>
-      <c r="J110" s="22"/>
-      <c r="K110" s="18"/>
-      <c r="L110" s="21"/>
-      <c r="M110" s="21"/>
-      <c r="N110" s="21"/>
-      <c r="O110" s="26"/>
-    </row>
-    <row r="111" spans="3:15" ht="18" customHeight="1">
-      <c r="C111" s="52"/>
-      <c r="D111" s="17"/>
-      <c r="E111" s="13"/>
-      <c r="F111" s="14"/>
-      <c r="G111" s="15"/>
-      <c r="H111" s="16"/>
-      <c r="I111" s="16"/>
-      <c r="J111" s="17"/>
-      <c r="K111" s="13"/>
-      <c r="L111" s="16"/>
-      <c r="M111" s="16"/>
-      <c r="N111" s="16"/>
-      <c r="O111" s="27"/>
-    </row>
-    <row r="112" spans="3:15" ht="18" customHeight="1">
-      <c r="C112" s="53"/>
-      <c r="D112" s="22"/>
-      <c r="E112" s="18"/>
-      <c r="F112" s="19"/>
-      <c r="G112" s="20"/>
-      <c r="H112" s="21"/>
-      <c r="I112" s="21"/>
-      <c r="J112" s="22"/>
-      <c r="K112" s="18"/>
-      <c r="L112" s="21"/>
-      <c r="M112" s="21"/>
-      <c r="N112" s="21"/>
-      <c r="O112" s="26"/>
-    </row>
-    <row r="113" spans="3:15" ht="18" customHeight="1">
-      <c r="C113" s="52"/>
-      <c r="D113" s="17"/>
-      <c r="E113" s="13"/>
-      <c r="F113" s="14"/>
-      <c r="G113" s="15"/>
-      <c r="H113" s="16"/>
-      <c r="I113" s="16"/>
-      <c r="J113" s="17"/>
-      <c r="K113" s="13"/>
-      <c r="L113" s="16"/>
-      <c r="M113" s="16"/>
-      <c r="N113" s="16"/>
-      <c r="O113" s="27"/>
-    </row>
-    <row r="114" spans="3:15" ht="18" customHeight="1">
-      <c r="C114" s="53"/>
-      <c r="D114" s="22"/>
-      <c r="E114" s="18"/>
-      <c r="F114" s="19"/>
-      <c r="G114" s="20"/>
-      <c r="H114" s="21"/>
-      <c r="I114" s="21"/>
-      <c r="J114" s="22"/>
-      <c r="K114" s="18"/>
-      <c r="L114" s="21"/>
-      <c r="M114" s="21"/>
-      <c r="N114" s="21"/>
-      <c r="O114" s="26"/>
-    </row>
-    <row r="115" spans="3:15" ht="18" customHeight="1">
-      <c r="C115" s="52"/>
-      <c r="D115" s="17"/>
-      <c r="E115" s="13"/>
-      <c r="F115" s="14"/>
-      <c r="G115" s="15"/>
-      <c r="H115" s="16"/>
-      <c r="I115" s="16"/>
-      <c r="J115" s="17"/>
-      <c r="K115" s="13"/>
-      <c r="L115" s="16"/>
-      <c r="M115" s="16"/>
-      <c r="N115" s="16"/>
-      <c r="O115" s="27"/>
-    </row>
-    <row r="116" spans="3:15" ht="18" customHeight="1">
-      <c r="C116" s="53"/>
-      <c r="D116" s="22"/>
-      <c r="E116" s="18"/>
-      <c r="F116" s="19"/>
-      <c r="G116" s="20"/>
-      <c r="H116" s="21"/>
-      <c r="I116" s="21"/>
-      <c r="J116" s="22"/>
-      <c r="K116" s="18"/>
-      <c r="L116" s="21"/>
-      <c r="M116" s="21"/>
-      <c r="N116" s="21"/>
-      <c r="O116" s="26"/>
-    </row>
-    <row r="117" spans="3:15" ht="18" customHeight="1">
-      <c r="C117" s="52"/>
-      <c r="D117" s="17"/>
-      <c r="E117" s="13"/>
-      <c r="F117" s="14"/>
-      <c r="G117" s="15"/>
-      <c r="H117" s="16"/>
-      <c r="I117" s="16"/>
-      <c r="J117" s="17"/>
-      <c r="K117" s="13"/>
-      <c r="L117" s="16"/>
-      <c r="M117" s="16"/>
-      <c r="N117" s="16"/>
-      <c r="O117" s="27"/>
-    </row>
-    <row r="118" spans="3:15" ht="18" customHeight="1">
-      <c r="C118" s="53"/>
-      <c r="D118" s="22"/>
-      <c r="E118" s="18"/>
-      <c r="F118" s="19"/>
-      <c r="G118" s="20"/>
-      <c r="H118" s="21"/>
-      <c r="I118" s="21"/>
-      <c r="J118" s="22"/>
-      <c r="K118" s="18"/>
-      <c r="L118" s="21"/>
-      <c r="M118" s="21"/>
-      <c r="N118" s="21"/>
-      <c r="O118" s="26"/>
-    </row>
-    <row r="119" spans="3:15" ht="18" customHeight="1">
-      <c r="C119" s="52"/>
-      <c r="D119" s="17"/>
-      <c r="E119" s="13"/>
-      <c r="F119" s="14"/>
-      <c r="G119" s="15"/>
-      <c r="H119" s="16"/>
-      <c r="I119" s="16"/>
-      <c r="J119" s="17"/>
-      <c r="K119" s="13"/>
-      <c r="L119" s="16"/>
-      <c r="M119" s="16"/>
-      <c r="N119" s="16"/>
-      <c r="O119" s="27"/>
-    </row>
-    <row r="120" spans="3:15" ht="18" customHeight="1">
-      <c r="C120" s="53"/>
-      <c r="D120" s="22"/>
-      <c r="E120" s="18"/>
-      <c r="F120" s="19"/>
-      <c r="G120" s="20"/>
-      <c r="H120" s="21"/>
-      <c r="I120" s="21"/>
-      <c r="J120" s="22"/>
-      <c r="K120" s="18"/>
-      <c r="L120" s="21"/>
-      <c r="M120" s="21"/>
-      <c r="N120" s="21"/>
-      <c r="O120" s="26"/>
-    </row>
-    <row r="121" spans="3:15" ht="18" customHeight="1">
-      <c r="C121" s="52"/>
-      <c r="D121" s="17"/>
-      <c r="E121" s="13"/>
-      <c r="F121" s="14"/>
-      <c r="G121" s="15"/>
-      <c r="H121" s="16"/>
-      <c r="I121" s="16"/>
-      <c r="J121" s="17"/>
-      <c r="K121" s="13"/>
-      <c r="L121" s="16"/>
-      <c r="M121" s="16"/>
-      <c r="N121" s="16"/>
-      <c r="O121" s="27"/>
-    </row>
-    <row r="122" spans="3:15" ht="18" customHeight="1">
-      <c r="C122" s="53"/>
-      <c r="D122" s="22"/>
-      <c r="E122" s="18"/>
-      <c r="F122" s="19"/>
-      <c r="G122" s="20"/>
-      <c r="H122" s="21"/>
-      <c r="I122" s="21"/>
-      <c r="J122" s="22"/>
-      <c r="K122" s="18"/>
-      <c r="L122" s="21"/>
-      <c r="M122" s="21"/>
-      <c r="N122" s="21"/>
-      <c r="O122" s="26"/>
-    </row>
-    <row r="123" spans="3:15" ht="18" customHeight="1">
-      <c r="C123" s="52"/>
-      <c r="D123" s="17"/>
-      <c r="E123" s="13"/>
-      <c r="F123" s="14"/>
-      <c r="G123" s="15"/>
-      <c r="H123" s="16"/>
-      <c r="I123" s="16"/>
-      <c r="J123" s="17"/>
-      <c r="K123" s="13"/>
-      <c r="L123" s="16"/>
-      <c r="M123" s="16"/>
-      <c r="N123" s="16"/>
-      <c r="O123" s="27"/>
-    </row>
-    <row r="124" spans="3:15" ht="18" customHeight="1">
-      <c r="C124" s="53"/>
-      <c r="D124" s="22"/>
-      <c r="E124" s="18"/>
-      <c r="F124" s="19"/>
-      <c r="G124" s="20"/>
-      <c r="H124" s="21"/>
-      <c r="I124" s="21"/>
-      <c r="J124" s="22"/>
-      <c r="K124" s="18"/>
-      <c r="L124" s="21"/>
-      <c r="M124" s="21"/>
-      <c r="N124" s="21"/>
-      <c r="O124" s="26"/>
-    </row>
-    <row r="125" spans="3:15" ht="18" customHeight="1">
-      <c r="C125" s="52"/>
-      <c r="D125" s="17"/>
-      <c r="E125" s="13"/>
-      <c r="F125" s="14"/>
-      <c r="G125" s="15"/>
-      <c r="H125" s="16"/>
-      <c r="I125" s="16"/>
-      <c r="J125" s="17"/>
-      <c r="K125" s="13"/>
-      <c r="L125" s="16"/>
-      <c r="M125" s="16"/>
-      <c r="N125" s="16"/>
-      <c r="O125" s="27"/>
-    </row>
-    <row r="126" spans="3:15" ht="18" customHeight="1">
-      <c r="C126" s="53"/>
-      <c r="D126" s="22"/>
-      <c r="E126" s="18"/>
-      <c r="F126" s="19"/>
-      <c r="G126" s="20"/>
-      <c r="H126" s="21"/>
-      <c r="I126" s="21"/>
-      <c r="J126" s="22"/>
-      <c r="K126" s="18"/>
-      <c r="L126" s="21"/>
-      <c r="M126" s="21"/>
-      <c r="N126" s="21"/>
-      <c r="O126" s="26"/>
-    </row>
-    <row r="127" spans="3:15" ht="18" customHeight="1">
-      <c r="C127" s="52"/>
-      <c r="D127" s="17"/>
-      <c r="E127" s="13"/>
-      <c r="F127" s="14"/>
-      <c r="G127" s="15"/>
-      <c r="H127" s="16"/>
-      <c r="I127" s="16"/>
-      <c r="J127" s="17"/>
-      <c r="K127" s="13"/>
-      <c r="L127" s="16"/>
-      <c r="M127" s="16"/>
-      <c r="N127" s="16"/>
-      <c r="O127" s="27"/>
-    </row>
-    <row r="128" spans="3:15" ht="18" customHeight="1">
-      <c r="C128" s="53"/>
-      <c r="D128" s="22"/>
-      <c r="E128" s="18"/>
-      <c r="F128" s="19"/>
-      <c r="G128" s="20"/>
-      <c r="H128" s="21"/>
-      <c r="I128" s="21"/>
-      <c r="J128" s="22"/>
-      <c r="K128" s="18"/>
-      <c r="L128" s="21"/>
-      <c r="M128" s="21"/>
-      <c r="N128" s="21"/>
-      <c r="O128" s="26"/>
-    </row>
-    <row r="129" spans="3:15" ht="18" customHeight="1">
-      <c r="C129" s="52"/>
-      <c r="D129" s="17"/>
-      <c r="E129" s="13"/>
-      <c r="F129" s="14"/>
-      <c r="G129" s="15"/>
-      <c r="H129" s="16"/>
-      <c r="I129" s="16"/>
-      <c r="J129" s="17"/>
-      <c r="K129" s="13"/>
-      <c r="L129" s="16"/>
-      <c r="M129" s="16"/>
-      <c r="N129" s="16"/>
-      <c r="O129" s="27"/>
-    </row>
-    <row r="130" spans="3:15" ht="18" customHeight="1">
-      <c r="C130" s="53"/>
-      <c r="D130" s="22"/>
-      <c r="E130" s="18"/>
-      <c r="F130" s="19"/>
-      <c r="G130" s="20"/>
-      <c r="H130" s="21"/>
-      <c r="I130" s="21"/>
-      <c r="J130" s="22"/>
-      <c r="K130" s="18"/>
-      <c r="L130" s="21"/>
-      <c r="M130" s="21"/>
-      <c r="N130" s="21"/>
-      <c r="O130" s="26"/>
-    </row>
-    <row r="131" spans="3:15" ht="18" customHeight="1">
-      <c r="C131" s="52"/>
-      <c r="D131" s="17"/>
-      <c r="E131" s="13"/>
-      <c r="F131" s="14"/>
-      <c r="G131" s="15"/>
-      <c r="H131" s="16"/>
-      <c r="I131" s="16"/>
-      <c r="J131" s="17"/>
-      <c r="K131" s="13"/>
-      <c r="L131" s="16"/>
-      <c r="M131" s="16"/>
-      <c r="N131" s="16"/>
-      <c r="O131" s="27"/>
-    </row>
-    <row r="132" spans="3:15" ht="18" customHeight="1">
-      <c r="C132" s="53"/>
-      <c r="D132" s="22"/>
-      <c r="E132" s="18"/>
-      <c r="F132" s="19"/>
-      <c r="G132" s="20"/>
-      <c r="H132" s="21"/>
-      <c r="I132" s="21"/>
-      <c r="J132" s="22"/>
-      <c r="K132" s="18"/>
-      <c r="L132" s="21"/>
-      <c r="M132" s="21"/>
-      <c r="N132" s="21"/>
-      <c r="O132" s="26"/>
-    </row>
-    <row r="133" spans="3:15" ht="18" customHeight="1">
-      <c r="C133" s="52"/>
-      <c r="D133" s="17"/>
-      <c r="E133" s="13"/>
-      <c r="F133" s="14"/>
-      <c r="G133" s="15"/>
-      <c r="H133" s="16"/>
-      <c r="I133" s="16"/>
-      <c r="J133" s="17"/>
-      <c r="K133" s="13"/>
-      <c r="L133" s="16"/>
-      <c r="M133" s="16"/>
-      <c r="N133" s="16"/>
-      <c r="O133" s="27"/>
-    </row>
-    <row r="134" spans="3:15" ht="18" customHeight="1">
-      <c r="C134" s="53"/>
-      <c r="D134" s="22"/>
-      <c r="E134" s="18"/>
-      <c r="F134" s="19"/>
-      <c r="G134" s="20"/>
-      <c r="H134" s="21"/>
-      <c r="I134" s="21"/>
-      <c r="J134" s="22"/>
-      <c r="K134" s="18"/>
-      <c r="L134" s="21"/>
-      <c r="M134" s="21"/>
-      <c r="N134" s="21"/>
-      <c r="O134" s="26"/>
-    </row>
-    <row r="135" spans="3:15" ht="18" customHeight="1">
-      <c r="C135" s="52"/>
-      <c r="D135" s="17"/>
-      <c r="E135" s="13"/>
-      <c r="F135" s="14"/>
-      <c r="G135" s="15"/>
-      <c r="H135" s="16"/>
-      <c r="I135" s="16"/>
-      <c r="J135" s="17"/>
-      <c r="K135" s="13"/>
-      <c r="L135" s="16"/>
-      <c r="M135" s="16"/>
-      <c r="N135" s="16"/>
-      <c r="O135" s="27"/>
-    </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="G71:J71"/>
-    <mergeCell ref="K71:N71"/>
-    <mergeCell ref="O71:O73"/>
-    <mergeCell ref="G72:H72"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="K72:L72"/>
-    <mergeCell ref="M72:N72"/>
+  <mergeCells count="9">
     <mergeCell ref="O3:O5"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
@@ -46716,15 +45778,1090 @@
     <mergeCell ref="M4:N4"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
-  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="32" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.98425196850393704" bottom="0.39370078740157499" header="0.31496062992126" footer="0.31496062992126"/>
+  <pageSetup paperSize="9" scale="64" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;10日通システム株式会社 &amp;C&amp;"ＭＳ ゴシック,Regular"&amp;16標準報酬月額表（厚生年金）&amp;R&amp;"ＭＳ ゴシック,Regular"&amp;10&amp;KFF0000 &amp;K01+000&amp;D　&amp;T　
 &amp;KFF0000 &amp;K01+000page&amp;P</oddHeader>
   </headerFooter>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="68" max="16383" man="1"/>
-  </rowBreaks>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:O67"/>
+  <sheetViews>
+    <sheetView view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="85" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12"/>
+  <cols>
+    <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="2.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="33" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="1" customWidth="1"/>
+    <col min="5" max="15" width="10.7109375" style="1"/>
+    <col min="16" max="16" width="1.28515625" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="10.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="4.9000000000000004" customHeight="1">
+      <c r="D2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="2:15" ht="18" customHeight="1">
+      <c r="C3" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="43"/>
+      <c r="E3" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="45"/>
+      <c r="G3" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="18" customHeight="1">
+      <c r="C4" s="34"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="51"/>
+      <c r="I4" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="53"/>
+      <c r="K4" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="51"/>
+      <c r="M4" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="53"/>
+      <c r="O4" s="41"/>
+    </row>
+    <row r="5" spans="2:15" ht="18" customHeight="1" thickBot="1">
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" s="41"/>
+    </row>
+    <row r="6" spans="2:15" ht="18" customHeight="1" thickTop="1">
+      <c r="C6" s="38"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="26"/>
+    </row>
+    <row r="7" spans="2:15" ht="18" customHeight="1">
+      <c r="C7" s="39"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="27"/>
+    </row>
+    <row r="8" spans="2:15" ht="18" customHeight="1">
+      <c r="C8" s="40"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="26"/>
+    </row>
+    <row r="9" spans="2:15" ht="18" customHeight="1">
+      <c r="C9" s="39"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="27"/>
+    </row>
+    <row r="10" spans="2:15" ht="18" customHeight="1">
+      <c r="C10" s="40"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="26"/>
+    </row>
+    <row r="11" spans="2:15" ht="18" customHeight="1">
+      <c r="C11" s="39"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="27"/>
+    </row>
+    <row r="12" spans="2:15" ht="18" customHeight="1">
+      <c r="C12" s="40"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="26"/>
+    </row>
+    <row r="13" spans="2:15" ht="18" customHeight="1">
+      <c r="C13" s="39"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="27"/>
+    </row>
+    <row r="14" spans="2:15" ht="18" customHeight="1">
+      <c r="C14" s="40"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="26"/>
+    </row>
+    <row r="15" spans="2:15" ht="18" customHeight="1">
+      <c r="C15" s="39"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="27"/>
+    </row>
+    <row r="16" spans="2:15" ht="18" customHeight="1">
+      <c r="C16" s="40"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="26"/>
+    </row>
+    <row r="17" spans="3:15" ht="18" customHeight="1">
+      <c r="C17" s="39"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="27"/>
+    </row>
+    <row r="18" spans="3:15" ht="18" customHeight="1">
+      <c r="C18" s="40"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="26"/>
+    </row>
+    <row r="19" spans="3:15" ht="18" customHeight="1">
+      <c r="C19" s="39"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="27"/>
+    </row>
+    <row r="20" spans="3:15" ht="18" customHeight="1">
+      <c r="C20" s="40"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="26"/>
+    </row>
+    <row r="21" spans="3:15" ht="18" customHeight="1">
+      <c r="C21" s="39"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="27"/>
+    </row>
+    <row r="22" spans="3:15" ht="18" customHeight="1">
+      <c r="C22" s="40"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="26"/>
+    </row>
+    <row r="23" spans="3:15" ht="18" customHeight="1">
+      <c r="C23" s="39"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="27"/>
+    </row>
+    <row r="24" spans="3:15" ht="18" customHeight="1">
+      <c r="C24" s="40"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="26"/>
+    </row>
+    <row r="25" spans="3:15" ht="18" customHeight="1">
+      <c r="C25" s="39"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="27"/>
+    </row>
+    <row r="26" spans="3:15" ht="18" customHeight="1">
+      <c r="C26" s="40"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="26"/>
+    </row>
+    <row r="27" spans="3:15" ht="18" customHeight="1">
+      <c r="C27" s="39"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="27"/>
+    </row>
+    <row r="28" spans="3:15" ht="18" customHeight="1">
+      <c r="C28" s="40"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="26"/>
+    </row>
+    <row r="29" spans="3:15" ht="18" customHeight="1">
+      <c r="C29" s="39"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="27"/>
+    </row>
+    <row r="30" spans="3:15" ht="18" customHeight="1">
+      <c r="C30" s="40"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="26"/>
+    </row>
+    <row r="31" spans="3:15" ht="18" customHeight="1">
+      <c r="C31" s="39"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="27"/>
+    </row>
+    <row r="32" spans="3:15" ht="18" customHeight="1">
+      <c r="C32" s="40"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="26"/>
+    </row>
+    <row r="33" spans="3:15" ht="18" customHeight="1">
+      <c r="C33" s="39"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="27"/>
+    </row>
+    <row r="34" spans="3:15" ht="18" customHeight="1">
+      <c r="C34" s="40"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="21"/>
+      <c r="O34" s="26"/>
+    </row>
+    <row r="35" spans="3:15" ht="18" customHeight="1">
+      <c r="C35" s="39"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="27"/>
+    </row>
+    <row r="36" spans="3:15" ht="18" customHeight="1">
+      <c r="C36" s="40"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="21"/>
+      <c r="O36" s="26"/>
+    </row>
+    <row r="37" spans="3:15" ht="18" customHeight="1">
+      <c r="C37" s="39"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="27"/>
+    </row>
+    <row r="38" spans="3:15" ht="18" customHeight="1">
+      <c r="C38" s="38"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="30"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="26"/>
+    </row>
+    <row r="39" spans="3:15" ht="18" customHeight="1">
+      <c r="C39" s="39"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
+      <c r="N39" s="16"/>
+      <c r="O39" s="27"/>
+    </row>
+    <row r="40" spans="3:15" ht="18" customHeight="1">
+      <c r="C40" s="40"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="26"/>
+    </row>
+    <row r="41" spans="3:15" ht="18" customHeight="1">
+      <c r="C41" s="39"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="17"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="16"/>
+      <c r="N41" s="16"/>
+      <c r="O41" s="27"/>
+    </row>
+    <row r="42" spans="3:15" ht="18" customHeight="1">
+      <c r="C42" s="40"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="26"/>
+    </row>
+    <row r="43" spans="3:15" ht="18" customHeight="1">
+      <c r="C43" s="39"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="16"/>
+      <c r="N43" s="16"/>
+      <c r="O43" s="27"/>
+    </row>
+    <row r="44" spans="3:15" ht="18" customHeight="1">
+      <c r="C44" s="40"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="21"/>
+      <c r="M44" s="21"/>
+      <c r="N44" s="21"/>
+      <c r="O44" s="26"/>
+    </row>
+    <row r="45" spans="3:15" ht="18" customHeight="1">
+      <c r="C45" s="39"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="17"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="16"/>
+      <c r="M45" s="16"/>
+      <c r="N45" s="16"/>
+      <c r="O45" s="27"/>
+    </row>
+    <row r="46" spans="3:15" ht="18" customHeight="1">
+      <c r="C46" s="40"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="22"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="21"/>
+      <c r="N46" s="21"/>
+      <c r="O46" s="26"/>
+    </row>
+    <row r="47" spans="3:15" ht="18" customHeight="1">
+      <c r="C47" s="39"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="16"/>
+      <c r="M47" s="16"/>
+      <c r="N47" s="16"/>
+      <c r="O47" s="27"/>
+    </row>
+    <row r="48" spans="3:15" ht="18" customHeight="1">
+      <c r="C48" s="40"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="21"/>
+      <c r="M48" s="21"/>
+      <c r="N48" s="21"/>
+      <c r="O48" s="26"/>
+    </row>
+    <row r="49" spans="3:15" ht="18" customHeight="1">
+      <c r="C49" s="39"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="16"/>
+      <c r="I49" s="16"/>
+      <c r="J49" s="17"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="16"/>
+      <c r="M49" s="16"/>
+      <c r="N49" s="16"/>
+      <c r="O49" s="27"/>
+    </row>
+    <row r="50" spans="3:15" ht="18" customHeight="1">
+      <c r="C50" s="40"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="22"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="21"/>
+      <c r="M50" s="21"/>
+      <c r="N50" s="21"/>
+      <c r="O50" s="26"/>
+    </row>
+    <row r="51" spans="3:15" ht="18" customHeight="1">
+      <c r="C51" s="39"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="16"/>
+      <c r="I51" s="16"/>
+      <c r="J51" s="17"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="16"/>
+      <c r="M51" s="16"/>
+      <c r="N51" s="16"/>
+      <c r="O51" s="27"/>
+    </row>
+    <row r="52" spans="3:15" ht="18" customHeight="1">
+      <c r="C52" s="40"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="21"/>
+      <c r="J52" s="22"/>
+      <c r="K52" s="18"/>
+      <c r="L52" s="21"/>
+      <c r="M52" s="21"/>
+      <c r="N52" s="21"/>
+      <c r="O52" s="26"/>
+    </row>
+    <row r="53" spans="3:15" ht="18" customHeight="1">
+      <c r="C53" s="39"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="16"/>
+      <c r="J53" s="17"/>
+      <c r="K53" s="13"/>
+      <c r="L53" s="16"/>
+      <c r="M53" s="16"/>
+      <c r="N53" s="16"/>
+      <c r="O53" s="27"/>
+    </row>
+    <row r="54" spans="3:15" ht="18" customHeight="1">
+      <c r="C54" s="40"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="20"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="21"/>
+      <c r="J54" s="22"/>
+      <c r="K54" s="18"/>
+      <c r="L54" s="21"/>
+      <c r="M54" s="21"/>
+      <c r="N54" s="21"/>
+      <c r="O54" s="26"/>
+    </row>
+    <row r="55" spans="3:15" ht="18" customHeight="1">
+      <c r="C55" s="39"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="16"/>
+      <c r="I55" s="16"/>
+      <c r="J55" s="17"/>
+      <c r="K55" s="13"/>
+      <c r="L55" s="16"/>
+      <c r="M55" s="16"/>
+      <c r="N55" s="16"/>
+      <c r="O55" s="27"/>
+    </row>
+    <row r="56" spans="3:15" ht="18" customHeight="1">
+      <c r="C56" s="40"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="21"/>
+      <c r="I56" s="21"/>
+      <c r="J56" s="22"/>
+      <c r="K56" s="18"/>
+      <c r="L56" s="21"/>
+      <c r="M56" s="21"/>
+      <c r="N56" s="21"/>
+      <c r="O56" s="26"/>
+    </row>
+    <row r="57" spans="3:15" ht="18" customHeight="1">
+      <c r="C57" s="39"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="16"/>
+      <c r="I57" s="16"/>
+      <c r="J57" s="17"/>
+      <c r="K57" s="13"/>
+      <c r="L57" s="16"/>
+      <c r="M57" s="16"/>
+      <c r="N57" s="16"/>
+      <c r="O57" s="27"/>
+    </row>
+    <row r="58" spans="3:15" ht="18" customHeight="1">
+      <c r="C58" s="40"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="19"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="22"/>
+      <c r="K58" s="18"/>
+      <c r="L58" s="21"/>
+      <c r="M58" s="21"/>
+      <c r="N58" s="21"/>
+      <c r="O58" s="26"/>
+    </row>
+    <row r="59" spans="3:15" ht="18" customHeight="1">
+      <c r="C59" s="39"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="16"/>
+      <c r="I59" s="16"/>
+      <c r="J59" s="17"/>
+      <c r="K59" s="13"/>
+      <c r="L59" s="16"/>
+      <c r="M59" s="16"/>
+      <c r="N59" s="16"/>
+      <c r="O59" s="27"/>
+    </row>
+    <row r="60" spans="3:15" ht="18" customHeight="1">
+      <c r="C60" s="40"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="19"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="21"/>
+      <c r="I60" s="21"/>
+      <c r="J60" s="22"/>
+      <c r="K60" s="18"/>
+      <c r="L60" s="21"/>
+      <c r="M60" s="21"/>
+      <c r="N60" s="21"/>
+      <c r="O60" s="26"/>
+    </row>
+    <row r="61" spans="3:15" ht="18" customHeight="1">
+      <c r="C61" s="39"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="16"/>
+      <c r="I61" s="16"/>
+      <c r="J61" s="17"/>
+      <c r="K61" s="13"/>
+      <c r="L61" s="16"/>
+      <c r="M61" s="16"/>
+      <c r="N61" s="16"/>
+      <c r="O61" s="27"/>
+    </row>
+    <row r="62" spans="3:15" ht="18" customHeight="1">
+      <c r="C62" s="40"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="19"/>
+      <c r="G62" s="20"/>
+      <c r="H62" s="21"/>
+      <c r="I62" s="21"/>
+      <c r="J62" s="22"/>
+      <c r="K62" s="18"/>
+      <c r="L62" s="21"/>
+      <c r="M62" s="21"/>
+      <c r="N62" s="21"/>
+      <c r="O62" s="26"/>
+    </row>
+    <row r="63" spans="3:15" ht="18" customHeight="1">
+      <c r="C63" s="39"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="16"/>
+      <c r="I63" s="16"/>
+      <c r="J63" s="17"/>
+      <c r="K63" s="13"/>
+      <c r="L63" s="16"/>
+      <c r="M63" s="16"/>
+      <c r="N63" s="16"/>
+      <c r="O63" s="27"/>
+    </row>
+    <row r="64" spans="3:15" ht="18" customHeight="1">
+      <c r="C64" s="40"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="20"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="21"/>
+      <c r="J64" s="22"/>
+      <c r="K64" s="18"/>
+      <c r="L64" s="21"/>
+      <c r="M64" s="21"/>
+      <c r="N64" s="21"/>
+      <c r="O64" s="26"/>
+    </row>
+    <row r="65" spans="3:15" ht="18" customHeight="1">
+      <c r="C65" s="39"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="16"/>
+      <c r="I65" s="16"/>
+      <c r="J65" s="17"/>
+      <c r="K65" s="13"/>
+      <c r="L65" s="16"/>
+      <c r="M65" s="16"/>
+      <c r="N65" s="16"/>
+      <c r="O65" s="27"/>
+    </row>
+    <row r="66" spans="3:15" ht="18" customHeight="1">
+      <c r="C66" s="40"/>
+      <c r="D66" s="22"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="20"/>
+      <c r="H66" s="21"/>
+      <c r="I66" s="21"/>
+      <c r="J66" s="22"/>
+      <c r="K66" s="18"/>
+      <c r="L66" s="21"/>
+      <c r="M66" s="21"/>
+      <c r="N66" s="21"/>
+      <c r="O66" s="26"/>
+    </row>
+    <row r="67" spans="3:15" ht="18" customHeight="1">
+      <c r="C67" s="39"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="16"/>
+      <c r="I67" s="16"/>
+      <c r="J67" s="17"/>
+      <c r="K67" s="13"/>
+      <c r="L67" s="16"/>
+      <c r="M67" s="16"/>
+      <c r="N67" s="16"/>
+      <c r="O67" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="O3:O5"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+  </mergeCells>
+  <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.98425196850393704" bottom="0.39370078740157499" header="0.31496062992126" footer="0.31496062992126"/>
+  <pageSetup paperSize="9" scale="64" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;10日通システム株式会社 &amp;C&amp;"ＭＳ ゴシック,Regular"&amp;16標準報酬月額表（厚生年金）&amp;R&amp;"ＭＳ ゴシック,Regular"&amp;10&amp;KFF0000 &amp;K01+000&amp;D　&amp;T　
+&amp;KFF0000 &amp;K01+000page&amp;P</oddHeader>
+  </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[SMAL] QMM008 Screen F Fix bug 1527 1530
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_標準報酬月額表（厚生年金).xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_標準報酬月額表（厚生年金).xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\nts.uk\uk.pr\pr.file\nts.uk.file.pr.infra\src\main\resources\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nittsu\QMM008\MasterList\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="マスタリスト" sheetId="11" r:id="rId1"/>
@@ -1036,11 +1036,11 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="285271" y="218193"/>
-          <a:ext cx="9862365" cy="14562366"/>
+          <a:ext cx="9705482" cy="14562366"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 390"/>
+            <a:gd name="adj" fmla="val 0"/>
           </a:avLst>
         </a:prstGeom>
         <a:noFill/>
@@ -1105,11 +1105,11 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="287512" y="214831"/>
-          <a:ext cx="9855081" cy="14853719"/>
+          <a:ext cx="9721731" cy="14853719"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 390"/>
+            <a:gd name="adj" fmla="val 0"/>
           </a:avLst>
         </a:prstGeom>
         <a:noFill/>
@@ -44716,7 +44716,7 @@
   </sheetPr>
   <dimension ref="B1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12"/>
   <cols>
@@ -45778,8 +45778,8 @@
     <mergeCell ref="M4:N4"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
-  <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.98425196850393704" bottom="0.39370078740157499" header="0.31496062992126" footer="0.31496062992126"/>
-  <pageSetup paperSize="9" scale="64" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="65" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;10日通システム株式会社 &amp;C&amp;"ＭＳ ゴシック,Regular"&amp;16標準報酬月額表（厚生年金）&amp;R&amp;"ＭＳ ゴシック,Regular"&amp;10&amp;KFF0000 &amp;K01+000&amp;D　&amp;T　
 &amp;KFF0000 &amp;K01+000page&amp;P</oddHeader>
@@ -45795,7 +45795,7 @@
   </sheetPr>
   <dimension ref="B1:O67"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="85" workbookViewId="0"/>
+    <sheetView view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12"/>
   <cols>
@@ -46856,8 +46856,8 @@
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M4:N4"/>
   </mergeCells>
-  <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.98425196850393704" bottom="0.39370078740157499" header="0.31496062992126" footer="0.31496062992126"/>
-  <pageSetup paperSize="9" scale="64" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="65" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;10日通システム株式会社 &amp;C&amp;"ＭＳ ゴシック,Regular"&amp;16標準報酬月額表（厚生年金）&amp;R&amp;"ＭＳ ゴシック,Regular"&amp;10&amp;KFF0000 &amp;K01+000&amp;D　&amp;T　
 &amp;KFF0000 &amp;K01+000page&amp;P</oddHeader>

</xml_diff>

<commit_message>
[SMAL] QMM008_F fix bug 1558
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_標準報酬月額表（厚生年金).xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_標準報酬月額表（厚生年金).xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nittsu\QMM008\MasterList\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\nts.uk\uk.pr\pr.file\nts.uk.file.pr.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -44716,7 +44716,9 @@
   </sheetPr>
   <dimension ref="B1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3:O5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12"/>
   <cols>
@@ -44724,7 +44726,8 @@
     <col min="2" max="2" width="2.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" style="33" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="1" customWidth="1"/>
-    <col min="5" max="15" width="10.7109375" style="1"/>
+    <col min="5" max="14" width="10.7109375" style="1"/>
+    <col min="15" max="15" width="9.28515625" style="1" customWidth="1"/>
     <col min="16" max="16" width="1.28515625" style="1" customWidth="1"/>
     <col min="17" max="16384" width="10.7109375" style="1"/>
   </cols>
@@ -45779,7 +45782,7 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="65" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="64" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;10日通システム株式会社 &amp;C&amp;"ＭＳ ゴシック,Regular"&amp;16標準報酬月額表（厚生年金）&amp;R&amp;"ＭＳ ゴシック,Regular"&amp;10&amp;KFF0000 &amp;K01+000&amp;D　&amp;T　
 &amp;KFF0000 &amp;K01+000page&amp;P</oddHeader>

</xml_diff>

<commit_message>
[SMAL] QMM008_F  fix template
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_標準報酬月額表（厚生年金).xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_標準報酬月額表（厚生年金).xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="マスタリスト" sheetId="11" r:id="rId1"/>
-    <sheet name="マスタリスト (2)" sheetId="12" r:id="rId2"/>
+    <sheet name="マスタリスト (2)" sheetId="13" r:id="rId2"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
@@ -1105,7 +1105,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="287512" y="214831"/>
-          <a:ext cx="9721731" cy="14853719"/>
+          <a:ext cx="9759831" cy="14853719"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -44716,9 +44716,7 @@
   </sheetPr>
   <dimension ref="B1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:O5"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12"/>
   <cols>
@@ -45806,7 +45804,8 @@
     <col min="2" max="2" width="2.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" style="33" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="1" customWidth="1"/>
-    <col min="5" max="15" width="10.7109375" style="1"/>
+    <col min="5" max="14" width="10.7109375" style="1"/>
+    <col min="15" max="15" width="9.28515625" style="1" customWidth="1"/>
     <col min="16" max="16" width="1.28515625" style="1" customWidth="1"/>
     <col min="17" max="16384" width="10.7109375" style="1"/>
   </cols>
@@ -46860,7 +46859,7 @@
     <mergeCell ref="M4:N4"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="65" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="64" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;10日通システム株式会社 &amp;C&amp;"ＭＳ ゴシック,Regular"&amp;16標準報酬月額表（厚生年金）&amp;R&amp;"ＭＳ ゴシック,Regular"&amp;10&amp;KFF0000 &amp;K01+000&amp;D　&amp;T　
 &amp;KFF0000 &amp;K01+000page&amp;P</oddHeader>

</xml_diff>

<commit_message>
[SMAL] QMM008F fix template
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_標準報酬月額表（厚生年金).xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_標準報酬月額表（厚生年金).xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\uk\nts.uk\uk.pr\pr.file\nts.uk.file.pr.infra\src\main\resources\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\nts.uk\uk.pr\pr.file\nts.uk.file.pr.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="マスタリスト" sheetId="11" r:id="rId1"/>
-    <sheet name="マスタリスト (2)" sheetId="13" r:id="rId2"/>
+    <sheet name="マスタリスト (2)" sheetId="14" r:id="rId2"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
@@ -46,8 +46,8 @@
     <definedName name="_面接から採用に至るまでの情報管理とする_____アウトソーシングにて_採用された情報を_ファイ__ルにて取込を行う_">#REF!</definedName>
     <definedName name="・面接から採用に至るまでの情報管理とする。___・アウトソーシングにて_採用された情報を_ファイ__ルにて取込を行う。" localSheetId="1">#REF!</definedName>
     <definedName name="・面接から採用に至るまでの情報管理とする。___・アウトソーシングにて_採用された情報を_ファイ__ルにて取込を行う。">#REF!</definedName>
-    <definedName name="a" localSheetId="1">'[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="a">'[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
+    <definedName name="a" localSheetId="1">[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="a">[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
     <definedName name="AAA" localSheetId="1">#REF!</definedName>
     <definedName name="AAA">#REF!</definedName>
     <definedName name="AAAA" hidden="1">{"VIEW1",#N/A,FALSE,"懸案事項";"VIEW2",#N/A,FALSE,"懸案事項"}</definedName>
@@ -94,8 +94,8 @@
     <definedName name="ＭＨ">#REF!</definedName>
     <definedName name="Ｍホ" localSheetId="1">#REF!</definedName>
     <definedName name="Ｍホ">#REF!</definedName>
-    <definedName name="ｎ" localSheetId="1">'[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="ｎ">'[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
+    <definedName name="ｎ" localSheetId="1">[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="ｎ">[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
     <definedName name="ＯＨ" localSheetId="1">#REF!</definedName>
     <definedName name="ＯＨ">#REF!</definedName>
     <definedName name="OPT_NO" localSheetId="1">[5]!OPT_NO</definedName>
@@ -153,10 +153,10 @@
     <definedName name="クニホ">#REF!</definedName>
     <definedName name="クホ" localSheetId="1">#REF!</definedName>
     <definedName name="クホ">#REF!</definedName>
-    <definedName name="サＨ" localSheetId="1">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サＨ">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サホ" localSheetId="1">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サホ">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
+    <definedName name="サＨ" localSheetId="1">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サＨ">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サホ" localSheetId="1">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サホ">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
     <definedName name="サホ1" localSheetId="1">#REF!</definedName>
     <definedName name="サホ1">#REF!</definedName>
     <definedName name="ツール別見積工数" localSheetId="1">#REF!</definedName>
@@ -330,7 +330,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -409,7 +409,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="52">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -816,272 +816,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </left>
-      <right style="thin">
-        <color theme="6"/>
-      </right>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="6"/>
-      </left>
-      <right style="thin">
-        <color theme="6"/>
-      </right>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right style="thick">
-        <color theme="6"/>
-      </right>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="6"/>
-      </right>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right style="thin">
-        <color theme="6"/>
-      </right>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </right>
-      <top style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color theme="6" tint="0.79992065187536243"/>
-      </left>
-      <right style="thin">
-        <color theme="6" tint="0.79998168889431442"/>
-      </right>
-      <top style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="thin">
-        <color theme="6" tint="0.79998168889431442"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6" tint="0.79998168889431442"/>
-      </left>
-      <right style="thin">
-        <color theme="6" tint="0.79998168889431442"/>
-      </right>
-      <top style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="thin">
-        <color theme="6" tint="0.79998168889431442"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6" tint="0.79998168889431442"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="thin">
-        <color theme="6" tint="0.79998168889431442"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color theme="6" tint="0.79998168889431442"/>
-      </left>
-      <right style="thin">
-        <color theme="6" tint="0.79998168889431442"/>
-      </right>
-      <top style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="thin">
-        <color theme="6" tint="0.79998168889431442"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6" tint="0.79998168889431442"/>
-      </left>
-      <right style="double">
-        <color theme="6" tint="0.79992065187536243"/>
-      </right>
-      <top style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="thin">
-        <color theme="6" tint="0.79998168889431442"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </left>
-      <right style="thin">
-        <color theme="6" tint="0.79998168889431442"/>
-      </right>
-      <top style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="thin">
-        <color theme="6" tint="0.79998168889431442"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6" tint="0.79998168889431442"/>
-      </left>
-      <right style="double">
-        <color theme="6" tint="0.79998168889431442"/>
-      </right>
-      <top style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="thin">
-        <color theme="6" tint="0.79998168889431442"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="6" tint="-0.249977111117893"/>
-      </left>
-      <right style="thin">
-        <color theme="6" tint="0.79998168889431442"/>
-      </right>
-      <top style="thin">
-        <color theme="6" tint="0.79998168889431442"/>
-      </top>
-      <bottom style="thin">
-        <color theme="6" tint="0.79998168889431442"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1093,7 +827,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1173,6 +907,9 @@
     <xf numFmtId="38" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="38" fontId="4" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="40" fontId="4" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1202,6 +939,18 @@
     </xf>
     <xf numFmtId="40" fontId="4" fillId="0" borderId="30" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1239,96 +988,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="4" fillId="3" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="4" fillId="3" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="4" fillId="3" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="4" fillId="3" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="4" fillId="3" borderId="38" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="4" fillId="0" borderId="32" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="4" fillId="3" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="38" fontId="4" fillId="3" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="4" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="4" fillId="3" borderId="41" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="39" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
@@ -1352,6 +1011,144 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>173212</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>5281</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>17518</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="角丸四角形 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="285271" y="218193"/>
+          <a:ext cx="9705482" cy="14562366"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 0"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>173212</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>5281</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>17518</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="角丸四角形 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="277987" y="214831"/>
+          <a:ext cx="11569581" cy="14853719"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 0"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -44917,17 +44714,20 @@
   <sheetPr codeName="Sheet7">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:O68"/>
+  <dimension ref="B1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="2.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" style="32" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="33" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="1" customWidth="1"/>
-    <col min="5" max="14" width="10.7109375" style="1"/>
+    <col min="5" max="6" width="10.7109375" style="1"/>
+    <col min="7" max="14" width="14.42578125" style="1" customWidth="1"/>
     <col min="15" max="15" width="9.28515625" style="1" customWidth="1"/>
     <col min="16" max="16" width="1.28515625" style="1" customWidth="1"/>
     <col min="17" max="16384" width="10.7109375" style="1"/>
@@ -44947,73 +44747,60 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:15" ht="4.9000000000000004" customHeight="1" thickBot="1">
-      <c r="C2" s="66"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
+    <row r="2" spans="2:15" ht="4.9000000000000004" customHeight="1">
+      <c r="D2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:15" ht="18" customHeight="1" thickTop="1">
-      <c r="B3" s="52"/>
-      <c r="C3" s="37" t="s">
+    <row r="3" spans="2:15" ht="18" customHeight="1">
+      <c r="C3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="39" t="s">
+      <c r="D3" s="43"/>
+      <c r="E3" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41" t="s">
+      <c r="F3" s="45"/>
+      <c r="G3" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="41" t="s">
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="62" t="s">
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="41" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:15" ht="18" customHeight="1">
-      <c r="B4" s="52"/>
-      <c r="C4" s="33"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="23"/>
       <c r="E4" s="24"/>
       <c r="F4" s="25"/>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="46"/>
-      <c r="I4" s="47" t="s">
+      <c r="H4" s="51"/>
+      <c r="I4" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="48"/>
-      <c r="K4" s="45" t="s">
+      <c r="J4" s="53"/>
+      <c r="K4" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="46"/>
-      <c r="M4" s="47" t="s">
+      <c r="L4" s="51"/>
+      <c r="M4" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="48"/>
-      <c r="O4" s="62"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="41"/>
     </row>
     <row r="5" spans="2:15" ht="18" customHeight="1" thickBot="1">
-      <c r="B5" s="52"/>
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
@@ -45050,27 +44837,25 @@
       <c r="N5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="62"/>
+      <c r="O5" s="41"/>
     </row>
     <row r="6" spans="2:15" ht="18" customHeight="1" thickTop="1">
-      <c r="B6" s="52"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="31"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="32"/>
       <c r="E6" s="11"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="60"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="26"/>
     </row>
     <row r="7" spans="2:15" ht="18" customHeight="1">
-      <c r="B7" s="52"/>
-      <c r="C7" s="50"/>
+      <c r="C7" s="39"/>
       <c r="D7" s="17"/>
       <c r="E7" s="13"/>
       <c r="F7" s="14"/>
@@ -45082,11 +44867,10 @@
       <c r="L7" s="16"/>
       <c r="M7" s="16"/>
       <c r="N7" s="16"/>
-      <c r="O7" s="61"/>
+      <c r="O7" s="27"/>
     </row>
     <row r="8" spans="2:15" ht="18" customHeight="1">
-      <c r="B8" s="52"/>
-      <c r="C8" s="51"/>
+      <c r="C8" s="40"/>
       <c r="D8" s="22"/>
       <c r="E8" s="18"/>
       <c r="F8" s="19"/>
@@ -45098,11 +44882,10 @@
       <c r="L8" s="21"/>
       <c r="M8" s="21"/>
       <c r="N8" s="21"/>
-      <c r="O8" s="60"/>
+      <c r="O8" s="26"/>
     </row>
     <row r="9" spans="2:15" ht="18" customHeight="1">
-      <c r="B9" s="52"/>
-      <c r="C9" s="50"/>
+      <c r="C9" s="39"/>
       <c r="D9" s="17"/>
       <c r="E9" s="13"/>
       <c r="F9" s="14"/>
@@ -45114,11 +44897,10 @@
       <c r="L9" s="16"/>
       <c r="M9" s="16"/>
       <c r="N9" s="16"/>
-      <c r="O9" s="61"/>
+      <c r="O9" s="27"/>
     </row>
     <row r="10" spans="2:15" ht="18" customHeight="1">
-      <c r="B10" s="52"/>
-      <c r="C10" s="51"/>
+      <c r="C10" s="40"/>
       <c r="D10" s="22"/>
       <c r="E10" s="18"/>
       <c r="F10" s="19"/>
@@ -45130,11 +44912,10 @@
       <c r="L10" s="21"/>
       <c r="M10" s="21"/>
       <c r="N10" s="21"/>
-      <c r="O10" s="60"/>
+      <c r="O10" s="26"/>
     </row>
     <row r="11" spans="2:15" ht="18" customHeight="1">
-      <c r="B11" s="52"/>
-      <c r="C11" s="50"/>
+      <c r="C11" s="39"/>
       <c r="D11" s="17"/>
       <c r="E11" s="13"/>
       <c r="F11" s="14"/>
@@ -45146,11 +44927,10 @@
       <c r="L11" s="16"/>
       <c r="M11" s="16"/>
       <c r="N11" s="16"/>
-      <c r="O11" s="61"/>
+      <c r="O11" s="27"/>
     </row>
     <row r="12" spans="2:15" ht="18" customHeight="1">
-      <c r="B12" s="52"/>
-      <c r="C12" s="51"/>
+      <c r="C12" s="40"/>
       <c r="D12" s="22"/>
       <c r="E12" s="18"/>
       <c r="F12" s="19"/>
@@ -45162,11 +44942,10 @@
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
       <c r="N12" s="21"/>
-      <c r="O12" s="60"/>
+      <c r="O12" s="26"/>
     </row>
     <row r="13" spans="2:15" ht="18" customHeight="1">
-      <c r="B13" s="52"/>
-      <c r="C13" s="50"/>
+      <c r="C13" s="39"/>
       <c r="D13" s="17"/>
       <c r="E13" s="13"/>
       <c r="F13" s="14"/>
@@ -45178,11 +44957,10 @@
       <c r="L13" s="16"/>
       <c r="M13" s="16"/>
       <c r="N13" s="16"/>
-      <c r="O13" s="61"/>
+      <c r="O13" s="27"/>
     </row>
     <row r="14" spans="2:15" ht="18" customHeight="1">
-      <c r="B14" s="52"/>
-      <c r="C14" s="51"/>
+      <c r="C14" s="40"/>
       <c r="D14" s="22"/>
       <c r="E14" s="18"/>
       <c r="F14" s="19"/>
@@ -45194,11 +44972,10 @@
       <c r="L14" s="21"/>
       <c r="M14" s="21"/>
       <c r="N14" s="21"/>
-      <c r="O14" s="60"/>
+      <c r="O14" s="26"/>
     </row>
     <row r="15" spans="2:15" ht="18" customHeight="1">
-      <c r="B15" s="52"/>
-      <c r="C15" s="50"/>
+      <c r="C15" s="39"/>
       <c r="D15" s="17"/>
       <c r="E15" s="13"/>
       <c r="F15" s="14"/>
@@ -45210,11 +44987,10 @@
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
       <c r="N15" s="16"/>
-      <c r="O15" s="61"/>
+      <c r="O15" s="27"/>
     </row>
     <row r="16" spans="2:15" ht="18" customHeight="1">
-      <c r="B16" s="52"/>
-      <c r="C16" s="51"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="22"/>
       <c r="E16" s="18"/>
       <c r="F16" s="19"/>
@@ -45226,11 +45002,10 @@
       <c r="L16" s="21"/>
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>
-      <c r="O16" s="60"/>
+      <c r="O16" s="26"/>
     </row>
-    <row r="17" spans="2:15" ht="18" customHeight="1">
-      <c r="B17" s="52"/>
-      <c r="C17" s="50"/>
+    <row r="17" spans="3:15" ht="18" customHeight="1">
+      <c r="C17" s="39"/>
       <c r="D17" s="17"/>
       <c r="E17" s="13"/>
       <c r="F17" s="14"/>
@@ -45242,11 +45017,10 @@
       <c r="L17" s="16"/>
       <c r="M17" s="16"/>
       <c r="N17" s="16"/>
-      <c r="O17" s="63"/>
+      <c r="O17" s="27"/>
     </row>
-    <row r="18" spans="2:15" ht="18" customHeight="1">
-      <c r="B18" s="52"/>
-      <c r="C18" s="51"/>
+    <row r="18" spans="3:15" ht="18" customHeight="1">
+      <c r="C18" s="40"/>
       <c r="D18" s="22"/>
       <c r="E18" s="18"/>
       <c r="F18" s="19"/>
@@ -45258,11 +45032,10 @@
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
       <c r="N18" s="21"/>
-      <c r="O18" s="64"/>
+      <c r="O18" s="26"/>
     </row>
-    <row r="19" spans="2:15" ht="18" customHeight="1">
-      <c r="B19" s="52"/>
-      <c r="C19" s="50"/>
+    <row r="19" spans="3:15" ht="18" customHeight="1">
+      <c r="C19" s="39"/>
       <c r="D19" s="17"/>
       <c r="E19" s="13"/>
       <c r="F19" s="14"/>
@@ -45274,11 +45047,10 @@
       <c r="L19" s="16"/>
       <c r="M19" s="16"/>
       <c r="N19" s="16"/>
-      <c r="O19" s="63"/>
+      <c r="O19" s="27"/>
     </row>
-    <row r="20" spans="2:15" ht="18" customHeight="1">
-      <c r="B20" s="52"/>
-      <c r="C20" s="51"/>
+    <row r="20" spans="3:15" ht="18" customHeight="1">
+      <c r="C20" s="40"/>
       <c r="D20" s="22"/>
       <c r="E20" s="18"/>
       <c r="F20" s="19"/>
@@ -45290,11 +45062,10 @@
       <c r="L20" s="21"/>
       <c r="M20" s="21"/>
       <c r="N20" s="21"/>
-      <c r="O20" s="64"/>
+      <c r="O20" s="26"/>
     </row>
-    <row r="21" spans="2:15" ht="18" customHeight="1">
-      <c r="B21" s="52"/>
-      <c r="C21" s="50"/>
+    <row r="21" spans="3:15" ht="18" customHeight="1">
+      <c r="C21" s="39"/>
       <c r="D21" s="17"/>
       <c r="E21" s="13"/>
       <c r="F21" s="14"/>
@@ -45306,11 +45077,10 @@
       <c r="L21" s="16"/>
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
-      <c r="O21" s="63"/>
+      <c r="O21" s="27"/>
     </row>
-    <row r="22" spans="2:15" ht="18" customHeight="1">
-      <c r="B22" s="52"/>
-      <c r="C22" s="51"/>
+    <row r="22" spans="3:15" ht="18" customHeight="1">
+      <c r="C22" s="40"/>
       <c r="D22" s="22"/>
       <c r="E22" s="18"/>
       <c r="F22" s="19"/>
@@ -45322,11 +45092,10 @@
       <c r="L22" s="21"/>
       <c r="M22" s="21"/>
       <c r="N22" s="21"/>
-      <c r="O22" s="64"/>
+      <c r="O22" s="26"/>
     </row>
-    <row r="23" spans="2:15" ht="18" customHeight="1">
-      <c r="B23" s="52"/>
-      <c r="C23" s="50"/>
+    <row r="23" spans="3:15" ht="18" customHeight="1">
+      <c r="C23" s="39"/>
       <c r="D23" s="17"/>
       <c r="E23" s="13"/>
       <c r="F23" s="14"/>
@@ -45338,11 +45107,10 @@
       <c r="L23" s="16"/>
       <c r="M23" s="16"/>
       <c r="N23" s="16"/>
-      <c r="O23" s="63"/>
+      <c r="O23" s="27"/>
     </row>
-    <row r="24" spans="2:15" ht="18" customHeight="1">
-      <c r="B24" s="52"/>
-      <c r="C24" s="51"/>
+    <row r="24" spans="3:15" ht="18" customHeight="1">
+      <c r="C24" s="40"/>
       <c r="D24" s="22"/>
       <c r="E24" s="18"/>
       <c r="F24" s="19"/>
@@ -45354,11 +45122,10 @@
       <c r="L24" s="21"/>
       <c r="M24" s="21"/>
       <c r="N24" s="21"/>
-      <c r="O24" s="64"/>
+      <c r="O24" s="26"/>
     </row>
-    <row r="25" spans="2:15" ht="18" customHeight="1">
-      <c r="B25" s="52"/>
-      <c r="C25" s="50"/>
+    <row r="25" spans="3:15" ht="18" customHeight="1">
+      <c r="C25" s="39"/>
       <c r="D25" s="17"/>
       <c r="E25" s="13"/>
       <c r="F25" s="14"/>
@@ -45370,11 +45137,10 @@
       <c r="L25" s="16"/>
       <c r="M25" s="16"/>
       <c r="N25" s="16"/>
-      <c r="O25" s="63"/>
+      <c r="O25" s="27"/>
     </row>
-    <row r="26" spans="2:15" ht="18" customHeight="1">
-      <c r="B26" s="52"/>
-      <c r="C26" s="51"/>
+    <row r="26" spans="3:15" ht="18" customHeight="1">
+      <c r="C26" s="40"/>
       <c r="D26" s="22"/>
       <c r="E26" s="18"/>
       <c r="F26" s="19"/>
@@ -45386,11 +45152,10 @@
       <c r="L26" s="21"/>
       <c r="M26" s="21"/>
       <c r="N26" s="21"/>
-      <c r="O26" s="64"/>
+      <c r="O26" s="26"/>
     </row>
-    <row r="27" spans="2:15" ht="18" customHeight="1">
-      <c r="B27" s="52"/>
-      <c r="C27" s="50"/>
+    <row r="27" spans="3:15" ht="18" customHeight="1">
+      <c r="C27" s="39"/>
       <c r="D27" s="17"/>
       <c r="E27" s="13"/>
       <c r="F27" s="14"/>
@@ -45402,11 +45167,10 @@
       <c r="L27" s="16"/>
       <c r="M27" s="16"/>
       <c r="N27" s="16"/>
-      <c r="O27" s="63"/>
+      <c r="O27" s="27"/>
     </row>
-    <row r="28" spans="2:15" ht="18" customHeight="1">
-      <c r="B28" s="52"/>
-      <c r="C28" s="51"/>
+    <row r="28" spans="3:15" ht="18" customHeight="1">
+      <c r="C28" s="40"/>
       <c r="D28" s="22"/>
       <c r="E28" s="18"/>
       <c r="F28" s="19"/>
@@ -45418,11 +45182,10 @@
       <c r="L28" s="21"/>
       <c r="M28" s="21"/>
       <c r="N28" s="21"/>
-      <c r="O28" s="64"/>
+      <c r="O28" s="26"/>
     </row>
-    <row r="29" spans="2:15" ht="18" customHeight="1">
-      <c r="B29" s="52"/>
-      <c r="C29" s="50"/>
+    <row r="29" spans="3:15" ht="18" customHeight="1">
+      <c r="C29" s="39"/>
       <c r="D29" s="17"/>
       <c r="E29" s="13"/>
       <c r="F29" s="14"/>
@@ -45434,11 +45197,10 @@
       <c r="L29" s="16"/>
       <c r="M29" s="16"/>
       <c r="N29" s="16"/>
-      <c r="O29" s="63"/>
+      <c r="O29" s="27"/>
     </row>
-    <row r="30" spans="2:15" ht="18" customHeight="1">
-      <c r="B30" s="52"/>
-      <c r="C30" s="51"/>
+    <row r="30" spans="3:15" ht="18" customHeight="1">
+      <c r="C30" s="40"/>
       <c r="D30" s="22"/>
       <c r="E30" s="18"/>
       <c r="F30" s="19"/>
@@ -45450,11 +45212,10 @@
       <c r="L30" s="21"/>
       <c r="M30" s="21"/>
       <c r="N30" s="21"/>
-      <c r="O30" s="64"/>
+      <c r="O30" s="26"/>
     </row>
-    <row r="31" spans="2:15" ht="18" customHeight="1">
-      <c r="B31" s="52"/>
-      <c r="C31" s="50"/>
+    <row r="31" spans="3:15" ht="18" customHeight="1">
+      <c r="C31" s="39"/>
       <c r="D31" s="17"/>
       <c r="E31" s="13"/>
       <c r="F31" s="14"/>
@@ -45466,11 +45227,10 @@
       <c r="L31" s="16"/>
       <c r="M31" s="16"/>
       <c r="N31" s="16"/>
-      <c r="O31" s="63"/>
+      <c r="O31" s="27"/>
     </row>
-    <row r="32" spans="2:15" ht="18" customHeight="1">
-      <c r="B32" s="52"/>
-      <c r="C32" s="51"/>
+    <row r="32" spans="3:15" ht="18" customHeight="1">
+      <c r="C32" s="40"/>
       <c r="D32" s="22"/>
       <c r="E32" s="18"/>
       <c r="F32" s="19"/>
@@ -45482,11 +45242,10 @@
       <c r="L32" s="21"/>
       <c r="M32" s="21"/>
       <c r="N32" s="21"/>
-      <c r="O32" s="64"/>
+      <c r="O32" s="26"/>
     </row>
-    <row r="33" spans="2:15" ht="18" customHeight="1">
-      <c r="B33" s="52"/>
-      <c r="C33" s="50"/>
+    <row r="33" spans="3:15" ht="18" customHeight="1">
+      <c r="C33" s="39"/>
       <c r="D33" s="17"/>
       <c r="E33" s="13"/>
       <c r="F33" s="14"/>
@@ -45498,11 +45257,10 @@
       <c r="L33" s="16"/>
       <c r="M33" s="16"/>
       <c r="N33" s="16"/>
-      <c r="O33" s="63"/>
+      <c r="O33" s="27"/>
     </row>
-    <row r="34" spans="2:15" ht="18" customHeight="1">
-      <c r="B34" s="52"/>
-      <c r="C34" s="51"/>
+    <row r="34" spans="3:15" ht="18" customHeight="1">
+      <c r="C34" s="40"/>
       <c r="D34" s="22"/>
       <c r="E34" s="18"/>
       <c r="F34" s="19"/>
@@ -45514,11 +45272,10 @@
       <c r="L34" s="21"/>
       <c r="M34" s="21"/>
       <c r="N34" s="21"/>
-      <c r="O34" s="64"/>
+      <c r="O34" s="26"/>
     </row>
-    <row r="35" spans="2:15" ht="18" customHeight="1">
-      <c r="B35" s="52"/>
-      <c r="C35" s="50"/>
+    <row r="35" spans="3:15" ht="18" customHeight="1">
+      <c r="C35" s="39"/>
       <c r="D35" s="17"/>
       <c r="E35" s="13"/>
       <c r="F35" s="14"/>
@@ -45530,11 +45287,10 @@
       <c r="L35" s="16"/>
       <c r="M35" s="16"/>
       <c r="N35" s="16"/>
-      <c r="O35" s="63"/>
+      <c r="O35" s="27"/>
     </row>
-    <row r="36" spans="2:15" ht="18" customHeight="1">
-      <c r="B36" s="52"/>
-      <c r="C36" s="51"/>
+    <row r="36" spans="3:15" ht="18" customHeight="1">
+      <c r="C36" s="40"/>
       <c r="D36" s="22"/>
       <c r="E36" s="18"/>
       <c r="F36" s="19"/>
@@ -45546,11 +45302,10 @@
       <c r="L36" s="21"/>
       <c r="M36" s="21"/>
       <c r="N36" s="21"/>
-      <c r="O36" s="64"/>
+      <c r="O36" s="26"/>
     </row>
-    <row r="37" spans="2:15" ht="18" customHeight="1">
-      <c r="B37" s="52"/>
-      <c r="C37" s="50"/>
+    <row r="37" spans="3:15" ht="18" customHeight="1">
+      <c r="C37" s="39"/>
       <c r="D37" s="17"/>
       <c r="E37" s="13"/>
       <c r="F37" s="14"/>
@@ -45562,27 +45317,25 @@
       <c r="L37" s="16"/>
       <c r="M37" s="16"/>
       <c r="N37" s="16"/>
-      <c r="O37" s="63"/>
+      <c r="O37" s="27"/>
     </row>
-    <row r="38" spans="2:15" ht="18" customHeight="1">
-      <c r="B38" s="52"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="28"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="36"/>
-      <c r="L38" s="28"/>
-      <c r="M38" s="28"/>
-      <c r="N38" s="28"/>
-      <c r="O38" s="64"/>
+    <row r="38" spans="3:15" ht="18" customHeight="1">
+      <c r="C38" s="38"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="30"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="26"/>
     </row>
-    <row r="39" spans="2:15" ht="18" customHeight="1">
-      <c r="B39" s="52"/>
-      <c r="C39" s="50"/>
+    <row r="39" spans="3:15" ht="18" customHeight="1">
+      <c r="C39" s="39"/>
       <c r="D39" s="17"/>
       <c r="E39" s="13"/>
       <c r="F39" s="14"/>
@@ -45594,11 +45347,10 @@
       <c r="L39" s="16"/>
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
-      <c r="O39" s="63"/>
+      <c r="O39" s="27"/>
     </row>
-    <row r="40" spans="2:15" ht="18" customHeight="1">
-      <c r="B40" s="52"/>
-      <c r="C40" s="51"/>
+    <row r="40" spans="3:15" ht="18" customHeight="1">
+      <c r="C40" s="40"/>
       <c r="D40" s="22"/>
       <c r="E40" s="18"/>
       <c r="F40" s="19"/>
@@ -45610,11 +45362,10 @@
       <c r="L40" s="21"/>
       <c r="M40" s="21"/>
       <c r="N40" s="21"/>
-      <c r="O40" s="64"/>
+      <c r="O40" s="26"/>
     </row>
-    <row r="41" spans="2:15" ht="18" customHeight="1">
-      <c r="B41" s="52"/>
-      <c r="C41" s="50"/>
+    <row r="41" spans="3:15" ht="18" customHeight="1">
+      <c r="C41" s="39"/>
       <c r="D41" s="17"/>
       <c r="E41" s="13"/>
       <c r="F41" s="14"/>
@@ -45626,11 +45377,10 @@
       <c r="L41" s="16"/>
       <c r="M41" s="16"/>
       <c r="N41" s="16"/>
-      <c r="O41" s="63"/>
+      <c r="O41" s="27"/>
     </row>
-    <row r="42" spans="2:15" ht="18" customHeight="1">
-      <c r="B42" s="52"/>
-      <c r="C42" s="51"/>
+    <row r="42" spans="3:15" ht="18" customHeight="1">
+      <c r="C42" s="40"/>
       <c r="D42" s="22"/>
       <c r="E42" s="18"/>
       <c r="F42" s="19"/>
@@ -45642,11 +45392,10 @@
       <c r="L42" s="21"/>
       <c r="M42" s="21"/>
       <c r="N42" s="21"/>
-      <c r="O42" s="64"/>
+      <c r="O42" s="26"/>
     </row>
-    <row r="43" spans="2:15" ht="18" customHeight="1">
-      <c r="B43" s="52"/>
-      <c r="C43" s="50"/>
+    <row r="43" spans="3:15" ht="18" customHeight="1">
+      <c r="C43" s="39"/>
       <c r="D43" s="17"/>
       <c r="E43" s="13"/>
       <c r="F43" s="14"/>
@@ -45658,11 +45407,10 @@
       <c r="L43" s="16"/>
       <c r="M43" s="16"/>
       <c r="N43" s="16"/>
-      <c r="O43" s="63"/>
+      <c r="O43" s="27"/>
     </row>
-    <row r="44" spans="2:15" ht="18" customHeight="1">
-      <c r="B44" s="52"/>
-      <c r="C44" s="51"/>
+    <row r="44" spans="3:15" ht="18" customHeight="1">
+      <c r="C44" s="40"/>
       <c r="D44" s="22"/>
       <c r="E44" s="18"/>
       <c r="F44" s="19"/>
@@ -45674,11 +45422,10 @@
       <c r="L44" s="21"/>
       <c r="M44" s="21"/>
       <c r="N44" s="21"/>
-      <c r="O44" s="64"/>
+      <c r="O44" s="26"/>
     </row>
-    <row r="45" spans="2:15" ht="18" customHeight="1">
-      <c r="B45" s="52"/>
-      <c r="C45" s="50"/>
+    <row r="45" spans="3:15" ht="18" customHeight="1">
+      <c r="C45" s="39"/>
       <c r="D45" s="17"/>
       <c r="E45" s="13"/>
       <c r="F45" s="14"/>
@@ -45690,11 +45437,10 @@
       <c r="L45" s="16"/>
       <c r="M45" s="16"/>
       <c r="N45" s="16"/>
-      <c r="O45" s="63"/>
+      <c r="O45" s="27"/>
     </row>
-    <row r="46" spans="2:15" ht="18" customHeight="1">
-      <c r="B46" s="52"/>
-      <c r="C46" s="51"/>
+    <row r="46" spans="3:15" ht="18" customHeight="1">
+      <c r="C46" s="40"/>
       <c r="D46" s="22"/>
       <c r="E46" s="18"/>
       <c r="F46" s="19"/>
@@ -45706,11 +45452,10 @@
       <c r="L46" s="21"/>
       <c r="M46" s="21"/>
       <c r="N46" s="21"/>
-      <c r="O46" s="64"/>
+      <c r="O46" s="26"/>
     </row>
-    <row r="47" spans="2:15" ht="18" customHeight="1">
-      <c r="B47" s="52"/>
-      <c r="C47" s="50"/>
+    <row r="47" spans="3:15" ht="18" customHeight="1">
+      <c r="C47" s="39"/>
       <c r="D47" s="17"/>
       <c r="E47" s="13"/>
       <c r="F47" s="14"/>
@@ -45722,11 +45467,10 @@
       <c r="L47" s="16"/>
       <c r="M47" s="16"/>
       <c r="N47" s="16"/>
-      <c r="O47" s="63"/>
+      <c r="O47" s="27"/>
     </row>
-    <row r="48" spans="2:15" ht="18" customHeight="1">
-      <c r="B48" s="52"/>
-      <c r="C48" s="51"/>
+    <row r="48" spans="3:15" ht="18" customHeight="1">
+      <c r="C48" s="40"/>
       <c r="D48" s="22"/>
       <c r="E48" s="18"/>
       <c r="F48" s="19"/>
@@ -45738,11 +45482,10 @@
       <c r="L48" s="21"/>
       <c r="M48" s="21"/>
       <c r="N48" s="21"/>
-      <c r="O48" s="64"/>
+      <c r="O48" s="26"/>
     </row>
-    <row r="49" spans="2:15" ht="18" customHeight="1">
-      <c r="B49" s="52"/>
-      <c r="C49" s="50"/>
+    <row r="49" spans="3:15" ht="18" customHeight="1">
+      <c r="C49" s="39"/>
       <c r="D49" s="17"/>
       <c r="E49" s="13"/>
       <c r="F49" s="14"/>
@@ -45754,11 +45497,10 @@
       <c r="L49" s="16"/>
       <c r="M49" s="16"/>
       <c r="N49" s="16"/>
-      <c r="O49" s="63"/>
+      <c r="O49" s="27"/>
     </row>
-    <row r="50" spans="2:15" ht="18" customHeight="1">
-      <c r="B50" s="52"/>
-      <c r="C50" s="51"/>
+    <row r="50" spans="3:15" ht="18" customHeight="1">
+      <c r="C50" s="40"/>
       <c r="D50" s="22"/>
       <c r="E50" s="18"/>
       <c r="F50" s="19"/>
@@ -45770,11 +45512,10 @@
       <c r="L50" s="21"/>
       <c r="M50" s="21"/>
       <c r="N50" s="21"/>
-      <c r="O50" s="64"/>
+      <c r="O50" s="26"/>
     </row>
-    <row r="51" spans="2:15" ht="18" customHeight="1">
-      <c r="B51" s="52"/>
-      <c r="C51" s="50"/>
+    <row r="51" spans="3:15" ht="18" customHeight="1">
+      <c r="C51" s="39"/>
       <c r="D51" s="17"/>
       <c r="E51" s="13"/>
       <c r="F51" s="14"/>
@@ -45786,11 +45527,10 @@
       <c r="L51" s="16"/>
       <c r="M51" s="16"/>
       <c r="N51" s="16"/>
-      <c r="O51" s="63"/>
+      <c r="O51" s="27"/>
     </row>
-    <row r="52" spans="2:15" ht="18" customHeight="1">
-      <c r="B52" s="52"/>
-      <c r="C52" s="51"/>
+    <row r="52" spans="3:15" ht="18" customHeight="1">
+      <c r="C52" s="40"/>
       <c r="D52" s="22"/>
       <c r="E52" s="18"/>
       <c r="F52" s="19"/>
@@ -45802,11 +45542,10 @@
       <c r="L52" s="21"/>
       <c r="M52" s="21"/>
       <c r="N52" s="21"/>
-      <c r="O52" s="64"/>
+      <c r="O52" s="26"/>
     </row>
-    <row r="53" spans="2:15" ht="18" customHeight="1">
-      <c r="B53" s="52"/>
-      <c r="C53" s="50"/>
+    <row r="53" spans="3:15" ht="18" customHeight="1">
+      <c r="C53" s="39"/>
       <c r="D53" s="17"/>
       <c r="E53" s="13"/>
       <c r="F53" s="14"/>
@@ -45818,11 +45557,10 @@
       <c r="L53" s="16"/>
       <c r="M53" s="16"/>
       <c r="N53" s="16"/>
-      <c r="O53" s="63"/>
+      <c r="O53" s="27"/>
     </row>
-    <row r="54" spans="2:15" ht="18" customHeight="1">
-      <c r="B54" s="52"/>
-      <c r="C54" s="51"/>
+    <row r="54" spans="3:15" ht="18" customHeight="1">
+      <c r="C54" s="40"/>
       <c r="D54" s="22"/>
       <c r="E54" s="18"/>
       <c r="F54" s="19"/>
@@ -45834,11 +45572,10 @@
       <c r="L54" s="21"/>
       <c r="M54" s="21"/>
       <c r="N54" s="21"/>
-      <c r="O54" s="64"/>
+      <c r="O54" s="26"/>
     </row>
-    <row r="55" spans="2:15" ht="18" customHeight="1">
-      <c r="B55" s="52"/>
-      <c r="C55" s="50"/>
+    <row r="55" spans="3:15" ht="18" customHeight="1">
+      <c r="C55" s="39"/>
       <c r="D55" s="17"/>
       <c r="E55" s="13"/>
       <c r="F55" s="14"/>
@@ -45850,11 +45587,10 @@
       <c r="L55" s="16"/>
       <c r="M55" s="16"/>
       <c r="N55" s="16"/>
-      <c r="O55" s="63"/>
+      <c r="O55" s="27"/>
     </row>
-    <row r="56" spans="2:15" ht="18" customHeight="1">
-      <c r="B56" s="52"/>
-      <c r="C56" s="51"/>
+    <row r="56" spans="3:15" ht="18" customHeight="1">
+      <c r="C56" s="40"/>
       <c r="D56" s="22"/>
       <c r="E56" s="18"/>
       <c r="F56" s="19"/>
@@ -45866,11 +45602,10 @@
       <c r="L56" s="21"/>
       <c r="M56" s="21"/>
       <c r="N56" s="21"/>
-      <c r="O56" s="64"/>
+      <c r="O56" s="26"/>
     </row>
-    <row r="57" spans="2:15" ht="18" customHeight="1">
-      <c r="B57" s="52"/>
-      <c r="C57" s="50"/>
+    <row r="57" spans="3:15" ht="18" customHeight="1">
+      <c r="C57" s="39"/>
       <c r="D57" s="17"/>
       <c r="E57" s="13"/>
       <c r="F57" s="14"/>
@@ -45882,11 +45617,10 @@
       <c r="L57" s="16"/>
       <c r="M57" s="16"/>
       <c r="N57" s="16"/>
-      <c r="O57" s="63"/>
+      <c r="O57" s="27"/>
     </row>
-    <row r="58" spans="2:15" ht="18" customHeight="1">
-      <c r="B58" s="52"/>
-      <c r="C58" s="51"/>
+    <row r="58" spans="3:15" ht="18" customHeight="1">
+      <c r="C58" s="40"/>
       <c r="D58" s="22"/>
       <c r="E58" s="18"/>
       <c r="F58" s="19"/>
@@ -45898,11 +45632,10 @@
       <c r="L58" s="21"/>
       <c r="M58" s="21"/>
       <c r="N58" s="21"/>
-      <c r="O58" s="64"/>
+      <c r="O58" s="26"/>
     </row>
-    <row r="59" spans="2:15" ht="18" customHeight="1">
-      <c r="B59" s="52"/>
-      <c r="C59" s="50"/>
+    <row r="59" spans="3:15" ht="18" customHeight="1">
+      <c r="C59" s="39"/>
       <c r="D59" s="17"/>
       <c r="E59" s="13"/>
       <c r="F59" s="14"/>
@@ -45914,11 +45647,10 @@
       <c r="L59" s="16"/>
       <c r="M59" s="16"/>
       <c r="N59" s="16"/>
-      <c r="O59" s="63"/>
+      <c r="O59" s="27"/>
     </row>
-    <row r="60" spans="2:15" ht="18" customHeight="1">
-      <c r="B60" s="52"/>
-      <c r="C60" s="51"/>
+    <row r="60" spans="3:15" ht="18" customHeight="1">
+      <c r="C60" s="40"/>
       <c r="D60" s="22"/>
       <c r="E60" s="18"/>
       <c r="F60" s="19"/>
@@ -45930,11 +45662,10 @@
       <c r="L60" s="21"/>
       <c r="M60" s="21"/>
       <c r="N60" s="21"/>
-      <c r="O60" s="64"/>
+      <c r="O60" s="26"/>
     </row>
-    <row r="61" spans="2:15" ht="18" customHeight="1">
-      <c r="B61" s="52"/>
-      <c r="C61" s="50"/>
+    <row r="61" spans="3:15" ht="18" customHeight="1">
+      <c r="C61" s="39"/>
       <c r="D61" s="17"/>
       <c r="E61" s="13"/>
       <c r="F61" s="14"/>
@@ -45946,11 +45677,10 @@
       <c r="L61" s="16"/>
       <c r="M61" s="16"/>
       <c r="N61" s="16"/>
-      <c r="O61" s="63"/>
+      <c r="O61" s="27"/>
     </row>
-    <row r="62" spans="2:15" ht="18" customHeight="1">
-      <c r="B62" s="52"/>
-      <c r="C62" s="51"/>
+    <row r="62" spans="3:15" ht="18" customHeight="1">
+      <c r="C62" s="40"/>
       <c r="D62" s="22"/>
       <c r="E62" s="18"/>
       <c r="F62" s="19"/>
@@ -45962,11 +45692,10 @@
       <c r="L62" s="21"/>
       <c r="M62" s="21"/>
       <c r="N62" s="21"/>
-      <c r="O62" s="64"/>
+      <c r="O62" s="26"/>
     </row>
-    <row r="63" spans="2:15" ht="18" customHeight="1">
-      <c r="B63" s="52"/>
-      <c r="C63" s="50"/>
+    <row r="63" spans="3:15" ht="18" customHeight="1">
+      <c r="C63" s="39"/>
       <c r="D63" s="17"/>
       <c r="E63" s="13"/>
       <c r="F63" s="14"/>
@@ -45978,11 +45707,10 @@
       <c r="L63" s="16"/>
       <c r="M63" s="16"/>
       <c r="N63" s="16"/>
-      <c r="O63" s="63"/>
+      <c r="O63" s="27"/>
     </row>
-    <row r="64" spans="2:15" ht="18" customHeight="1">
-      <c r="B64" s="52"/>
-      <c r="C64" s="51"/>
+    <row r="64" spans="3:15" ht="18" customHeight="1">
+      <c r="C64" s="40"/>
       <c r="D64" s="22"/>
       <c r="E64" s="18"/>
       <c r="F64" s="19"/>
@@ -45994,11 +45722,10 @@
       <c r="L64" s="21"/>
       <c r="M64" s="21"/>
       <c r="N64" s="21"/>
-      <c r="O64" s="64"/>
+      <c r="O64" s="26"/>
     </row>
-    <row r="65" spans="2:15" ht="18" customHeight="1">
-      <c r="B65" s="52"/>
-      <c r="C65" s="50"/>
+    <row r="65" spans="3:15" ht="18" customHeight="1">
+      <c r="C65" s="39"/>
       <c r="D65" s="17"/>
       <c r="E65" s="13"/>
       <c r="F65" s="14"/>
@@ -46010,11 +45737,10 @@
       <c r="L65" s="16"/>
       <c r="M65" s="16"/>
       <c r="N65" s="16"/>
-      <c r="O65" s="63"/>
+      <c r="O65" s="27"/>
     </row>
-    <row r="66" spans="2:15" ht="18" customHeight="1">
-      <c r="B66" s="52"/>
-      <c r="C66" s="51"/>
+    <row r="66" spans="3:15" ht="18" customHeight="1">
+      <c r="C66" s="40"/>
       <c r="D66" s="22"/>
       <c r="E66" s="18"/>
       <c r="F66" s="19"/>
@@ -46026,25 +45752,23 @@
       <c r="L66" s="21"/>
       <c r="M66" s="21"/>
       <c r="N66" s="21"/>
-      <c r="O66" s="64"/>
+      <c r="O66" s="26"/>
     </row>
-    <row r="67" spans="2:15" ht="18" customHeight="1" thickBot="1">
-      <c r="B67" s="52"/>
-      <c r="C67" s="53"/>
-      <c r="D67" s="54"/>
-      <c r="E67" s="55"/>
-      <c r="F67" s="56"/>
-      <c r="G67" s="57"/>
-      <c r="H67" s="58"/>
-      <c r="I67" s="58"/>
-      <c r="J67" s="54"/>
-      <c r="K67" s="55"/>
-      <c r="L67" s="58"/>
-      <c r="M67" s="58"/>
-      <c r="N67" s="58"/>
-      <c r="O67" s="65"/>
+    <row r="67" spans="3:15" ht="18" customHeight="1">
+      <c r="C67" s="39"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="16"/>
+      <c r="I67" s="16"/>
+      <c r="J67" s="17"/>
+      <c r="K67" s="13"/>
+      <c r="L67" s="16"/>
+      <c r="M67" s="16"/>
+      <c r="N67" s="16"/>
+      <c r="O67" s="27"/>
     </row>
-    <row r="68" spans="2:15" ht="12.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="O3:O5"/>
@@ -46059,11 +45783,12 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="64" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="55" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;10日通システム株式会社 &amp;C&amp;"ＭＳ ゴシック,Regular"&amp;16標準報酬月額表（厚生年金）&amp;R&amp;"ＭＳ ゴシック,Regular"&amp;10&amp;KFF0000 &amp;K01+000&amp;D　&amp;T　
 &amp;KFF0000 &amp;K01+000page&amp;P</oddHeader>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -46072,23 +45797,26 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:P68"/>
+  <dimension ref="B1:O67"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0"/>
+    <sheetView view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="2.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" style="32" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="33" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="1" customWidth="1"/>
-    <col min="5" max="14" width="10.7109375" style="1"/>
+    <col min="5" max="6" width="10.7109375" style="1"/>
+    <col min="7" max="14" width="14.42578125" style="1" customWidth="1"/>
     <col min="15" max="15" width="9.28515625" style="1" customWidth="1"/>
     <col min="16" max="16" width="1.28515625" style="1" customWidth="1"/>
     <col min="17" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16">
+    <row r="1" spans="2:15">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -46102,65 +45830,60 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:16" ht="4.9000000000000004" customHeight="1" thickBot="1">
+    <row r="2" spans="2:15" ht="4.9000000000000004" customHeight="1">
       <c r="D2" s="2"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="68"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:16" ht="18" customHeight="1" thickTop="1">
-      <c r="B3" s="52"/>
-      <c r="C3" s="76" t="s">
+    <row r="3" spans="2:15" ht="18" customHeight="1">
+      <c r="C3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="77"/>
-      <c r="E3" s="39" t="s">
+      <c r="D3" s="43"/>
+      <c r="E3" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="40"/>
-      <c r="G3" s="74" t="s">
+      <c r="F3" s="45"/>
+      <c r="G3" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="71" t="s">
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="70" t="s">
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="69"/>
     </row>
-    <row r="4" spans="2:16" ht="18" customHeight="1">
-      <c r="B4" s="52"/>
-      <c r="C4" s="78"/>
+    <row r="4" spans="2:15" ht="18" customHeight="1">
+      <c r="C4" s="34"/>
       <c r="D4" s="23"/>
       <c r="E4" s="24"/>
       <c r="F4" s="25"/>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="46"/>
-      <c r="I4" s="47" t="s">
+      <c r="H4" s="51"/>
+      <c r="I4" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="48"/>
-      <c r="K4" s="45" t="s">
+      <c r="J4" s="53"/>
+      <c r="K4" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="46"/>
-      <c r="M4" s="47" t="s">
+      <c r="L4" s="51"/>
+      <c r="M4" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="48"/>
-      <c r="O4" s="62"/>
-      <c r="P4" s="69"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="41"/>
     </row>
-    <row r="5" spans="2:16" ht="18" customHeight="1" thickBot="1">
-      <c r="B5" s="52"/>
+    <row r="5" spans="2:15" ht="18" customHeight="1" thickBot="1">
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
@@ -46197,29 +45920,25 @@
       <c r="N5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="62"/>
-      <c r="P5" s="69"/>
+      <c r="O5" s="41"/>
     </row>
-    <row r="6" spans="2:16" ht="18" customHeight="1" thickTop="1">
-      <c r="B6" s="52"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="31"/>
+    <row r="6" spans="2:15" ht="18" customHeight="1" thickTop="1">
+      <c r="C6" s="38"/>
+      <c r="D6" s="32"/>
       <c r="E6" s="11"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
       <c r="O6" s="26"/>
-      <c r="P6" s="69"/>
     </row>
-    <row r="7" spans="2:16" ht="18" customHeight="1">
-      <c r="B7" s="52"/>
-      <c r="C7" s="50"/>
+    <row r="7" spans="2:15" ht="18" customHeight="1">
+      <c r="C7" s="39"/>
       <c r="D7" s="17"/>
       <c r="E7" s="13"/>
       <c r="F7" s="14"/>
@@ -46231,11 +45950,10 @@
       <c r="L7" s="16"/>
       <c r="M7" s="16"/>
       <c r="N7" s="16"/>
-      <c r="O7" s="63"/>
+      <c r="O7" s="27"/>
     </row>
-    <row r="8" spans="2:16" ht="18" customHeight="1">
-      <c r="B8" s="52"/>
-      <c r="C8" s="51"/>
+    <row r="8" spans="2:15" ht="18" customHeight="1">
+      <c r="C8" s="40"/>
       <c r="D8" s="22"/>
       <c r="E8" s="18"/>
       <c r="F8" s="19"/>
@@ -46247,11 +45965,10 @@
       <c r="L8" s="21"/>
       <c r="M8" s="21"/>
       <c r="N8" s="21"/>
-      <c r="O8" s="64"/>
+      <c r="O8" s="26"/>
     </row>
-    <row r="9" spans="2:16" ht="18" customHeight="1">
-      <c r="B9" s="52"/>
-      <c r="C9" s="50"/>
+    <row r="9" spans="2:15" ht="18" customHeight="1">
+      <c r="C9" s="39"/>
       <c r="D9" s="17"/>
       <c r="E9" s="13"/>
       <c r="F9" s="14"/>
@@ -46263,11 +45980,10 @@
       <c r="L9" s="16"/>
       <c r="M9" s="16"/>
       <c r="N9" s="16"/>
-      <c r="O9" s="63"/>
+      <c r="O9" s="27"/>
     </row>
-    <row r="10" spans="2:16" ht="18" customHeight="1">
-      <c r="B10" s="52"/>
-      <c r="C10" s="51"/>
+    <row r="10" spans="2:15" ht="18" customHeight="1">
+      <c r="C10" s="40"/>
       <c r="D10" s="22"/>
       <c r="E10" s="18"/>
       <c r="F10" s="19"/>
@@ -46279,11 +45995,10 @@
       <c r="L10" s="21"/>
       <c r="M10" s="21"/>
       <c r="N10" s="21"/>
-      <c r="O10" s="64"/>
+      <c r="O10" s="26"/>
     </row>
-    <row r="11" spans="2:16" ht="18" customHeight="1">
-      <c r="B11" s="52"/>
-      <c r="C11" s="50"/>
+    <row r="11" spans="2:15" ht="18" customHeight="1">
+      <c r="C11" s="39"/>
       <c r="D11" s="17"/>
       <c r="E11" s="13"/>
       <c r="F11" s="14"/>
@@ -46295,11 +46010,10 @@
       <c r="L11" s="16"/>
       <c r="M11" s="16"/>
       <c r="N11" s="16"/>
-      <c r="O11" s="63"/>
+      <c r="O11" s="27"/>
     </row>
-    <row r="12" spans="2:16" ht="18" customHeight="1">
-      <c r="B12" s="52"/>
-      <c r="C12" s="51"/>
+    <row r="12" spans="2:15" ht="18" customHeight="1">
+      <c r="C12" s="40"/>
       <c r="D12" s="22"/>
       <c r="E12" s="18"/>
       <c r="F12" s="19"/>
@@ -46311,11 +46025,10 @@
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
       <c r="N12" s="21"/>
-      <c r="O12" s="64"/>
+      <c r="O12" s="26"/>
     </row>
-    <row r="13" spans="2:16" ht="18" customHeight="1">
-      <c r="B13" s="52"/>
-      <c r="C13" s="50"/>
+    <row r="13" spans="2:15" ht="18" customHeight="1">
+      <c r="C13" s="39"/>
       <c r="D13" s="17"/>
       <c r="E13" s="13"/>
       <c r="F13" s="14"/>
@@ -46327,11 +46040,10 @@
       <c r="L13" s="16"/>
       <c r="M13" s="16"/>
       <c r="N13" s="16"/>
-      <c r="O13" s="63"/>
+      <c r="O13" s="27"/>
     </row>
-    <row r="14" spans="2:16" ht="18" customHeight="1">
-      <c r="B14" s="52"/>
-      <c r="C14" s="51"/>
+    <row r="14" spans="2:15" ht="18" customHeight="1">
+      <c r="C14" s="40"/>
       <c r="D14" s="22"/>
       <c r="E14" s="18"/>
       <c r="F14" s="19"/>
@@ -46343,11 +46055,10 @@
       <c r="L14" s="21"/>
       <c r="M14" s="21"/>
       <c r="N14" s="21"/>
-      <c r="O14" s="64"/>
+      <c r="O14" s="26"/>
     </row>
-    <row r="15" spans="2:16" ht="18" customHeight="1">
-      <c r="B15" s="52"/>
-      <c r="C15" s="50"/>
+    <row r="15" spans="2:15" ht="18" customHeight="1">
+      <c r="C15" s="39"/>
       <c r="D15" s="17"/>
       <c r="E15" s="13"/>
       <c r="F15" s="14"/>
@@ -46359,11 +46070,10 @@
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
       <c r="N15" s="16"/>
-      <c r="O15" s="63"/>
+      <c r="O15" s="27"/>
     </row>
-    <row r="16" spans="2:16" ht="18" customHeight="1">
-      <c r="B16" s="52"/>
-      <c r="C16" s="51"/>
+    <row r="16" spans="2:15" ht="18" customHeight="1">
+      <c r="C16" s="40"/>
       <c r="D16" s="22"/>
       <c r="E16" s="18"/>
       <c r="F16" s="19"/>
@@ -46375,11 +46085,10 @@
       <c r="L16" s="21"/>
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>
-      <c r="O16" s="64"/>
+      <c r="O16" s="26"/>
     </row>
-    <row r="17" spans="2:15" ht="18" customHeight="1">
-      <c r="B17" s="52"/>
-      <c r="C17" s="50"/>
+    <row r="17" spans="3:15" ht="18" customHeight="1">
+      <c r="C17" s="39"/>
       <c r="D17" s="17"/>
       <c r="E17" s="13"/>
       <c r="F17" s="14"/>
@@ -46391,11 +46100,10 @@
       <c r="L17" s="16"/>
       <c r="M17" s="16"/>
       <c r="N17" s="16"/>
-      <c r="O17" s="63"/>
+      <c r="O17" s="27"/>
     </row>
-    <row r="18" spans="2:15" ht="18" customHeight="1">
-      <c r="B18" s="52"/>
-      <c r="C18" s="51"/>
+    <row r="18" spans="3:15" ht="18" customHeight="1">
+      <c r="C18" s="40"/>
       <c r="D18" s="22"/>
       <c r="E18" s="18"/>
       <c r="F18" s="19"/>
@@ -46407,11 +46115,10 @@
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
       <c r="N18" s="21"/>
-      <c r="O18" s="64"/>
+      <c r="O18" s="26"/>
     </row>
-    <row r="19" spans="2:15" ht="18" customHeight="1">
-      <c r="B19" s="52"/>
-      <c r="C19" s="50"/>
+    <row r="19" spans="3:15" ht="18" customHeight="1">
+      <c r="C19" s="39"/>
       <c r="D19" s="17"/>
       <c r="E19" s="13"/>
       <c r="F19" s="14"/>
@@ -46423,11 +46130,10 @@
       <c r="L19" s="16"/>
       <c r="M19" s="16"/>
       <c r="N19" s="16"/>
-      <c r="O19" s="63"/>
+      <c r="O19" s="27"/>
     </row>
-    <row r="20" spans="2:15" ht="18" customHeight="1">
-      <c r="B20" s="52"/>
-      <c r="C20" s="51"/>
+    <row r="20" spans="3:15" ht="18" customHeight="1">
+      <c r="C20" s="40"/>
       <c r="D20" s="22"/>
       <c r="E20" s="18"/>
       <c r="F20" s="19"/>
@@ -46439,11 +46145,10 @@
       <c r="L20" s="21"/>
       <c r="M20" s="21"/>
       <c r="N20" s="21"/>
-      <c r="O20" s="64"/>
+      <c r="O20" s="26"/>
     </row>
-    <row r="21" spans="2:15" ht="18" customHeight="1">
-      <c r="B21" s="52"/>
-      <c r="C21" s="50"/>
+    <row r="21" spans="3:15" ht="18" customHeight="1">
+      <c r="C21" s="39"/>
       <c r="D21" s="17"/>
       <c r="E21" s="13"/>
       <c r="F21" s="14"/>
@@ -46455,11 +46160,10 @@
       <c r="L21" s="16"/>
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
-      <c r="O21" s="63"/>
+      <c r="O21" s="27"/>
     </row>
-    <row r="22" spans="2:15" ht="18" customHeight="1">
-      <c r="B22" s="52"/>
-      <c r="C22" s="51"/>
+    <row r="22" spans="3:15" ht="18" customHeight="1">
+      <c r="C22" s="40"/>
       <c r="D22" s="22"/>
       <c r="E22" s="18"/>
       <c r="F22" s="19"/>
@@ -46471,11 +46175,10 @@
       <c r="L22" s="21"/>
       <c r="M22" s="21"/>
       <c r="N22" s="21"/>
-      <c r="O22" s="64"/>
+      <c r="O22" s="26"/>
     </row>
-    <row r="23" spans="2:15" ht="18" customHeight="1">
-      <c r="B23" s="52"/>
-      <c r="C23" s="50"/>
+    <row r="23" spans="3:15" ht="18" customHeight="1">
+      <c r="C23" s="39"/>
       <c r="D23" s="17"/>
       <c r="E23" s="13"/>
       <c r="F23" s="14"/>
@@ -46487,11 +46190,10 @@
       <c r="L23" s="16"/>
       <c r="M23" s="16"/>
       <c r="N23" s="16"/>
-      <c r="O23" s="63"/>
+      <c r="O23" s="27"/>
     </row>
-    <row r="24" spans="2:15" ht="18" customHeight="1">
-      <c r="B24" s="52"/>
-      <c r="C24" s="51"/>
+    <row r="24" spans="3:15" ht="18" customHeight="1">
+      <c r="C24" s="40"/>
       <c r="D24" s="22"/>
       <c r="E24" s="18"/>
       <c r="F24" s="19"/>
@@ -46503,11 +46205,10 @@
       <c r="L24" s="21"/>
       <c r="M24" s="21"/>
       <c r="N24" s="21"/>
-      <c r="O24" s="64"/>
+      <c r="O24" s="26"/>
     </row>
-    <row r="25" spans="2:15" ht="18" customHeight="1">
-      <c r="B25" s="52"/>
-      <c r="C25" s="50"/>
+    <row r="25" spans="3:15" ht="18" customHeight="1">
+      <c r="C25" s="39"/>
       <c r="D25" s="17"/>
       <c r="E25" s="13"/>
       <c r="F25" s="14"/>
@@ -46519,11 +46220,10 @@
       <c r="L25" s="16"/>
       <c r="M25" s="16"/>
       <c r="N25" s="16"/>
-      <c r="O25" s="63"/>
+      <c r="O25" s="27"/>
     </row>
-    <row r="26" spans="2:15" ht="18" customHeight="1">
-      <c r="B26" s="52"/>
-      <c r="C26" s="51"/>
+    <row r="26" spans="3:15" ht="18" customHeight="1">
+      <c r="C26" s="40"/>
       <c r="D26" s="22"/>
       <c r="E26" s="18"/>
       <c r="F26" s="19"/>
@@ -46535,11 +46235,10 @@
       <c r="L26" s="21"/>
       <c r="M26" s="21"/>
       <c r="N26" s="21"/>
-      <c r="O26" s="64"/>
+      <c r="O26" s="26"/>
     </row>
-    <row r="27" spans="2:15" ht="18" customHeight="1">
-      <c r="B27" s="52"/>
-      <c r="C27" s="50"/>
+    <row r="27" spans="3:15" ht="18" customHeight="1">
+      <c r="C27" s="39"/>
       <c r="D27" s="17"/>
       <c r="E27" s="13"/>
       <c r="F27" s="14"/>
@@ -46551,11 +46250,10 @@
       <c r="L27" s="16"/>
       <c r="M27" s="16"/>
       <c r="N27" s="16"/>
-      <c r="O27" s="63"/>
+      <c r="O27" s="27"/>
     </row>
-    <row r="28" spans="2:15" ht="18" customHeight="1">
-      <c r="B28" s="52"/>
-      <c r="C28" s="51"/>
+    <row r="28" spans="3:15" ht="18" customHeight="1">
+      <c r="C28" s="40"/>
       <c r="D28" s="22"/>
       <c r="E28" s="18"/>
       <c r="F28" s="19"/>
@@ -46567,11 +46265,10 @@
       <c r="L28" s="21"/>
       <c r="M28" s="21"/>
       <c r="N28" s="21"/>
-      <c r="O28" s="64"/>
+      <c r="O28" s="26"/>
     </row>
-    <row r="29" spans="2:15" ht="18" customHeight="1">
-      <c r="B29" s="52"/>
-      <c r="C29" s="50"/>
+    <row r="29" spans="3:15" ht="18" customHeight="1">
+      <c r="C29" s="39"/>
       <c r="D29" s="17"/>
       <c r="E29" s="13"/>
       <c r="F29" s="14"/>
@@ -46583,11 +46280,10 @@
       <c r="L29" s="16"/>
       <c r="M29" s="16"/>
       <c r="N29" s="16"/>
-      <c r="O29" s="63"/>
+      <c r="O29" s="27"/>
     </row>
-    <row r="30" spans="2:15" ht="18" customHeight="1">
-      <c r="B30" s="52"/>
-      <c r="C30" s="51"/>
+    <row r="30" spans="3:15" ht="18" customHeight="1">
+      <c r="C30" s="40"/>
       <c r="D30" s="22"/>
       <c r="E30" s="18"/>
       <c r="F30" s="19"/>
@@ -46599,11 +46295,10 @@
       <c r="L30" s="21"/>
       <c r="M30" s="21"/>
       <c r="N30" s="21"/>
-      <c r="O30" s="64"/>
+      <c r="O30" s="26"/>
     </row>
-    <row r="31" spans="2:15" ht="18" customHeight="1">
-      <c r="B31" s="52"/>
-      <c r="C31" s="50"/>
+    <row r="31" spans="3:15" ht="18" customHeight="1">
+      <c r="C31" s="39"/>
       <c r="D31" s="17"/>
       <c r="E31" s="13"/>
       <c r="F31" s="14"/>
@@ -46615,11 +46310,10 @@
       <c r="L31" s="16"/>
       <c r="M31" s="16"/>
       <c r="N31" s="16"/>
-      <c r="O31" s="63"/>
+      <c r="O31" s="27"/>
     </row>
-    <row r="32" spans="2:15" ht="18" customHeight="1">
-      <c r="B32" s="52"/>
-      <c r="C32" s="51"/>
+    <row r="32" spans="3:15" ht="18" customHeight="1">
+      <c r="C32" s="40"/>
       <c r="D32" s="22"/>
       <c r="E32" s="18"/>
       <c r="F32" s="19"/>
@@ -46631,11 +46325,10 @@
       <c r="L32" s="21"/>
       <c r="M32" s="21"/>
       <c r="N32" s="21"/>
-      <c r="O32" s="64"/>
+      <c r="O32" s="26"/>
     </row>
-    <row r="33" spans="2:15" ht="18" customHeight="1">
-      <c r="B33" s="52"/>
-      <c r="C33" s="50"/>
+    <row r="33" spans="3:15" ht="18" customHeight="1">
+      <c r="C33" s="39"/>
       <c r="D33" s="17"/>
       <c r="E33" s="13"/>
       <c r="F33" s="14"/>
@@ -46647,11 +46340,10 @@
       <c r="L33" s="16"/>
       <c r="M33" s="16"/>
       <c r="N33" s="16"/>
-      <c r="O33" s="63"/>
+      <c r="O33" s="27"/>
     </row>
-    <row r="34" spans="2:15" ht="18" customHeight="1">
-      <c r="B34" s="52"/>
-      <c r="C34" s="51"/>
+    <row r="34" spans="3:15" ht="18" customHeight="1">
+      <c r="C34" s="40"/>
       <c r="D34" s="22"/>
       <c r="E34" s="18"/>
       <c r="F34" s="19"/>
@@ -46663,11 +46355,10 @@
       <c r="L34" s="21"/>
       <c r="M34" s="21"/>
       <c r="N34" s="21"/>
-      <c r="O34" s="64"/>
+      <c r="O34" s="26"/>
     </row>
-    <row r="35" spans="2:15" ht="18" customHeight="1">
-      <c r="B35" s="52"/>
-      <c r="C35" s="50"/>
+    <row r="35" spans="3:15" ht="18" customHeight="1">
+      <c r="C35" s="39"/>
       <c r="D35" s="17"/>
       <c r="E35" s="13"/>
       <c r="F35" s="14"/>
@@ -46679,11 +46370,10 @@
       <c r="L35" s="16"/>
       <c r="M35" s="16"/>
       <c r="N35" s="16"/>
-      <c r="O35" s="63"/>
+      <c r="O35" s="27"/>
     </row>
-    <row r="36" spans="2:15" ht="18" customHeight="1">
-      <c r="B36" s="52"/>
-      <c r="C36" s="51"/>
+    <row r="36" spans="3:15" ht="18" customHeight="1">
+      <c r="C36" s="40"/>
       <c r="D36" s="22"/>
       <c r="E36" s="18"/>
       <c r="F36" s="19"/>
@@ -46695,11 +46385,10 @@
       <c r="L36" s="21"/>
       <c r="M36" s="21"/>
       <c r="N36" s="21"/>
-      <c r="O36" s="64"/>
+      <c r="O36" s="26"/>
     </row>
-    <row r="37" spans="2:15" ht="18" customHeight="1">
-      <c r="B37" s="52"/>
-      <c r="C37" s="50"/>
+    <row r="37" spans="3:15" ht="18" customHeight="1">
+      <c r="C37" s="39"/>
       <c r="D37" s="17"/>
       <c r="E37" s="13"/>
       <c r="F37" s="14"/>
@@ -46711,27 +46400,25 @@
       <c r="L37" s="16"/>
       <c r="M37" s="16"/>
       <c r="N37" s="16"/>
-      <c r="O37" s="63"/>
+      <c r="O37" s="27"/>
     </row>
-    <row r="38" spans="2:15" ht="18" customHeight="1">
-      <c r="B38" s="52"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="28"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="36"/>
-      <c r="L38" s="28"/>
-      <c r="M38" s="28"/>
-      <c r="N38" s="28"/>
-      <c r="O38" s="64"/>
+    <row r="38" spans="3:15" ht="18" customHeight="1">
+      <c r="C38" s="38"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="30"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="26"/>
     </row>
-    <row r="39" spans="2:15" ht="18" customHeight="1">
-      <c r="B39" s="52"/>
-      <c r="C39" s="50"/>
+    <row r="39" spans="3:15" ht="18" customHeight="1">
+      <c r="C39" s="39"/>
       <c r="D39" s="17"/>
       <c r="E39" s="13"/>
       <c r="F39" s="14"/>
@@ -46743,11 +46430,10 @@
       <c r="L39" s="16"/>
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
-      <c r="O39" s="63"/>
+      <c r="O39" s="27"/>
     </row>
-    <row r="40" spans="2:15" ht="18" customHeight="1">
-      <c r="B40" s="52"/>
-      <c r="C40" s="51"/>
+    <row r="40" spans="3:15" ht="18" customHeight="1">
+      <c r="C40" s="40"/>
       <c r="D40" s="22"/>
       <c r="E40" s="18"/>
       <c r="F40" s="19"/>
@@ -46759,11 +46445,10 @@
       <c r="L40" s="21"/>
       <c r="M40" s="21"/>
       <c r="N40" s="21"/>
-      <c r="O40" s="64"/>
+      <c r="O40" s="26"/>
     </row>
-    <row r="41" spans="2:15" ht="18" customHeight="1">
-      <c r="B41" s="52"/>
-      <c r="C41" s="50"/>
+    <row r="41" spans="3:15" ht="18" customHeight="1">
+      <c r="C41" s="39"/>
       <c r="D41" s="17"/>
       <c r="E41" s="13"/>
       <c r="F41" s="14"/>
@@ -46775,11 +46460,10 @@
       <c r="L41" s="16"/>
       <c r="M41" s="16"/>
       <c r="N41" s="16"/>
-      <c r="O41" s="63"/>
+      <c r="O41" s="27"/>
     </row>
-    <row r="42" spans="2:15" ht="18" customHeight="1">
-      <c r="B42" s="52"/>
-      <c r="C42" s="51"/>
+    <row r="42" spans="3:15" ht="18" customHeight="1">
+      <c r="C42" s="40"/>
       <c r="D42" s="22"/>
       <c r="E42" s="18"/>
       <c r="F42" s="19"/>
@@ -46791,11 +46475,10 @@
       <c r="L42" s="21"/>
       <c r="M42" s="21"/>
       <c r="N42" s="21"/>
-      <c r="O42" s="64"/>
+      <c r="O42" s="26"/>
     </row>
-    <row r="43" spans="2:15" ht="18" customHeight="1">
-      <c r="B43" s="52"/>
-      <c r="C43" s="50"/>
+    <row r="43" spans="3:15" ht="18" customHeight="1">
+      <c r="C43" s="39"/>
       <c r="D43" s="17"/>
       <c r="E43" s="13"/>
       <c r="F43" s="14"/>
@@ -46807,11 +46490,10 @@
       <c r="L43" s="16"/>
       <c r="M43" s="16"/>
       <c r="N43" s="16"/>
-      <c r="O43" s="63"/>
+      <c r="O43" s="27"/>
     </row>
-    <row r="44" spans="2:15" ht="18" customHeight="1">
-      <c r="B44" s="52"/>
-      <c r="C44" s="51"/>
+    <row r="44" spans="3:15" ht="18" customHeight="1">
+      <c r="C44" s="40"/>
       <c r="D44" s="22"/>
       <c r="E44" s="18"/>
       <c r="F44" s="19"/>
@@ -46823,11 +46505,10 @@
       <c r="L44" s="21"/>
       <c r="M44" s="21"/>
       <c r="N44" s="21"/>
-      <c r="O44" s="64"/>
+      <c r="O44" s="26"/>
     </row>
-    <row r="45" spans="2:15" ht="18" customHeight="1">
-      <c r="B45" s="52"/>
-      <c r="C45" s="50"/>
+    <row r="45" spans="3:15" ht="18" customHeight="1">
+      <c r="C45" s="39"/>
       <c r="D45" s="17"/>
       <c r="E45" s="13"/>
       <c r="F45" s="14"/>
@@ -46839,11 +46520,10 @@
       <c r="L45" s="16"/>
       <c r="M45" s="16"/>
       <c r="N45" s="16"/>
-      <c r="O45" s="63"/>
+      <c r="O45" s="27"/>
     </row>
-    <row r="46" spans="2:15" ht="18" customHeight="1">
-      <c r="B46" s="52"/>
-      <c r="C46" s="51"/>
+    <row r="46" spans="3:15" ht="18" customHeight="1">
+      <c r="C46" s="40"/>
       <c r="D46" s="22"/>
       <c r="E46" s="18"/>
       <c r="F46" s="19"/>
@@ -46855,11 +46535,10 @@
       <c r="L46" s="21"/>
       <c r="M46" s="21"/>
       <c r="N46" s="21"/>
-      <c r="O46" s="64"/>
+      <c r="O46" s="26"/>
     </row>
-    <row r="47" spans="2:15" ht="18" customHeight="1">
-      <c r="B47" s="52"/>
-      <c r="C47" s="50"/>
+    <row r="47" spans="3:15" ht="18" customHeight="1">
+      <c r="C47" s="39"/>
       <c r="D47" s="17"/>
       <c r="E47" s="13"/>
       <c r="F47" s="14"/>
@@ -46871,11 +46550,10 @@
       <c r="L47" s="16"/>
       <c r="M47" s="16"/>
       <c r="N47" s="16"/>
-      <c r="O47" s="63"/>
+      <c r="O47" s="27"/>
     </row>
-    <row r="48" spans="2:15" ht="18" customHeight="1">
-      <c r="B48" s="52"/>
-      <c r="C48" s="51"/>
+    <row r="48" spans="3:15" ht="18" customHeight="1">
+      <c r="C48" s="40"/>
       <c r="D48" s="22"/>
       <c r="E48" s="18"/>
       <c r="F48" s="19"/>
@@ -46887,11 +46565,10 @@
       <c r="L48" s="21"/>
       <c r="M48" s="21"/>
       <c r="N48" s="21"/>
-      <c r="O48" s="64"/>
+      <c r="O48" s="26"/>
     </row>
-    <row r="49" spans="2:15" ht="18" customHeight="1">
-      <c r="B49" s="52"/>
-      <c r="C49" s="50"/>
+    <row r="49" spans="3:15" ht="18" customHeight="1">
+      <c r="C49" s="39"/>
       <c r="D49" s="17"/>
       <c r="E49" s="13"/>
       <c r="F49" s="14"/>
@@ -46903,11 +46580,10 @@
       <c r="L49" s="16"/>
       <c r="M49" s="16"/>
       <c r="N49" s="16"/>
-      <c r="O49" s="63"/>
+      <c r="O49" s="27"/>
     </row>
-    <row r="50" spans="2:15" ht="18" customHeight="1">
-      <c r="B50" s="52"/>
-      <c r="C50" s="51"/>
+    <row r="50" spans="3:15" ht="18" customHeight="1">
+      <c r="C50" s="40"/>
       <c r="D50" s="22"/>
       <c r="E50" s="18"/>
       <c r="F50" s="19"/>
@@ -46919,11 +46595,10 @@
       <c r="L50" s="21"/>
       <c r="M50" s="21"/>
       <c r="N50" s="21"/>
-      <c r="O50" s="64"/>
+      <c r="O50" s="26"/>
     </row>
-    <row r="51" spans="2:15" ht="18" customHeight="1">
-      <c r="B51" s="52"/>
-      <c r="C51" s="50"/>
+    <row r="51" spans="3:15" ht="18" customHeight="1">
+      <c r="C51" s="39"/>
       <c r="D51" s="17"/>
       <c r="E51" s="13"/>
       <c r="F51" s="14"/>
@@ -46935,11 +46610,10 @@
       <c r="L51" s="16"/>
       <c r="M51" s="16"/>
       <c r="N51" s="16"/>
-      <c r="O51" s="63"/>
+      <c r="O51" s="27"/>
     </row>
-    <row r="52" spans="2:15" ht="18" customHeight="1">
-      <c r="B52" s="52"/>
-      <c r="C52" s="51"/>
+    <row r="52" spans="3:15" ht="18" customHeight="1">
+      <c r="C52" s="40"/>
       <c r="D52" s="22"/>
       <c r="E52" s="18"/>
       <c r="F52" s="19"/>
@@ -46951,11 +46625,10 @@
       <c r="L52" s="21"/>
       <c r="M52" s="21"/>
       <c r="N52" s="21"/>
-      <c r="O52" s="64"/>
+      <c r="O52" s="26"/>
     </row>
-    <row r="53" spans="2:15" ht="18" customHeight="1">
-      <c r="B53" s="52"/>
-      <c r="C53" s="50"/>
+    <row r="53" spans="3:15" ht="18" customHeight="1">
+      <c r="C53" s="39"/>
       <c r="D53" s="17"/>
       <c r="E53" s="13"/>
       <c r="F53" s="14"/>
@@ -46967,11 +46640,10 @@
       <c r="L53" s="16"/>
       <c r="M53" s="16"/>
       <c r="N53" s="16"/>
-      <c r="O53" s="63"/>
+      <c r="O53" s="27"/>
     </row>
-    <row r="54" spans="2:15" ht="18" customHeight="1">
-      <c r="B54" s="52"/>
-      <c r="C54" s="51"/>
+    <row r="54" spans="3:15" ht="18" customHeight="1">
+      <c r="C54" s="40"/>
       <c r="D54" s="22"/>
       <c r="E54" s="18"/>
       <c r="F54" s="19"/>
@@ -46983,11 +46655,10 @@
       <c r="L54" s="21"/>
       <c r="M54" s="21"/>
       <c r="N54" s="21"/>
-      <c r="O54" s="64"/>
+      <c r="O54" s="26"/>
     </row>
-    <row r="55" spans="2:15" ht="18" customHeight="1">
-      <c r="B55" s="52"/>
-      <c r="C55" s="50"/>
+    <row r="55" spans="3:15" ht="18" customHeight="1">
+      <c r="C55" s="39"/>
       <c r="D55" s="17"/>
       <c r="E55" s="13"/>
       <c r="F55" s="14"/>
@@ -46999,11 +46670,10 @@
       <c r="L55" s="16"/>
       <c r="M55" s="16"/>
       <c r="N55" s="16"/>
-      <c r="O55" s="63"/>
+      <c r="O55" s="27"/>
     </row>
-    <row r="56" spans="2:15" ht="18" customHeight="1">
-      <c r="B56" s="52"/>
-      <c r="C56" s="51"/>
+    <row r="56" spans="3:15" ht="18" customHeight="1">
+      <c r="C56" s="40"/>
       <c r="D56" s="22"/>
       <c r="E56" s="18"/>
       <c r="F56" s="19"/>
@@ -47015,11 +46685,10 @@
       <c r="L56" s="21"/>
       <c r="M56" s="21"/>
       <c r="N56" s="21"/>
-      <c r="O56" s="64"/>
+      <c r="O56" s="26"/>
     </row>
-    <row r="57" spans="2:15" ht="18" customHeight="1">
-      <c r="B57" s="52"/>
-      <c r="C57" s="50"/>
+    <row r="57" spans="3:15" ht="18" customHeight="1">
+      <c r="C57" s="39"/>
       <c r="D57" s="17"/>
       <c r="E57" s="13"/>
       <c r="F57" s="14"/>
@@ -47031,11 +46700,10 @@
       <c r="L57" s="16"/>
       <c r="M57" s="16"/>
       <c r="N57" s="16"/>
-      <c r="O57" s="63"/>
+      <c r="O57" s="27"/>
     </row>
-    <row r="58" spans="2:15" ht="18" customHeight="1">
-      <c r="B58" s="52"/>
-      <c r="C58" s="51"/>
+    <row r="58" spans="3:15" ht="18" customHeight="1">
+      <c r="C58" s="40"/>
       <c r="D58" s="22"/>
       <c r="E58" s="18"/>
       <c r="F58" s="19"/>
@@ -47047,11 +46715,10 @@
       <c r="L58" s="21"/>
       <c r="M58" s="21"/>
       <c r="N58" s="21"/>
-      <c r="O58" s="64"/>
+      <c r="O58" s="26"/>
     </row>
-    <row r="59" spans="2:15" ht="18" customHeight="1">
-      <c r="B59" s="52"/>
-      <c r="C59" s="50"/>
+    <row r="59" spans="3:15" ht="18" customHeight="1">
+      <c r="C59" s="39"/>
       <c r="D59" s="17"/>
       <c r="E59" s="13"/>
       <c r="F59" s="14"/>
@@ -47063,11 +46730,10 @@
       <c r="L59" s="16"/>
       <c r="M59" s="16"/>
       <c r="N59" s="16"/>
-      <c r="O59" s="63"/>
+      <c r="O59" s="27"/>
     </row>
-    <row r="60" spans="2:15" ht="18" customHeight="1">
-      <c r="B60" s="52"/>
-      <c r="C60" s="51"/>
+    <row r="60" spans="3:15" ht="18" customHeight="1">
+      <c r="C60" s="40"/>
       <c r="D60" s="22"/>
       <c r="E60" s="18"/>
       <c r="F60" s="19"/>
@@ -47079,11 +46745,10 @@
       <c r="L60" s="21"/>
       <c r="M60" s="21"/>
       <c r="N60" s="21"/>
-      <c r="O60" s="64"/>
+      <c r="O60" s="26"/>
     </row>
-    <row r="61" spans="2:15" ht="18" customHeight="1">
-      <c r="B61" s="52"/>
-      <c r="C61" s="50"/>
+    <row r="61" spans="3:15" ht="18" customHeight="1">
+      <c r="C61" s="39"/>
       <c r="D61" s="17"/>
       <c r="E61" s="13"/>
       <c r="F61" s="14"/>
@@ -47095,11 +46760,10 @@
       <c r="L61" s="16"/>
       <c r="M61" s="16"/>
       <c r="N61" s="16"/>
-      <c r="O61" s="63"/>
+      <c r="O61" s="27"/>
     </row>
-    <row r="62" spans="2:15" ht="18" customHeight="1">
-      <c r="B62" s="52"/>
-      <c r="C62" s="51"/>
+    <row r="62" spans="3:15" ht="18" customHeight="1">
+      <c r="C62" s="40"/>
       <c r="D62" s="22"/>
       <c r="E62" s="18"/>
       <c r="F62" s="19"/>
@@ -47111,11 +46775,10 @@
       <c r="L62" s="21"/>
       <c r="M62" s="21"/>
       <c r="N62" s="21"/>
-      <c r="O62" s="64"/>
+      <c r="O62" s="26"/>
     </row>
-    <row r="63" spans="2:15" ht="18" customHeight="1">
-      <c r="B63" s="52"/>
-      <c r="C63" s="50"/>
+    <row r="63" spans="3:15" ht="18" customHeight="1">
+      <c r="C63" s="39"/>
       <c r="D63" s="17"/>
       <c r="E63" s="13"/>
       <c r="F63" s="14"/>
@@ -47127,11 +46790,10 @@
       <c r="L63" s="16"/>
       <c r="M63" s="16"/>
       <c r="N63" s="16"/>
-      <c r="O63" s="63"/>
+      <c r="O63" s="27"/>
     </row>
-    <row r="64" spans="2:15" ht="18" customHeight="1">
-      <c r="B64" s="52"/>
-      <c r="C64" s="51"/>
+    <row r="64" spans="3:15" ht="18" customHeight="1">
+      <c r="C64" s="40"/>
       <c r="D64" s="22"/>
       <c r="E64" s="18"/>
       <c r="F64" s="19"/>
@@ -47143,11 +46805,10 @@
       <c r="L64" s="21"/>
       <c r="M64" s="21"/>
       <c r="N64" s="21"/>
-      <c r="O64" s="64"/>
+      <c r="O64" s="26"/>
     </row>
-    <row r="65" spans="2:15" ht="18" customHeight="1">
-      <c r="B65" s="52"/>
-      <c r="C65" s="50"/>
+    <row r="65" spans="3:15" ht="18" customHeight="1">
+      <c r="C65" s="39"/>
       <c r="D65" s="17"/>
       <c r="E65" s="13"/>
       <c r="F65" s="14"/>
@@ -47159,11 +46820,10 @@
       <c r="L65" s="16"/>
       <c r="M65" s="16"/>
       <c r="N65" s="16"/>
-      <c r="O65" s="63"/>
+      <c r="O65" s="27"/>
     </row>
-    <row r="66" spans="2:15" ht="18" customHeight="1">
-      <c r="B66" s="52"/>
-      <c r="C66" s="51"/>
+    <row r="66" spans="3:15" ht="18" customHeight="1">
+      <c r="C66" s="40"/>
       <c r="D66" s="22"/>
       <c r="E66" s="18"/>
       <c r="F66" s="19"/>
@@ -47175,25 +46835,23 @@
       <c r="L66" s="21"/>
       <c r="M66" s="21"/>
       <c r="N66" s="21"/>
-      <c r="O66" s="64"/>
+      <c r="O66" s="26"/>
     </row>
-    <row r="67" spans="2:15" ht="18" customHeight="1" thickBot="1">
-      <c r="B67" s="52"/>
-      <c r="C67" s="53"/>
-      <c r="D67" s="54"/>
-      <c r="E67" s="55"/>
-      <c r="F67" s="56"/>
-      <c r="G67" s="57"/>
-      <c r="H67" s="58"/>
-      <c r="I67" s="58"/>
-      <c r="J67" s="54"/>
-      <c r="K67" s="55"/>
-      <c r="L67" s="58"/>
-      <c r="M67" s="58"/>
-      <c r="N67" s="58"/>
-      <c r="O67" s="65"/>
+    <row r="67" spans="3:15" ht="18" customHeight="1">
+      <c r="C67" s="39"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="16"/>
+      <c r="I67" s="16"/>
+      <c r="J67" s="17"/>
+      <c r="K67" s="13"/>
+      <c r="L67" s="16"/>
+      <c r="M67" s="16"/>
+      <c r="N67" s="16"/>
+      <c r="O67" s="27"/>
     </row>
-    <row r="68" spans="2:15" ht="12.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="C3:D3"/>
@@ -47207,10 +46865,11 @@
     <mergeCell ref="M4:N4"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="64" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="55" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;10日通システム株式会社 &amp;C&amp;"ＭＳ ゴシック,Regular"&amp;16標準報酬月額表（厚生年金）&amp;R&amp;"ＭＳ ゴシック,Regular"&amp;10&amp;KFF0000 &amp;K01+000&amp;D　&amp;T　
 &amp;KFF0000 &amp;K01+000page&amp;P</oddHeader>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[SMAL] QMM008F update template
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_標準報酬月額表（厚生年金).xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_標準報酬月額表（厚生年金).xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="マスタリスト" sheetId="11" r:id="rId1"/>
-    <sheet name="マスタリスト (2)" sheetId="14" r:id="rId2"/>
+    <sheet name="マスタリスト (2)" sheetId="15" r:id="rId2"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
@@ -409,7 +409,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -816,6 +816,134 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="6"/>
+      </left>
+      <right style="thin">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right style="thick">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right style="thin">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -827,7 +955,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -904,12 +1032,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="4" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="40" fontId="4" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -940,17 +1062,17 @@
     <xf numFmtId="40" fontId="4" fillId="0" borderId="30" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -988,6 +1110,54 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="33" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="32" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="3" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="3" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="3" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="3" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="3" borderId="38" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="3" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="3" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="3" borderId="41" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
@@ -1011,144 +1181,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>173212</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>5281</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>17518</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="角丸四角形 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="285271" y="218193"/>
-          <a:ext cx="9705482" cy="14562366"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 0"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="accent3">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>173212</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>5281</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>17518</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="角丸四角形 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="277987" y="214831"/>
-          <a:ext cx="11569581" cy="14853719"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 0"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="accent3">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -44714,17 +44746,15 @@
   <sheetPr codeName="Sheet7">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:O67"/>
+  <dimension ref="B1:O68"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="2.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" style="33" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="31" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="1" customWidth="1"/>
     <col min="5" max="6" width="10.7109375" style="1"/>
     <col min="7" max="14" width="14.42578125" style="1" customWidth="1"/>
@@ -44747,60 +44777,73 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:15" ht="4.9000000000000004" customHeight="1">
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
+    <row r="2" spans="2:15" ht="4.9000000000000004" customHeight="1" thickBot="1">
+      <c r="C2" s="52"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
     </row>
-    <row r="3" spans="2:15" ht="18" customHeight="1">
-      <c r="C3" s="42" t="s">
+    <row r="3" spans="2:15" ht="18" customHeight="1" thickTop="1">
+      <c r="B3" s="39"/>
+      <c r="C3" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="44" t="s">
+      <c r="D3" s="41"/>
+      <c r="E3" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="45"/>
-      <c r="G3" s="46" t="s">
+      <c r="F3" s="43"/>
+      <c r="G3" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="46" t="s">
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="41" t="s">
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="58" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:15" ht="18" customHeight="1">
-      <c r="C4" s="34"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="23"/>
       <c r="E4" s="24"/>
       <c r="F4" s="25"/>
-      <c r="G4" s="50" t="s">
+      <c r="G4" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="51"/>
-      <c r="I4" s="52" t="s">
+      <c r="H4" s="49"/>
+      <c r="I4" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="53"/>
-      <c r="K4" s="50" t="s">
+      <c r="J4" s="51"/>
+      <c r="K4" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="51"/>
-      <c r="M4" s="52" t="s">
+      <c r="L4" s="49"/>
+      <c r="M4" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="53"/>
-      <c r="O4" s="41"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="58"/>
     </row>
     <row r="5" spans="2:15" ht="18" customHeight="1" thickBot="1">
+      <c r="B5" s="39"/>
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
@@ -44837,25 +44880,27 @@
       <c r="N5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="41"/>
+      <c r="O5" s="58"/>
     </row>
     <row r="6" spans="2:15" ht="18" customHeight="1" thickTop="1">
-      <c r="C6" s="38"/>
-      <c r="D6" s="32"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="30"/>
       <c r="E6" s="11"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="56"/>
     </row>
     <row r="7" spans="2:15" ht="18" customHeight="1">
-      <c r="C7" s="39"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="17"/>
       <c r="E7" s="13"/>
       <c r="F7" s="14"/>
@@ -44867,10 +44912,11 @@
       <c r="L7" s="16"/>
       <c r="M7" s="16"/>
       <c r="N7" s="16"/>
-      <c r="O7" s="27"/>
+      <c r="O7" s="57"/>
     </row>
     <row r="8" spans="2:15" ht="18" customHeight="1">
-      <c r="C8" s="40"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="38"/>
       <c r="D8" s="22"/>
       <c r="E8" s="18"/>
       <c r="F8" s="19"/>
@@ -44882,10 +44928,11 @@
       <c r="L8" s="21"/>
       <c r="M8" s="21"/>
       <c r="N8" s="21"/>
-      <c r="O8" s="26"/>
+      <c r="O8" s="56"/>
     </row>
     <row r="9" spans="2:15" ht="18" customHeight="1">
-      <c r="C9" s="39"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="17"/>
       <c r="E9" s="13"/>
       <c r="F9" s="14"/>
@@ -44897,10 +44944,11 @@
       <c r="L9" s="16"/>
       <c r="M9" s="16"/>
       <c r="N9" s="16"/>
-      <c r="O9" s="27"/>
+      <c r="O9" s="57"/>
     </row>
     <row r="10" spans="2:15" ht="18" customHeight="1">
-      <c r="C10" s="40"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="38"/>
       <c r="D10" s="22"/>
       <c r="E10" s="18"/>
       <c r="F10" s="19"/>
@@ -44912,10 +44960,11 @@
       <c r="L10" s="21"/>
       <c r="M10" s="21"/>
       <c r="N10" s="21"/>
-      <c r="O10" s="26"/>
+      <c r="O10" s="59"/>
     </row>
     <row r="11" spans="2:15" ht="18" customHeight="1">
-      <c r="C11" s="39"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="17"/>
       <c r="E11" s="13"/>
       <c r="F11" s="14"/>
@@ -44927,10 +44976,11 @@
       <c r="L11" s="16"/>
       <c r="M11" s="16"/>
       <c r="N11" s="16"/>
-      <c r="O11" s="27"/>
+      <c r="O11" s="60"/>
     </row>
     <row r="12" spans="2:15" ht="18" customHeight="1">
-      <c r="C12" s="40"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="22"/>
       <c r="E12" s="18"/>
       <c r="F12" s="19"/>
@@ -44942,10 +44992,11 @@
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
       <c r="N12" s="21"/>
-      <c r="O12" s="26"/>
+      <c r="O12" s="59"/>
     </row>
     <row r="13" spans="2:15" ht="18" customHeight="1">
-      <c r="C13" s="39"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="17"/>
       <c r="E13" s="13"/>
       <c r="F13" s="14"/>
@@ -44957,10 +45008,11 @@
       <c r="L13" s="16"/>
       <c r="M13" s="16"/>
       <c r="N13" s="16"/>
-      <c r="O13" s="27"/>
+      <c r="O13" s="60"/>
     </row>
     <row r="14" spans="2:15" ht="18" customHeight="1">
-      <c r="C14" s="40"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="38"/>
       <c r="D14" s="22"/>
       <c r="E14" s="18"/>
       <c r="F14" s="19"/>
@@ -44972,10 +45024,11 @@
       <c r="L14" s="21"/>
       <c r="M14" s="21"/>
       <c r="N14" s="21"/>
-      <c r="O14" s="26"/>
+      <c r="O14" s="59"/>
     </row>
     <row r="15" spans="2:15" ht="18" customHeight="1">
-      <c r="C15" s="39"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="17"/>
       <c r="E15" s="13"/>
       <c r="F15" s="14"/>
@@ -44987,10 +45040,11 @@
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
       <c r="N15" s="16"/>
-      <c r="O15" s="27"/>
+      <c r="O15" s="60"/>
     </row>
     <row r="16" spans="2:15" ht="18" customHeight="1">
-      <c r="C16" s="40"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="38"/>
       <c r="D16" s="22"/>
       <c r="E16" s="18"/>
       <c r="F16" s="19"/>
@@ -45002,10 +45056,11 @@
       <c r="L16" s="21"/>
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>
-      <c r="O16" s="26"/>
+      <c r="O16" s="59"/>
     </row>
-    <row r="17" spans="3:15" ht="18" customHeight="1">
-      <c r="C17" s="39"/>
+    <row r="17" spans="2:15" ht="18" customHeight="1">
+      <c r="B17" s="39"/>
+      <c r="C17" s="37"/>
       <c r="D17" s="17"/>
       <c r="E17" s="13"/>
       <c r="F17" s="14"/>
@@ -45017,10 +45072,11 @@
       <c r="L17" s="16"/>
       <c r="M17" s="16"/>
       <c r="N17" s="16"/>
-      <c r="O17" s="27"/>
+      <c r="O17" s="60"/>
     </row>
-    <row r="18" spans="3:15" ht="18" customHeight="1">
-      <c r="C18" s="40"/>
+    <row r="18" spans="2:15" ht="18" customHeight="1">
+      <c r="B18" s="39"/>
+      <c r="C18" s="38"/>
       <c r="D18" s="22"/>
       <c r="E18" s="18"/>
       <c r="F18" s="19"/>
@@ -45032,10 +45088,11 @@
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
       <c r="N18" s="21"/>
-      <c r="O18" s="26"/>
+      <c r="O18" s="59"/>
     </row>
-    <row r="19" spans="3:15" ht="18" customHeight="1">
-      <c r="C19" s="39"/>
+    <row r="19" spans="2:15" ht="18" customHeight="1">
+      <c r="B19" s="39"/>
+      <c r="C19" s="37"/>
       <c r="D19" s="17"/>
       <c r="E19" s="13"/>
       <c r="F19" s="14"/>
@@ -45047,10 +45104,11 @@
       <c r="L19" s="16"/>
       <c r="M19" s="16"/>
       <c r="N19" s="16"/>
-      <c r="O19" s="27"/>
+      <c r="O19" s="60"/>
     </row>
-    <row r="20" spans="3:15" ht="18" customHeight="1">
-      <c r="C20" s="40"/>
+    <row r="20" spans="2:15" ht="18" customHeight="1">
+      <c r="B20" s="39"/>
+      <c r="C20" s="38"/>
       <c r="D20" s="22"/>
       <c r="E20" s="18"/>
       <c r="F20" s="19"/>
@@ -45062,10 +45120,11 @@
       <c r="L20" s="21"/>
       <c r="M20" s="21"/>
       <c r="N20" s="21"/>
-      <c r="O20" s="26"/>
+      <c r="O20" s="59"/>
     </row>
-    <row r="21" spans="3:15" ht="18" customHeight="1">
-      <c r="C21" s="39"/>
+    <row r="21" spans="2:15" ht="18" customHeight="1">
+      <c r="B21" s="39"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="17"/>
       <c r="E21" s="13"/>
       <c r="F21" s="14"/>
@@ -45077,10 +45136,11 @@
       <c r="L21" s="16"/>
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
-      <c r="O21" s="27"/>
+      <c r="O21" s="60"/>
     </row>
-    <row r="22" spans="3:15" ht="18" customHeight="1">
-      <c r="C22" s="40"/>
+    <row r="22" spans="2:15" ht="18" customHeight="1">
+      <c r="B22" s="39"/>
+      <c r="C22" s="38"/>
       <c r="D22" s="22"/>
       <c r="E22" s="18"/>
       <c r="F22" s="19"/>
@@ -45092,10 +45152,11 @@
       <c r="L22" s="21"/>
       <c r="M22" s="21"/>
       <c r="N22" s="21"/>
-      <c r="O22" s="26"/>
+      <c r="O22" s="59"/>
     </row>
-    <row r="23" spans="3:15" ht="18" customHeight="1">
-      <c r="C23" s="39"/>
+    <row r="23" spans="2:15" ht="18" customHeight="1">
+      <c r="B23" s="39"/>
+      <c r="C23" s="37"/>
       <c r="D23" s="17"/>
       <c r="E23" s="13"/>
       <c r="F23" s="14"/>
@@ -45107,10 +45168,11 @@
       <c r="L23" s="16"/>
       <c r="M23" s="16"/>
       <c r="N23" s="16"/>
-      <c r="O23" s="27"/>
+      <c r="O23" s="60"/>
     </row>
-    <row r="24" spans="3:15" ht="18" customHeight="1">
-      <c r="C24" s="40"/>
+    <row r="24" spans="2:15" ht="18" customHeight="1">
+      <c r="B24" s="39"/>
+      <c r="C24" s="38"/>
       <c r="D24" s="22"/>
       <c r="E24" s="18"/>
       <c r="F24" s="19"/>
@@ -45122,10 +45184,11 @@
       <c r="L24" s="21"/>
       <c r="M24" s="21"/>
       <c r="N24" s="21"/>
-      <c r="O24" s="26"/>
+      <c r="O24" s="59"/>
     </row>
-    <row r="25" spans="3:15" ht="18" customHeight="1">
-      <c r="C25" s="39"/>
+    <row r="25" spans="2:15" ht="18" customHeight="1">
+      <c r="B25" s="39"/>
+      <c r="C25" s="37"/>
       <c r="D25" s="17"/>
       <c r="E25" s="13"/>
       <c r="F25" s="14"/>
@@ -45137,10 +45200,11 @@
       <c r="L25" s="16"/>
       <c r="M25" s="16"/>
       <c r="N25" s="16"/>
-      <c r="O25" s="27"/>
+      <c r="O25" s="60"/>
     </row>
-    <row r="26" spans="3:15" ht="18" customHeight="1">
-      <c r="C26" s="40"/>
+    <row r="26" spans="2:15" ht="18" customHeight="1">
+      <c r="B26" s="39"/>
+      <c r="C26" s="38"/>
       <c r="D26" s="22"/>
       <c r="E26" s="18"/>
       <c r="F26" s="19"/>
@@ -45152,10 +45216,11 @@
       <c r="L26" s="21"/>
       <c r="M26" s="21"/>
       <c r="N26" s="21"/>
-      <c r="O26" s="26"/>
+      <c r="O26" s="59"/>
     </row>
-    <row r="27" spans="3:15" ht="18" customHeight="1">
-      <c r="C27" s="39"/>
+    <row r="27" spans="2:15" ht="18" customHeight="1">
+      <c r="B27" s="39"/>
+      <c r="C27" s="37"/>
       <c r="D27" s="17"/>
       <c r="E27" s="13"/>
       <c r="F27" s="14"/>
@@ -45167,10 +45232,11 @@
       <c r="L27" s="16"/>
       <c r="M27" s="16"/>
       <c r="N27" s="16"/>
-      <c r="O27" s="27"/>
+      <c r="O27" s="60"/>
     </row>
-    <row r="28" spans="3:15" ht="18" customHeight="1">
-      <c r="C28" s="40"/>
+    <row r="28" spans="2:15" ht="18" customHeight="1">
+      <c r="B28" s="39"/>
+      <c r="C28" s="38"/>
       <c r="D28" s="22"/>
       <c r="E28" s="18"/>
       <c r="F28" s="19"/>
@@ -45182,10 +45248,11 @@
       <c r="L28" s="21"/>
       <c r="M28" s="21"/>
       <c r="N28" s="21"/>
-      <c r="O28" s="26"/>
+      <c r="O28" s="59"/>
     </row>
-    <row r="29" spans="3:15" ht="18" customHeight="1">
-      <c r="C29" s="39"/>
+    <row r="29" spans="2:15" ht="18" customHeight="1">
+      <c r="B29" s="39"/>
+      <c r="C29" s="37"/>
       <c r="D29" s="17"/>
       <c r="E29" s="13"/>
       <c r="F29" s="14"/>
@@ -45197,10 +45264,11 @@
       <c r="L29" s="16"/>
       <c r="M29" s="16"/>
       <c r="N29" s="16"/>
-      <c r="O29" s="27"/>
+      <c r="O29" s="60"/>
     </row>
-    <row r="30" spans="3:15" ht="18" customHeight="1">
-      <c r="C30" s="40"/>
+    <row r="30" spans="2:15" ht="18" customHeight="1">
+      <c r="B30" s="39"/>
+      <c r="C30" s="38"/>
       <c r="D30" s="22"/>
       <c r="E30" s="18"/>
       <c r="F30" s="19"/>
@@ -45212,10 +45280,11 @@
       <c r="L30" s="21"/>
       <c r="M30" s="21"/>
       <c r="N30" s="21"/>
-      <c r="O30" s="26"/>
+      <c r="O30" s="59"/>
     </row>
-    <row r="31" spans="3:15" ht="18" customHeight="1">
-      <c r="C31" s="39"/>
+    <row r="31" spans="2:15" ht="18" customHeight="1">
+      <c r="B31" s="39"/>
+      <c r="C31" s="37"/>
       <c r="D31" s="17"/>
       <c r="E31" s="13"/>
       <c r="F31" s="14"/>
@@ -45227,10 +45296,11 @@
       <c r="L31" s="16"/>
       <c r="M31" s="16"/>
       <c r="N31" s="16"/>
-      <c r="O31" s="27"/>
+      <c r="O31" s="60"/>
     </row>
-    <row r="32" spans="3:15" ht="18" customHeight="1">
-      <c r="C32" s="40"/>
+    <row r="32" spans="2:15" ht="18" customHeight="1">
+      <c r="B32" s="39"/>
+      <c r="C32" s="38"/>
       <c r="D32" s="22"/>
       <c r="E32" s="18"/>
       <c r="F32" s="19"/>
@@ -45242,10 +45312,11 @@
       <c r="L32" s="21"/>
       <c r="M32" s="21"/>
       <c r="N32" s="21"/>
-      <c r="O32" s="26"/>
+      <c r="O32" s="59"/>
     </row>
-    <row r="33" spans="3:15" ht="18" customHeight="1">
-      <c r="C33" s="39"/>
+    <row r="33" spans="2:15" ht="18" customHeight="1">
+      <c r="B33" s="39"/>
+      <c r="C33" s="37"/>
       <c r="D33" s="17"/>
       <c r="E33" s="13"/>
       <c r="F33" s="14"/>
@@ -45257,10 +45328,11 @@
       <c r="L33" s="16"/>
       <c r="M33" s="16"/>
       <c r="N33" s="16"/>
-      <c r="O33" s="27"/>
+      <c r="O33" s="60"/>
     </row>
-    <row r="34" spans="3:15" ht="18" customHeight="1">
-      <c r="C34" s="40"/>
+    <row r="34" spans="2:15" ht="18" customHeight="1">
+      <c r="B34" s="39"/>
+      <c r="C34" s="38"/>
       <c r="D34" s="22"/>
       <c r="E34" s="18"/>
       <c r="F34" s="19"/>
@@ -45272,10 +45344,11 @@
       <c r="L34" s="21"/>
       <c r="M34" s="21"/>
       <c r="N34" s="21"/>
-      <c r="O34" s="26"/>
+      <c r="O34" s="59"/>
     </row>
-    <row r="35" spans="3:15" ht="18" customHeight="1">
-      <c r="C35" s="39"/>
+    <row r="35" spans="2:15" ht="18" customHeight="1">
+      <c r="B35" s="39"/>
+      <c r="C35" s="37"/>
       <c r="D35" s="17"/>
       <c r="E35" s="13"/>
       <c r="F35" s="14"/>
@@ -45287,10 +45360,11 @@
       <c r="L35" s="16"/>
       <c r="M35" s="16"/>
       <c r="N35" s="16"/>
-      <c r="O35" s="27"/>
+      <c r="O35" s="60"/>
     </row>
-    <row r="36" spans="3:15" ht="18" customHeight="1">
-      <c r="C36" s="40"/>
+    <row r="36" spans="2:15" ht="18" customHeight="1">
+      <c r="B36" s="39"/>
+      <c r="C36" s="38"/>
       <c r="D36" s="22"/>
       <c r="E36" s="18"/>
       <c r="F36" s="19"/>
@@ -45302,10 +45376,11 @@
       <c r="L36" s="21"/>
       <c r="M36" s="21"/>
       <c r="N36" s="21"/>
-      <c r="O36" s="26"/>
+      <c r="O36" s="59"/>
     </row>
-    <row r="37" spans="3:15" ht="18" customHeight="1">
-      <c r="C37" s="39"/>
+    <row r="37" spans="2:15" ht="18" customHeight="1">
+      <c r="B37" s="39"/>
+      <c r="C37" s="37"/>
       <c r="D37" s="17"/>
       <c r="E37" s="13"/>
       <c r="F37" s="14"/>
@@ -45317,25 +45392,27 @@
       <c r="L37" s="16"/>
       <c r="M37" s="16"/>
       <c r="N37" s="16"/>
-      <c r="O37" s="27"/>
+      <c r="O37" s="60"/>
     </row>
-    <row r="38" spans="3:15" ht="18" customHeight="1">
-      <c r="C38" s="38"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="30"/>
-      <c r="K38" s="37"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
-      <c r="N38" s="29"/>
-      <c r="O38" s="26"/>
+    <row r="38" spans="2:15" ht="18" customHeight="1">
+      <c r="B38" s="39"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="28"/>
+      <c r="K38" s="35"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="27"/>
+      <c r="N38" s="27"/>
+      <c r="O38" s="59"/>
     </row>
-    <row r="39" spans="3:15" ht="18" customHeight="1">
-      <c r="C39" s="39"/>
+    <row r="39" spans="2:15" ht="18" customHeight="1">
+      <c r="B39" s="39"/>
+      <c r="C39" s="37"/>
       <c r="D39" s="17"/>
       <c r="E39" s="13"/>
       <c r="F39" s="14"/>
@@ -45347,10 +45424,11 @@
       <c r="L39" s="16"/>
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
-      <c r="O39" s="27"/>
+      <c r="O39" s="60"/>
     </row>
-    <row r="40" spans="3:15" ht="18" customHeight="1">
-      <c r="C40" s="40"/>
+    <row r="40" spans="2:15" ht="18" customHeight="1">
+      <c r="B40" s="39"/>
+      <c r="C40" s="38"/>
       <c r="D40" s="22"/>
       <c r="E40" s="18"/>
       <c r="F40" s="19"/>
@@ -45362,10 +45440,11 @@
       <c r="L40" s="21"/>
       <c r="M40" s="21"/>
       <c r="N40" s="21"/>
-      <c r="O40" s="26"/>
+      <c r="O40" s="59"/>
     </row>
-    <row r="41" spans="3:15" ht="18" customHeight="1">
-      <c r="C41" s="39"/>
+    <row r="41" spans="2:15" ht="18" customHeight="1">
+      <c r="B41" s="39"/>
+      <c r="C41" s="37"/>
       <c r="D41" s="17"/>
       <c r="E41" s="13"/>
       <c r="F41" s="14"/>
@@ -45377,10 +45456,11 @@
       <c r="L41" s="16"/>
       <c r="M41" s="16"/>
       <c r="N41" s="16"/>
-      <c r="O41" s="27"/>
+      <c r="O41" s="60"/>
     </row>
-    <row r="42" spans="3:15" ht="18" customHeight="1">
-      <c r="C42" s="40"/>
+    <row r="42" spans="2:15" ht="18" customHeight="1">
+      <c r="B42" s="39"/>
+      <c r="C42" s="38"/>
       <c r="D42" s="22"/>
       <c r="E42" s="18"/>
       <c r="F42" s="19"/>
@@ -45392,10 +45472,11 @@
       <c r="L42" s="21"/>
       <c r="M42" s="21"/>
       <c r="N42" s="21"/>
-      <c r="O42" s="26"/>
+      <c r="O42" s="59"/>
     </row>
-    <row r="43" spans="3:15" ht="18" customHeight="1">
-      <c r="C43" s="39"/>
+    <row r="43" spans="2:15" ht="18" customHeight="1">
+      <c r="B43" s="39"/>
+      <c r="C43" s="37"/>
       <c r="D43" s="17"/>
       <c r="E43" s="13"/>
       <c r="F43" s="14"/>
@@ -45407,10 +45488,11 @@
       <c r="L43" s="16"/>
       <c r="M43" s="16"/>
       <c r="N43" s="16"/>
-      <c r="O43" s="27"/>
+      <c r="O43" s="60"/>
     </row>
-    <row r="44" spans="3:15" ht="18" customHeight="1">
-      <c r="C44" s="40"/>
+    <row r="44" spans="2:15" ht="18" customHeight="1">
+      <c r="B44" s="39"/>
+      <c r="C44" s="38"/>
       <c r="D44" s="22"/>
       <c r="E44" s="18"/>
       <c r="F44" s="19"/>
@@ -45422,10 +45504,11 @@
       <c r="L44" s="21"/>
       <c r="M44" s="21"/>
       <c r="N44" s="21"/>
-      <c r="O44" s="26"/>
+      <c r="O44" s="59"/>
     </row>
-    <row r="45" spans="3:15" ht="18" customHeight="1">
-      <c r="C45" s="39"/>
+    <row r="45" spans="2:15" ht="18" customHeight="1">
+      <c r="B45" s="39"/>
+      <c r="C45" s="37"/>
       <c r="D45" s="17"/>
       <c r="E45" s="13"/>
       <c r="F45" s="14"/>
@@ -45437,10 +45520,11 @@
       <c r="L45" s="16"/>
       <c r="M45" s="16"/>
       <c r="N45" s="16"/>
-      <c r="O45" s="27"/>
+      <c r="O45" s="60"/>
     </row>
-    <row r="46" spans="3:15" ht="18" customHeight="1">
-      <c r="C46" s="40"/>
+    <row r="46" spans="2:15" ht="18" customHeight="1">
+      <c r="B46" s="39"/>
+      <c r="C46" s="38"/>
       <c r="D46" s="22"/>
       <c r="E46" s="18"/>
       <c r="F46" s="19"/>
@@ -45452,10 +45536,11 @@
       <c r="L46" s="21"/>
       <c r="M46" s="21"/>
       <c r="N46" s="21"/>
-      <c r="O46" s="26"/>
+      <c r="O46" s="59"/>
     </row>
-    <row r="47" spans="3:15" ht="18" customHeight="1">
-      <c r="C47" s="39"/>
+    <row r="47" spans="2:15" ht="18" customHeight="1">
+      <c r="B47" s="39"/>
+      <c r="C47" s="37"/>
       <c r="D47" s="17"/>
       <c r="E47" s="13"/>
       <c r="F47" s="14"/>
@@ -45467,10 +45552,11 @@
       <c r="L47" s="16"/>
       <c r="M47" s="16"/>
       <c r="N47" s="16"/>
-      <c r="O47" s="27"/>
+      <c r="O47" s="60"/>
     </row>
-    <row r="48" spans="3:15" ht="18" customHeight="1">
-      <c r="C48" s="40"/>
+    <row r="48" spans="2:15" ht="18" customHeight="1">
+      <c r="B48" s="39"/>
+      <c r="C48" s="38"/>
       <c r="D48" s="22"/>
       <c r="E48" s="18"/>
       <c r="F48" s="19"/>
@@ -45482,10 +45568,11 @@
       <c r="L48" s="21"/>
       <c r="M48" s="21"/>
       <c r="N48" s="21"/>
-      <c r="O48" s="26"/>
+      <c r="O48" s="59"/>
     </row>
-    <row r="49" spans="3:15" ht="18" customHeight="1">
-      <c r="C49" s="39"/>
+    <row r="49" spans="2:15" ht="18" customHeight="1">
+      <c r="B49" s="39"/>
+      <c r="C49" s="37"/>
       <c r="D49" s="17"/>
       <c r="E49" s="13"/>
       <c r="F49" s="14"/>
@@ -45497,10 +45584,11 @@
       <c r="L49" s="16"/>
       <c r="M49" s="16"/>
       <c r="N49" s="16"/>
-      <c r="O49" s="27"/>
+      <c r="O49" s="60"/>
     </row>
-    <row r="50" spans="3:15" ht="18" customHeight="1">
-      <c r="C50" s="40"/>
+    <row r="50" spans="2:15" ht="18" customHeight="1">
+      <c r="B50" s="39"/>
+      <c r="C50" s="38"/>
       <c r="D50" s="22"/>
       <c r="E50" s="18"/>
       <c r="F50" s="19"/>
@@ -45512,10 +45600,11 @@
       <c r="L50" s="21"/>
       <c r="M50" s="21"/>
       <c r="N50" s="21"/>
-      <c r="O50" s="26"/>
+      <c r="O50" s="59"/>
     </row>
-    <row r="51" spans="3:15" ht="18" customHeight="1">
-      <c r="C51" s="39"/>
+    <row r="51" spans="2:15" ht="18" customHeight="1">
+      <c r="B51" s="39"/>
+      <c r="C51" s="37"/>
       <c r="D51" s="17"/>
       <c r="E51" s="13"/>
       <c r="F51" s="14"/>
@@ -45527,10 +45616,11 @@
       <c r="L51" s="16"/>
       <c r="M51" s="16"/>
       <c r="N51" s="16"/>
-      <c r="O51" s="27"/>
+      <c r="O51" s="60"/>
     </row>
-    <row r="52" spans="3:15" ht="18" customHeight="1">
-      <c r="C52" s="40"/>
+    <row r="52" spans="2:15" ht="18" customHeight="1">
+      <c r="B52" s="39"/>
+      <c r="C52" s="38"/>
       <c r="D52" s="22"/>
       <c r="E52" s="18"/>
       <c r="F52" s="19"/>
@@ -45542,10 +45632,11 @@
       <c r="L52" s="21"/>
       <c r="M52" s="21"/>
       <c r="N52" s="21"/>
-      <c r="O52" s="26"/>
+      <c r="O52" s="59"/>
     </row>
-    <row r="53" spans="3:15" ht="18" customHeight="1">
-      <c r="C53" s="39"/>
+    <row r="53" spans="2:15" ht="18" customHeight="1">
+      <c r="B53" s="39"/>
+      <c r="C53" s="37"/>
       <c r="D53" s="17"/>
       <c r="E53" s="13"/>
       <c r="F53" s="14"/>
@@ -45557,10 +45648,11 @@
       <c r="L53" s="16"/>
       <c r="M53" s="16"/>
       <c r="N53" s="16"/>
-      <c r="O53" s="27"/>
+      <c r="O53" s="60"/>
     </row>
-    <row r="54" spans="3:15" ht="18" customHeight="1">
-      <c r="C54" s="40"/>
+    <row r="54" spans="2:15" ht="18" customHeight="1">
+      <c r="B54" s="39"/>
+      <c r="C54" s="38"/>
       <c r="D54" s="22"/>
       <c r="E54" s="18"/>
       <c r="F54" s="19"/>
@@ -45572,10 +45664,11 @@
       <c r="L54" s="21"/>
       <c r="M54" s="21"/>
       <c r="N54" s="21"/>
-      <c r="O54" s="26"/>
+      <c r="O54" s="59"/>
     </row>
-    <row r="55" spans="3:15" ht="18" customHeight="1">
-      <c r="C55" s="39"/>
+    <row r="55" spans="2:15" ht="18" customHeight="1">
+      <c r="B55" s="39"/>
+      <c r="C55" s="37"/>
       <c r="D55" s="17"/>
       <c r="E55" s="13"/>
       <c r="F55" s="14"/>
@@ -45587,10 +45680,11 @@
       <c r="L55" s="16"/>
       <c r="M55" s="16"/>
       <c r="N55" s="16"/>
-      <c r="O55" s="27"/>
+      <c r="O55" s="60"/>
     </row>
-    <row r="56" spans="3:15" ht="18" customHeight="1">
-      <c r="C56" s="40"/>
+    <row r="56" spans="2:15" ht="18" customHeight="1">
+      <c r="B56" s="39"/>
+      <c r="C56" s="38"/>
       <c r="D56" s="22"/>
       <c r="E56" s="18"/>
       <c r="F56" s="19"/>
@@ -45602,10 +45696,11 @@
       <c r="L56" s="21"/>
       <c r="M56" s="21"/>
       <c r="N56" s="21"/>
-      <c r="O56" s="26"/>
+      <c r="O56" s="59"/>
     </row>
-    <row r="57" spans="3:15" ht="18" customHeight="1">
-      <c r="C57" s="39"/>
+    <row r="57" spans="2:15" ht="18" customHeight="1">
+      <c r="B57" s="39"/>
+      <c r="C57" s="37"/>
       <c r="D57" s="17"/>
       <c r="E57" s="13"/>
       <c r="F57" s="14"/>
@@ -45617,10 +45712,11 @@
       <c r="L57" s="16"/>
       <c r="M57" s="16"/>
       <c r="N57" s="16"/>
-      <c r="O57" s="27"/>
+      <c r="O57" s="60"/>
     </row>
-    <row r="58" spans="3:15" ht="18" customHeight="1">
-      <c r="C58" s="40"/>
+    <row r="58" spans="2:15" ht="18" customHeight="1">
+      <c r="B58" s="39"/>
+      <c r="C58" s="38"/>
       <c r="D58" s="22"/>
       <c r="E58" s="18"/>
       <c r="F58" s="19"/>
@@ -45632,10 +45728,11 @@
       <c r="L58" s="21"/>
       <c r="M58" s="21"/>
       <c r="N58" s="21"/>
-      <c r="O58" s="26"/>
+      <c r="O58" s="59"/>
     </row>
-    <row r="59" spans="3:15" ht="18" customHeight="1">
-      <c r="C59" s="39"/>
+    <row r="59" spans="2:15" ht="18" customHeight="1">
+      <c r="B59" s="39"/>
+      <c r="C59" s="37"/>
       <c r="D59" s="17"/>
       <c r="E59" s="13"/>
       <c r="F59" s="14"/>
@@ -45647,10 +45744,11 @@
       <c r="L59" s="16"/>
       <c r="M59" s="16"/>
       <c r="N59" s="16"/>
-      <c r="O59" s="27"/>
+      <c r="O59" s="60"/>
     </row>
-    <row r="60" spans="3:15" ht="18" customHeight="1">
-      <c r="C60" s="40"/>
+    <row r="60" spans="2:15" ht="18" customHeight="1">
+      <c r="B60" s="39"/>
+      <c r="C60" s="38"/>
       <c r="D60" s="22"/>
       <c r="E60" s="18"/>
       <c r="F60" s="19"/>
@@ -45662,10 +45760,11 @@
       <c r="L60" s="21"/>
       <c r="M60" s="21"/>
       <c r="N60" s="21"/>
-      <c r="O60" s="26"/>
+      <c r="O60" s="59"/>
     </row>
-    <row r="61" spans="3:15" ht="18" customHeight="1">
-      <c r="C61" s="39"/>
+    <row r="61" spans="2:15" ht="18" customHeight="1">
+      <c r="B61" s="39"/>
+      <c r="C61" s="37"/>
       <c r="D61" s="17"/>
       <c r="E61" s="13"/>
       <c r="F61" s="14"/>
@@ -45677,10 +45776,11 @@
       <c r="L61" s="16"/>
       <c r="M61" s="16"/>
       <c r="N61" s="16"/>
-      <c r="O61" s="27"/>
+      <c r="O61" s="60"/>
     </row>
-    <row r="62" spans="3:15" ht="18" customHeight="1">
-      <c r="C62" s="40"/>
+    <row r="62" spans="2:15" ht="18" customHeight="1">
+      <c r="B62" s="39"/>
+      <c r="C62" s="38"/>
       <c r="D62" s="22"/>
       <c r="E62" s="18"/>
       <c r="F62" s="19"/>
@@ -45692,10 +45792,11 @@
       <c r="L62" s="21"/>
       <c r="M62" s="21"/>
       <c r="N62" s="21"/>
-      <c r="O62" s="26"/>
+      <c r="O62" s="59"/>
     </row>
-    <row r="63" spans="3:15" ht="18" customHeight="1">
-      <c r="C63" s="39"/>
+    <row r="63" spans="2:15" ht="18" customHeight="1">
+      <c r="B63" s="39"/>
+      <c r="C63" s="37"/>
       <c r="D63" s="17"/>
       <c r="E63" s="13"/>
       <c r="F63" s="14"/>
@@ -45707,10 +45808,11 @@
       <c r="L63" s="16"/>
       <c r="M63" s="16"/>
       <c r="N63" s="16"/>
-      <c r="O63" s="27"/>
+      <c r="O63" s="60"/>
     </row>
-    <row r="64" spans="3:15" ht="18" customHeight="1">
-      <c r="C64" s="40"/>
+    <row r="64" spans="2:15" ht="18" customHeight="1">
+      <c r="B64" s="39"/>
+      <c r="C64" s="38"/>
       <c r="D64" s="22"/>
       <c r="E64" s="18"/>
       <c r="F64" s="19"/>
@@ -45722,10 +45824,11 @@
       <c r="L64" s="21"/>
       <c r="M64" s="21"/>
       <c r="N64" s="21"/>
-      <c r="O64" s="26"/>
+      <c r="O64" s="59"/>
     </row>
-    <row r="65" spans="3:15" ht="18" customHeight="1">
-      <c r="C65" s="39"/>
+    <row r="65" spans="2:15" ht="18" customHeight="1">
+      <c r="B65" s="39"/>
+      <c r="C65" s="37"/>
       <c r="D65" s="17"/>
       <c r="E65" s="13"/>
       <c r="F65" s="14"/>
@@ -45737,10 +45840,11 @@
       <c r="L65" s="16"/>
       <c r="M65" s="16"/>
       <c r="N65" s="16"/>
-      <c r="O65" s="27"/>
+      <c r="O65" s="60"/>
     </row>
-    <row r="66" spans="3:15" ht="18" customHeight="1">
-      <c r="C66" s="40"/>
+    <row r="66" spans="2:15" ht="18" customHeight="1">
+      <c r="B66" s="39"/>
+      <c r="C66" s="38"/>
       <c r="D66" s="22"/>
       <c r="E66" s="18"/>
       <c r="F66" s="19"/>
@@ -45752,23 +45856,25 @@
       <c r="L66" s="21"/>
       <c r="M66" s="21"/>
       <c r="N66" s="21"/>
-      <c r="O66" s="26"/>
+      <c r="O66" s="59"/>
     </row>
-    <row r="67" spans="3:15" ht="18" customHeight="1">
-      <c r="C67" s="39"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="15"/>
-      <c r="H67" s="16"/>
-      <c r="I67" s="16"/>
-      <c r="J67" s="17"/>
-      <c r="K67" s="13"/>
-      <c r="L67" s="16"/>
-      <c r="M67" s="16"/>
-      <c r="N67" s="16"/>
-      <c r="O67" s="27"/>
+    <row r="67" spans="2:15" ht="18" customHeight="1" thickBot="1">
+      <c r="B67" s="39"/>
+      <c r="C67" s="61"/>
+      <c r="D67" s="62"/>
+      <c r="E67" s="63"/>
+      <c r="F67" s="64"/>
+      <c r="G67" s="65"/>
+      <c r="H67" s="66"/>
+      <c r="I67" s="66"/>
+      <c r="J67" s="62"/>
+      <c r="K67" s="63"/>
+      <c r="L67" s="66"/>
+      <c r="M67" s="66"/>
+      <c r="N67" s="66"/>
+      <c r="O67" s="67"/>
     </row>
+    <row r="68" spans="2:15" ht="12.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="O3:O5"/>
@@ -45783,12 +45889,11 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="55" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="56" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;10日通システム株式会社 &amp;C&amp;"ＭＳ ゴシック,Regular"&amp;16標準報酬月額表（厚生年金）&amp;R&amp;"ＭＳ ゴシック,Regular"&amp;10&amp;KFF0000 &amp;K01+000&amp;D　&amp;T　
 &amp;KFF0000 &amp;K01+000page&amp;P</oddHeader>
   </headerFooter>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -45797,17 +45902,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:O67"/>
+  <dimension ref="B1:O68"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
-    </sheetView>
+    <sheetView view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="2.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" style="33" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="31" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="1" customWidth="1"/>
     <col min="5" max="6" width="10.7109375" style="1"/>
     <col min="7" max="14" width="14.42578125" style="1" customWidth="1"/>
@@ -45830,60 +45933,73 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:15" ht="4.9000000000000004" customHeight="1">
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
+    <row r="2" spans="2:15" ht="4.9000000000000004" customHeight="1" thickBot="1">
+      <c r="C2" s="52"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
     </row>
-    <row r="3" spans="2:15" ht="18" customHeight="1">
-      <c r="C3" s="42" t="s">
+    <row r="3" spans="2:15" ht="18" customHeight="1" thickTop="1">
+      <c r="B3" s="39"/>
+      <c r="C3" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="44" t="s">
+      <c r="D3" s="41"/>
+      <c r="E3" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="45"/>
-      <c r="G3" s="46" t="s">
+      <c r="F3" s="43"/>
+      <c r="G3" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="46" t="s">
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="41" t="s">
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="58" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:15" ht="18" customHeight="1">
-      <c r="C4" s="34"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="23"/>
       <c r="E4" s="24"/>
       <c r="F4" s="25"/>
-      <c r="G4" s="50" t="s">
+      <c r="G4" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="51"/>
-      <c r="I4" s="52" t="s">
+      <c r="H4" s="49"/>
+      <c r="I4" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="53"/>
-      <c r="K4" s="50" t="s">
+      <c r="J4" s="51"/>
+      <c r="K4" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="51"/>
-      <c r="M4" s="52" t="s">
+      <c r="L4" s="49"/>
+      <c r="M4" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="53"/>
-      <c r="O4" s="41"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="58"/>
     </row>
     <row r="5" spans="2:15" ht="18" customHeight="1" thickBot="1">
+      <c r="B5" s="39"/>
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
@@ -45920,25 +46036,27 @@
       <c r="N5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="41"/>
+      <c r="O5" s="58"/>
     </row>
     <row r="6" spans="2:15" ht="18" customHeight="1" thickTop="1">
-      <c r="C6" s="38"/>
-      <c r="D6" s="32"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="30"/>
       <c r="E6" s="11"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="56"/>
     </row>
     <row r="7" spans="2:15" ht="18" customHeight="1">
-      <c r="C7" s="39"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="17"/>
       <c r="E7" s="13"/>
       <c r="F7" s="14"/>
@@ -45950,10 +46068,11 @@
       <c r="L7" s="16"/>
       <c r="M7" s="16"/>
       <c r="N7" s="16"/>
-      <c r="O7" s="27"/>
+      <c r="O7" s="57"/>
     </row>
     <row r="8" spans="2:15" ht="18" customHeight="1">
-      <c r="C8" s="40"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="38"/>
       <c r="D8" s="22"/>
       <c r="E8" s="18"/>
       <c r="F8" s="19"/>
@@ -45965,10 +46084,11 @@
       <c r="L8" s="21"/>
       <c r="M8" s="21"/>
       <c r="N8" s="21"/>
-      <c r="O8" s="26"/>
+      <c r="O8" s="56"/>
     </row>
     <row r="9" spans="2:15" ht="18" customHeight="1">
-      <c r="C9" s="39"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="17"/>
       <c r="E9" s="13"/>
       <c r="F9" s="14"/>
@@ -45980,10 +46100,11 @@
       <c r="L9" s="16"/>
       <c r="M9" s="16"/>
       <c r="N9" s="16"/>
-      <c r="O9" s="27"/>
+      <c r="O9" s="57"/>
     </row>
     <row r="10" spans="2:15" ht="18" customHeight="1">
-      <c r="C10" s="40"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="38"/>
       <c r="D10" s="22"/>
       <c r="E10" s="18"/>
       <c r="F10" s="19"/>
@@ -45995,10 +46116,11 @@
       <c r="L10" s="21"/>
       <c r="M10" s="21"/>
       <c r="N10" s="21"/>
-      <c r="O10" s="26"/>
+      <c r="O10" s="59"/>
     </row>
     <row r="11" spans="2:15" ht="18" customHeight="1">
-      <c r="C11" s="39"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="17"/>
       <c r="E11" s="13"/>
       <c r="F11" s="14"/>
@@ -46010,10 +46132,11 @@
       <c r="L11" s="16"/>
       <c r="M11" s="16"/>
       <c r="N11" s="16"/>
-      <c r="O11" s="27"/>
+      <c r="O11" s="60"/>
     </row>
     <row r="12" spans="2:15" ht="18" customHeight="1">
-      <c r="C12" s="40"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="22"/>
       <c r="E12" s="18"/>
       <c r="F12" s="19"/>
@@ -46025,10 +46148,11 @@
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
       <c r="N12" s="21"/>
-      <c r="O12" s="26"/>
+      <c r="O12" s="59"/>
     </row>
     <row r="13" spans="2:15" ht="18" customHeight="1">
-      <c r="C13" s="39"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="17"/>
       <c r="E13" s="13"/>
       <c r="F13" s="14"/>
@@ -46040,10 +46164,11 @@
       <c r="L13" s="16"/>
       <c r="M13" s="16"/>
       <c r="N13" s="16"/>
-      <c r="O13" s="27"/>
+      <c r="O13" s="60"/>
     </row>
     <row r="14" spans="2:15" ht="18" customHeight="1">
-      <c r="C14" s="40"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="38"/>
       <c r="D14" s="22"/>
       <c r="E14" s="18"/>
       <c r="F14" s="19"/>
@@ -46055,10 +46180,11 @@
       <c r="L14" s="21"/>
       <c r="M14" s="21"/>
       <c r="N14" s="21"/>
-      <c r="O14" s="26"/>
+      <c r="O14" s="59"/>
     </row>
     <row r="15" spans="2:15" ht="18" customHeight="1">
-      <c r="C15" s="39"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="17"/>
       <c r="E15" s="13"/>
       <c r="F15" s="14"/>
@@ -46070,10 +46196,11 @@
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
       <c r="N15" s="16"/>
-      <c r="O15" s="27"/>
+      <c r="O15" s="60"/>
     </row>
     <row r="16" spans="2:15" ht="18" customHeight="1">
-      <c r="C16" s="40"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="38"/>
       <c r="D16" s="22"/>
       <c r="E16" s="18"/>
       <c r="F16" s="19"/>
@@ -46085,10 +46212,11 @@
       <c r="L16" s="21"/>
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>
-      <c r="O16" s="26"/>
+      <c r="O16" s="59"/>
     </row>
-    <row r="17" spans="3:15" ht="18" customHeight="1">
-      <c r="C17" s="39"/>
+    <row r="17" spans="2:15" ht="18" customHeight="1">
+      <c r="B17" s="39"/>
+      <c r="C17" s="37"/>
       <c r="D17" s="17"/>
       <c r="E17" s="13"/>
       <c r="F17" s="14"/>
@@ -46100,10 +46228,11 @@
       <c r="L17" s="16"/>
       <c r="M17" s="16"/>
       <c r="N17" s="16"/>
-      <c r="O17" s="27"/>
+      <c r="O17" s="60"/>
     </row>
-    <row r="18" spans="3:15" ht="18" customHeight="1">
-      <c r="C18" s="40"/>
+    <row r="18" spans="2:15" ht="18" customHeight="1">
+      <c r="B18" s="39"/>
+      <c r="C18" s="38"/>
       <c r="D18" s="22"/>
       <c r="E18" s="18"/>
       <c r="F18" s="19"/>
@@ -46115,10 +46244,11 @@
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
       <c r="N18" s="21"/>
-      <c r="O18" s="26"/>
+      <c r="O18" s="59"/>
     </row>
-    <row r="19" spans="3:15" ht="18" customHeight="1">
-      <c r="C19" s="39"/>
+    <row r="19" spans="2:15" ht="18" customHeight="1">
+      <c r="B19" s="39"/>
+      <c r="C19" s="37"/>
       <c r="D19" s="17"/>
       <c r="E19" s="13"/>
       <c r="F19" s="14"/>
@@ -46130,10 +46260,11 @@
       <c r="L19" s="16"/>
       <c r="M19" s="16"/>
       <c r="N19" s="16"/>
-      <c r="O19" s="27"/>
+      <c r="O19" s="60"/>
     </row>
-    <row r="20" spans="3:15" ht="18" customHeight="1">
-      <c r="C20" s="40"/>
+    <row r="20" spans="2:15" ht="18" customHeight="1">
+      <c r="B20" s="39"/>
+      <c r="C20" s="38"/>
       <c r="D20" s="22"/>
       <c r="E20" s="18"/>
       <c r="F20" s="19"/>
@@ -46145,10 +46276,11 @@
       <c r="L20" s="21"/>
       <c r="M20" s="21"/>
       <c r="N20" s="21"/>
-      <c r="O20" s="26"/>
+      <c r="O20" s="59"/>
     </row>
-    <row r="21" spans="3:15" ht="18" customHeight="1">
-      <c r="C21" s="39"/>
+    <row r="21" spans="2:15" ht="18" customHeight="1">
+      <c r="B21" s="39"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="17"/>
       <c r="E21" s="13"/>
       <c r="F21" s="14"/>
@@ -46160,10 +46292,11 @@
       <c r="L21" s="16"/>
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
-      <c r="O21" s="27"/>
+      <c r="O21" s="60"/>
     </row>
-    <row r="22" spans="3:15" ht="18" customHeight="1">
-      <c r="C22" s="40"/>
+    <row r="22" spans="2:15" ht="18" customHeight="1">
+      <c r="B22" s="39"/>
+      <c r="C22" s="38"/>
       <c r="D22" s="22"/>
       <c r="E22" s="18"/>
       <c r="F22" s="19"/>
@@ -46175,10 +46308,11 @@
       <c r="L22" s="21"/>
       <c r="M22" s="21"/>
       <c r="N22" s="21"/>
-      <c r="O22" s="26"/>
+      <c r="O22" s="59"/>
     </row>
-    <row r="23" spans="3:15" ht="18" customHeight="1">
-      <c r="C23" s="39"/>
+    <row r="23" spans="2:15" ht="18" customHeight="1">
+      <c r="B23" s="39"/>
+      <c r="C23" s="37"/>
       <c r="D23" s="17"/>
       <c r="E23" s="13"/>
       <c r="F23" s="14"/>
@@ -46190,10 +46324,11 @@
       <c r="L23" s="16"/>
       <c r="M23" s="16"/>
       <c r="N23" s="16"/>
-      <c r="O23" s="27"/>
+      <c r="O23" s="60"/>
     </row>
-    <row r="24" spans="3:15" ht="18" customHeight="1">
-      <c r="C24" s="40"/>
+    <row r="24" spans="2:15" ht="18" customHeight="1">
+      <c r="B24" s="39"/>
+      <c r="C24" s="38"/>
       <c r="D24" s="22"/>
       <c r="E24" s="18"/>
       <c r="F24" s="19"/>
@@ -46205,10 +46340,11 @@
       <c r="L24" s="21"/>
       <c r="M24" s="21"/>
       <c r="N24" s="21"/>
-      <c r="O24" s="26"/>
+      <c r="O24" s="59"/>
     </row>
-    <row r="25" spans="3:15" ht="18" customHeight="1">
-      <c r="C25" s="39"/>
+    <row r="25" spans="2:15" ht="18" customHeight="1">
+      <c r="B25" s="39"/>
+      <c r="C25" s="37"/>
       <c r="D25" s="17"/>
       <c r="E25" s="13"/>
       <c r="F25" s="14"/>
@@ -46220,10 +46356,11 @@
       <c r="L25" s="16"/>
       <c r="M25" s="16"/>
       <c r="N25" s="16"/>
-      <c r="O25" s="27"/>
+      <c r="O25" s="60"/>
     </row>
-    <row r="26" spans="3:15" ht="18" customHeight="1">
-      <c r="C26" s="40"/>
+    <row r="26" spans="2:15" ht="18" customHeight="1">
+      <c r="B26" s="39"/>
+      <c r="C26" s="38"/>
       <c r="D26" s="22"/>
       <c r="E26" s="18"/>
       <c r="F26" s="19"/>
@@ -46235,10 +46372,11 @@
       <c r="L26" s="21"/>
       <c r="M26" s="21"/>
       <c r="N26" s="21"/>
-      <c r="O26" s="26"/>
+      <c r="O26" s="59"/>
     </row>
-    <row r="27" spans="3:15" ht="18" customHeight="1">
-      <c r="C27" s="39"/>
+    <row r="27" spans="2:15" ht="18" customHeight="1">
+      <c r="B27" s="39"/>
+      <c r="C27" s="37"/>
       <c r="D27" s="17"/>
       <c r="E27" s="13"/>
       <c r="F27" s="14"/>
@@ -46250,10 +46388,11 @@
       <c r="L27" s="16"/>
       <c r="M27" s="16"/>
       <c r="N27" s="16"/>
-      <c r="O27" s="27"/>
+      <c r="O27" s="60"/>
     </row>
-    <row r="28" spans="3:15" ht="18" customHeight="1">
-      <c r="C28" s="40"/>
+    <row r="28" spans="2:15" ht="18" customHeight="1">
+      <c r="B28" s="39"/>
+      <c r="C28" s="38"/>
       <c r="D28" s="22"/>
       <c r="E28" s="18"/>
       <c r="F28" s="19"/>
@@ -46265,10 +46404,11 @@
       <c r="L28" s="21"/>
       <c r="M28" s="21"/>
       <c r="N28" s="21"/>
-      <c r="O28" s="26"/>
+      <c r="O28" s="59"/>
     </row>
-    <row r="29" spans="3:15" ht="18" customHeight="1">
-      <c r="C29" s="39"/>
+    <row r="29" spans="2:15" ht="18" customHeight="1">
+      <c r="B29" s="39"/>
+      <c r="C29" s="37"/>
       <c r="D29" s="17"/>
       <c r="E29" s="13"/>
       <c r="F29" s="14"/>
@@ -46280,10 +46420,11 @@
       <c r="L29" s="16"/>
       <c r="M29" s="16"/>
       <c r="N29" s="16"/>
-      <c r="O29" s="27"/>
+      <c r="O29" s="60"/>
     </row>
-    <row r="30" spans="3:15" ht="18" customHeight="1">
-      <c r="C30" s="40"/>
+    <row r="30" spans="2:15" ht="18" customHeight="1">
+      <c r="B30" s="39"/>
+      <c r="C30" s="38"/>
       <c r="D30" s="22"/>
       <c r="E30" s="18"/>
       <c r="F30" s="19"/>
@@ -46295,10 +46436,11 @@
       <c r="L30" s="21"/>
       <c r="M30" s="21"/>
       <c r="N30" s="21"/>
-      <c r="O30" s="26"/>
+      <c r="O30" s="59"/>
     </row>
-    <row r="31" spans="3:15" ht="18" customHeight="1">
-      <c r="C31" s="39"/>
+    <row r="31" spans="2:15" ht="18" customHeight="1">
+      <c r="B31" s="39"/>
+      <c r="C31" s="37"/>
       <c r="D31" s="17"/>
       <c r="E31" s="13"/>
       <c r="F31" s="14"/>
@@ -46310,10 +46452,11 @@
       <c r="L31" s="16"/>
       <c r="M31" s="16"/>
       <c r="N31" s="16"/>
-      <c r="O31" s="27"/>
+      <c r="O31" s="60"/>
     </row>
-    <row r="32" spans="3:15" ht="18" customHeight="1">
-      <c r="C32" s="40"/>
+    <row r="32" spans="2:15" ht="18" customHeight="1">
+      <c r="B32" s="39"/>
+      <c r="C32" s="38"/>
       <c r="D32" s="22"/>
       <c r="E32" s="18"/>
       <c r="F32" s="19"/>
@@ -46325,10 +46468,11 @@
       <c r="L32" s="21"/>
       <c r="M32" s="21"/>
       <c r="N32" s="21"/>
-      <c r="O32" s="26"/>
+      <c r="O32" s="59"/>
     </row>
-    <row r="33" spans="3:15" ht="18" customHeight="1">
-      <c r="C33" s="39"/>
+    <row r="33" spans="2:15" ht="18" customHeight="1">
+      <c r="B33" s="39"/>
+      <c r="C33" s="37"/>
       <c r="D33" s="17"/>
       <c r="E33" s="13"/>
       <c r="F33" s="14"/>
@@ -46340,10 +46484,11 @@
       <c r="L33" s="16"/>
       <c r="M33" s="16"/>
       <c r="N33" s="16"/>
-      <c r="O33" s="27"/>
+      <c r="O33" s="60"/>
     </row>
-    <row r="34" spans="3:15" ht="18" customHeight="1">
-      <c r="C34" s="40"/>
+    <row r="34" spans="2:15" ht="18" customHeight="1">
+      <c r="B34" s="39"/>
+      <c r="C34" s="38"/>
       <c r="D34" s="22"/>
       <c r="E34" s="18"/>
       <c r="F34" s="19"/>
@@ -46355,10 +46500,11 @@
       <c r="L34" s="21"/>
       <c r="M34" s="21"/>
       <c r="N34" s="21"/>
-      <c r="O34" s="26"/>
+      <c r="O34" s="59"/>
     </row>
-    <row r="35" spans="3:15" ht="18" customHeight="1">
-      <c r="C35" s="39"/>
+    <row r="35" spans="2:15" ht="18" customHeight="1">
+      <c r="B35" s="39"/>
+      <c r="C35" s="37"/>
       <c r="D35" s="17"/>
       <c r="E35" s="13"/>
       <c r="F35" s="14"/>
@@ -46370,10 +46516,11 @@
       <c r="L35" s="16"/>
       <c r="M35" s="16"/>
       <c r="N35" s="16"/>
-      <c r="O35" s="27"/>
+      <c r="O35" s="60"/>
     </row>
-    <row r="36" spans="3:15" ht="18" customHeight="1">
-      <c r="C36" s="40"/>
+    <row r="36" spans="2:15" ht="18" customHeight="1">
+      <c r="B36" s="39"/>
+      <c r="C36" s="38"/>
       <c r="D36" s="22"/>
       <c r="E36" s="18"/>
       <c r="F36" s="19"/>
@@ -46385,10 +46532,11 @@
       <c r="L36" s="21"/>
       <c r="M36" s="21"/>
       <c r="N36" s="21"/>
-      <c r="O36" s="26"/>
+      <c r="O36" s="59"/>
     </row>
-    <row r="37" spans="3:15" ht="18" customHeight="1">
-      <c r="C37" s="39"/>
+    <row r="37" spans="2:15" ht="18" customHeight="1">
+      <c r="B37" s="39"/>
+      <c r="C37" s="37"/>
       <c r="D37" s="17"/>
       <c r="E37" s="13"/>
       <c r="F37" s="14"/>
@@ -46400,25 +46548,27 @@
       <c r="L37" s="16"/>
       <c r="M37" s="16"/>
       <c r="N37" s="16"/>
-      <c r="O37" s="27"/>
+      <c r="O37" s="60"/>
     </row>
-    <row r="38" spans="3:15" ht="18" customHeight="1">
-      <c r="C38" s="38"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="30"/>
-      <c r="K38" s="37"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
-      <c r="N38" s="29"/>
-      <c r="O38" s="26"/>
+    <row r="38" spans="2:15" ht="18" customHeight="1">
+      <c r="B38" s="39"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="28"/>
+      <c r="K38" s="35"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="27"/>
+      <c r="N38" s="27"/>
+      <c r="O38" s="59"/>
     </row>
-    <row r="39" spans="3:15" ht="18" customHeight="1">
-      <c r="C39" s="39"/>
+    <row r="39" spans="2:15" ht="18" customHeight="1">
+      <c r="B39" s="39"/>
+      <c r="C39" s="37"/>
       <c r="D39" s="17"/>
       <c r="E39" s="13"/>
       <c r="F39" s="14"/>
@@ -46430,10 +46580,11 @@
       <c r="L39" s="16"/>
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
-      <c r="O39" s="27"/>
+      <c r="O39" s="60"/>
     </row>
-    <row r="40" spans="3:15" ht="18" customHeight="1">
-      <c r="C40" s="40"/>
+    <row r="40" spans="2:15" ht="18" customHeight="1">
+      <c r="B40" s="39"/>
+      <c r="C40" s="38"/>
       <c r="D40" s="22"/>
       <c r="E40" s="18"/>
       <c r="F40" s="19"/>
@@ -46445,10 +46596,11 @@
       <c r="L40" s="21"/>
       <c r="M40" s="21"/>
       <c r="N40" s="21"/>
-      <c r="O40" s="26"/>
+      <c r="O40" s="59"/>
     </row>
-    <row r="41" spans="3:15" ht="18" customHeight="1">
-      <c r="C41" s="39"/>
+    <row r="41" spans="2:15" ht="18" customHeight="1">
+      <c r="B41" s="39"/>
+      <c r="C41" s="37"/>
       <c r="D41" s="17"/>
       <c r="E41" s="13"/>
       <c r="F41" s="14"/>
@@ -46460,10 +46612,11 @@
       <c r="L41" s="16"/>
       <c r="M41" s="16"/>
       <c r="N41" s="16"/>
-      <c r="O41" s="27"/>
+      <c r="O41" s="60"/>
     </row>
-    <row r="42" spans="3:15" ht="18" customHeight="1">
-      <c r="C42" s="40"/>
+    <row r="42" spans="2:15" ht="18" customHeight="1">
+      <c r="B42" s="39"/>
+      <c r="C42" s="38"/>
       <c r="D42" s="22"/>
       <c r="E42" s="18"/>
       <c r="F42" s="19"/>
@@ -46475,10 +46628,11 @@
       <c r="L42" s="21"/>
       <c r="M42" s="21"/>
       <c r="N42" s="21"/>
-      <c r="O42" s="26"/>
+      <c r="O42" s="59"/>
     </row>
-    <row r="43" spans="3:15" ht="18" customHeight="1">
-      <c r="C43" s="39"/>
+    <row r="43" spans="2:15" ht="18" customHeight="1">
+      <c r="B43" s="39"/>
+      <c r="C43" s="37"/>
       <c r="D43" s="17"/>
       <c r="E43" s="13"/>
       <c r="F43" s="14"/>
@@ -46490,10 +46644,11 @@
       <c r="L43" s="16"/>
       <c r="M43" s="16"/>
       <c r="N43" s="16"/>
-      <c r="O43" s="27"/>
+      <c r="O43" s="60"/>
     </row>
-    <row r="44" spans="3:15" ht="18" customHeight="1">
-      <c r="C44" s="40"/>
+    <row r="44" spans="2:15" ht="18" customHeight="1">
+      <c r="B44" s="39"/>
+      <c r="C44" s="38"/>
       <c r="D44" s="22"/>
       <c r="E44" s="18"/>
       <c r="F44" s="19"/>
@@ -46505,10 +46660,11 @@
       <c r="L44" s="21"/>
       <c r="M44" s="21"/>
       <c r="N44" s="21"/>
-      <c r="O44" s="26"/>
+      <c r="O44" s="59"/>
     </row>
-    <row r="45" spans="3:15" ht="18" customHeight="1">
-      <c r="C45" s="39"/>
+    <row r="45" spans="2:15" ht="18" customHeight="1">
+      <c r="B45" s="39"/>
+      <c r="C45" s="37"/>
       <c r="D45" s="17"/>
       <c r="E45" s="13"/>
       <c r="F45" s="14"/>
@@ -46520,10 +46676,11 @@
       <c r="L45" s="16"/>
       <c r="M45" s="16"/>
       <c r="N45" s="16"/>
-      <c r="O45" s="27"/>
+      <c r="O45" s="60"/>
     </row>
-    <row r="46" spans="3:15" ht="18" customHeight="1">
-      <c r="C46" s="40"/>
+    <row r="46" spans="2:15" ht="18" customHeight="1">
+      <c r="B46" s="39"/>
+      <c r="C46" s="38"/>
       <c r="D46" s="22"/>
       <c r="E46" s="18"/>
       <c r="F46" s="19"/>
@@ -46535,10 +46692,11 @@
       <c r="L46" s="21"/>
       <c r="M46" s="21"/>
       <c r="N46" s="21"/>
-      <c r="O46" s="26"/>
+      <c r="O46" s="59"/>
     </row>
-    <row r="47" spans="3:15" ht="18" customHeight="1">
-      <c r="C47" s="39"/>
+    <row r="47" spans="2:15" ht="18" customHeight="1">
+      <c r="B47" s="39"/>
+      <c r="C47" s="37"/>
       <c r="D47" s="17"/>
       <c r="E47" s="13"/>
       <c r="F47" s="14"/>
@@ -46550,10 +46708,11 @@
       <c r="L47" s="16"/>
       <c r="M47" s="16"/>
       <c r="N47" s="16"/>
-      <c r="O47" s="27"/>
+      <c r="O47" s="60"/>
     </row>
-    <row r="48" spans="3:15" ht="18" customHeight="1">
-      <c r="C48" s="40"/>
+    <row r="48" spans="2:15" ht="18" customHeight="1">
+      <c r="B48" s="39"/>
+      <c r="C48" s="38"/>
       <c r="D48" s="22"/>
       <c r="E48" s="18"/>
       <c r="F48" s="19"/>
@@ -46565,10 +46724,11 @@
       <c r="L48" s="21"/>
       <c r="M48" s="21"/>
       <c r="N48" s="21"/>
-      <c r="O48" s="26"/>
+      <c r="O48" s="59"/>
     </row>
-    <row r="49" spans="3:15" ht="18" customHeight="1">
-      <c r="C49" s="39"/>
+    <row r="49" spans="2:15" ht="18" customHeight="1">
+      <c r="B49" s="39"/>
+      <c r="C49" s="37"/>
       <c r="D49" s="17"/>
       <c r="E49" s="13"/>
       <c r="F49" s="14"/>
@@ -46580,10 +46740,11 @@
       <c r="L49" s="16"/>
       <c r="M49" s="16"/>
       <c r="N49" s="16"/>
-      <c r="O49" s="27"/>
+      <c r="O49" s="60"/>
     </row>
-    <row r="50" spans="3:15" ht="18" customHeight="1">
-      <c r="C50" s="40"/>
+    <row r="50" spans="2:15" ht="18" customHeight="1">
+      <c r="B50" s="39"/>
+      <c r="C50" s="38"/>
       <c r="D50" s="22"/>
       <c r="E50" s="18"/>
       <c r="F50" s="19"/>
@@ -46595,10 +46756,11 @@
       <c r="L50" s="21"/>
       <c r="M50" s="21"/>
       <c r="N50" s="21"/>
-      <c r="O50" s="26"/>
+      <c r="O50" s="59"/>
     </row>
-    <row r="51" spans="3:15" ht="18" customHeight="1">
-      <c r="C51" s="39"/>
+    <row r="51" spans="2:15" ht="18" customHeight="1">
+      <c r="B51" s="39"/>
+      <c r="C51" s="37"/>
       <c r="D51" s="17"/>
       <c r="E51" s="13"/>
       <c r="F51" s="14"/>
@@ -46610,10 +46772,11 @@
       <c r="L51" s="16"/>
       <c r="M51" s="16"/>
       <c r="N51" s="16"/>
-      <c r="O51" s="27"/>
+      <c r="O51" s="60"/>
     </row>
-    <row r="52" spans="3:15" ht="18" customHeight="1">
-      <c r="C52" s="40"/>
+    <row r="52" spans="2:15" ht="18" customHeight="1">
+      <c r="B52" s="39"/>
+      <c r="C52" s="38"/>
       <c r="D52" s="22"/>
       <c r="E52" s="18"/>
       <c r="F52" s="19"/>
@@ -46625,10 +46788,11 @@
       <c r="L52" s="21"/>
       <c r="M52" s="21"/>
       <c r="N52" s="21"/>
-      <c r="O52" s="26"/>
+      <c r="O52" s="59"/>
     </row>
-    <row r="53" spans="3:15" ht="18" customHeight="1">
-      <c r="C53" s="39"/>
+    <row r="53" spans="2:15" ht="18" customHeight="1">
+      <c r="B53" s="39"/>
+      <c r="C53" s="37"/>
       <c r="D53" s="17"/>
       <c r="E53" s="13"/>
       <c r="F53" s="14"/>
@@ -46640,10 +46804,11 @@
       <c r="L53" s="16"/>
       <c r="M53" s="16"/>
       <c r="N53" s="16"/>
-      <c r="O53" s="27"/>
+      <c r="O53" s="60"/>
     </row>
-    <row r="54" spans="3:15" ht="18" customHeight="1">
-      <c r="C54" s="40"/>
+    <row r="54" spans="2:15" ht="18" customHeight="1">
+      <c r="B54" s="39"/>
+      <c r="C54" s="38"/>
       <c r="D54" s="22"/>
       <c r="E54" s="18"/>
       <c r="F54" s="19"/>
@@ -46655,10 +46820,11 @@
       <c r="L54" s="21"/>
       <c r="M54" s="21"/>
       <c r="N54" s="21"/>
-      <c r="O54" s="26"/>
+      <c r="O54" s="59"/>
     </row>
-    <row r="55" spans="3:15" ht="18" customHeight="1">
-      <c r="C55" s="39"/>
+    <row r="55" spans="2:15" ht="18" customHeight="1">
+      <c r="B55" s="39"/>
+      <c r="C55" s="37"/>
       <c r="D55" s="17"/>
       <c r="E55" s="13"/>
       <c r="F55" s="14"/>
@@ -46670,10 +46836,11 @@
       <c r="L55" s="16"/>
       <c r="M55" s="16"/>
       <c r="N55" s="16"/>
-      <c r="O55" s="27"/>
+      <c r="O55" s="60"/>
     </row>
-    <row r="56" spans="3:15" ht="18" customHeight="1">
-      <c r="C56" s="40"/>
+    <row r="56" spans="2:15" ht="18" customHeight="1">
+      <c r="B56" s="39"/>
+      <c r="C56" s="38"/>
       <c r="D56" s="22"/>
       <c r="E56" s="18"/>
       <c r="F56" s="19"/>
@@ -46685,10 +46852,11 @@
       <c r="L56" s="21"/>
       <c r="M56" s="21"/>
       <c r="N56" s="21"/>
-      <c r="O56" s="26"/>
+      <c r="O56" s="59"/>
     </row>
-    <row r="57" spans="3:15" ht="18" customHeight="1">
-      <c r="C57" s="39"/>
+    <row r="57" spans="2:15" ht="18" customHeight="1">
+      <c r="B57" s="39"/>
+      <c r="C57" s="37"/>
       <c r="D57" s="17"/>
       <c r="E57" s="13"/>
       <c r="F57" s="14"/>
@@ -46700,10 +46868,11 @@
       <c r="L57" s="16"/>
       <c r="M57" s="16"/>
       <c r="N57" s="16"/>
-      <c r="O57" s="27"/>
+      <c r="O57" s="60"/>
     </row>
-    <row r="58" spans="3:15" ht="18" customHeight="1">
-      <c r="C58" s="40"/>
+    <row r="58" spans="2:15" ht="18" customHeight="1">
+      <c r="B58" s="39"/>
+      <c r="C58" s="38"/>
       <c r="D58" s="22"/>
       <c r="E58" s="18"/>
       <c r="F58" s="19"/>
@@ -46715,10 +46884,11 @@
       <c r="L58" s="21"/>
       <c r="M58" s="21"/>
       <c r="N58" s="21"/>
-      <c r="O58" s="26"/>
+      <c r="O58" s="59"/>
     </row>
-    <row r="59" spans="3:15" ht="18" customHeight="1">
-      <c r="C59" s="39"/>
+    <row r="59" spans="2:15" ht="18" customHeight="1">
+      <c r="B59" s="39"/>
+      <c r="C59" s="37"/>
       <c r="D59" s="17"/>
       <c r="E59" s="13"/>
       <c r="F59" s="14"/>
@@ -46730,10 +46900,11 @@
       <c r="L59" s="16"/>
       <c r="M59" s="16"/>
       <c r="N59" s="16"/>
-      <c r="O59" s="27"/>
+      <c r="O59" s="60"/>
     </row>
-    <row r="60" spans="3:15" ht="18" customHeight="1">
-      <c r="C60" s="40"/>
+    <row r="60" spans="2:15" ht="18" customHeight="1">
+      <c r="B60" s="39"/>
+      <c r="C60" s="38"/>
       <c r="D60" s="22"/>
       <c r="E60" s="18"/>
       <c r="F60" s="19"/>
@@ -46745,10 +46916,11 @@
       <c r="L60" s="21"/>
       <c r="M60" s="21"/>
       <c r="N60" s="21"/>
-      <c r="O60" s="26"/>
+      <c r="O60" s="59"/>
     </row>
-    <row r="61" spans="3:15" ht="18" customHeight="1">
-      <c r="C61" s="39"/>
+    <row r="61" spans="2:15" ht="18" customHeight="1">
+      <c r="B61" s="39"/>
+      <c r="C61" s="37"/>
       <c r="D61" s="17"/>
       <c r="E61" s="13"/>
       <c r="F61" s="14"/>
@@ -46760,10 +46932,11 @@
       <c r="L61" s="16"/>
       <c r="M61" s="16"/>
       <c r="N61" s="16"/>
-      <c r="O61" s="27"/>
+      <c r="O61" s="60"/>
     </row>
-    <row r="62" spans="3:15" ht="18" customHeight="1">
-      <c r="C62" s="40"/>
+    <row r="62" spans="2:15" ht="18" customHeight="1">
+      <c r="B62" s="39"/>
+      <c r="C62" s="38"/>
       <c r="D62" s="22"/>
       <c r="E62" s="18"/>
       <c r="F62" s="19"/>
@@ -46775,10 +46948,11 @@
       <c r="L62" s="21"/>
       <c r="M62" s="21"/>
       <c r="N62" s="21"/>
-      <c r="O62" s="26"/>
+      <c r="O62" s="59"/>
     </row>
-    <row r="63" spans="3:15" ht="18" customHeight="1">
-      <c r="C63" s="39"/>
+    <row r="63" spans="2:15" ht="18" customHeight="1">
+      <c r="B63" s="39"/>
+      <c r="C63" s="37"/>
       <c r="D63" s="17"/>
       <c r="E63" s="13"/>
       <c r="F63" s="14"/>
@@ -46790,10 +46964,11 @@
       <c r="L63" s="16"/>
       <c r="M63" s="16"/>
       <c r="N63" s="16"/>
-      <c r="O63" s="27"/>
+      <c r="O63" s="60"/>
     </row>
-    <row r="64" spans="3:15" ht="18" customHeight="1">
-      <c r="C64" s="40"/>
+    <row r="64" spans="2:15" ht="18" customHeight="1">
+      <c r="B64" s="39"/>
+      <c r="C64" s="38"/>
       <c r="D64" s="22"/>
       <c r="E64" s="18"/>
       <c r="F64" s="19"/>
@@ -46805,10 +46980,11 @@
       <c r="L64" s="21"/>
       <c r="M64" s="21"/>
       <c r="N64" s="21"/>
-      <c r="O64" s="26"/>
+      <c r="O64" s="59"/>
     </row>
-    <row r="65" spans="3:15" ht="18" customHeight="1">
-      <c r="C65" s="39"/>
+    <row r="65" spans="2:15" ht="18" customHeight="1">
+      <c r="B65" s="39"/>
+      <c r="C65" s="37"/>
       <c r="D65" s="17"/>
       <c r="E65" s="13"/>
       <c r="F65" s="14"/>
@@ -46820,10 +46996,11 @@
       <c r="L65" s="16"/>
       <c r="M65" s="16"/>
       <c r="N65" s="16"/>
-      <c r="O65" s="27"/>
+      <c r="O65" s="60"/>
     </row>
-    <row r="66" spans="3:15" ht="18" customHeight="1">
-      <c r="C66" s="40"/>
+    <row r="66" spans="2:15" ht="18" customHeight="1">
+      <c r="B66" s="39"/>
+      <c r="C66" s="38"/>
       <c r="D66" s="22"/>
       <c r="E66" s="18"/>
       <c r="F66" s="19"/>
@@ -46835,23 +47012,25 @@
       <c r="L66" s="21"/>
       <c r="M66" s="21"/>
       <c r="N66" s="21"/>
-      <c r="O66" s="26"/>
+      <c r="O66" s="59"/>
     </row>
-    <row r="67" spans="3:15" ht="18" customHeight="1">
-      <c r="C67" s="39"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="15"/>
-      <c r="H67" s="16"/>
-      <c r="I67" s="16"/>
-      <c r="J67" s="17"/>
-      <c r="K67" s="13"/>
-      <c r="L67" s="16"/>
-      <c r="M67" s="16"/>
-      <c r="N67" s="16"/>
-      <c r="O67" s="27"/>
+    <row r="67" spans="2:15" ht="18" customHeight="1" thickBot="1">
+      <c r="B67" s="39"/>
+      <c r="C67" s="61"/>
+      <c r="D67" s="62"/>
+      <c r="E67" s="63"/>
+      <c r="F67" s="64"/>
+      <c r="G67" s="65"/>
+      <c r="H67" s="66"/>
+      <c r="I67" s="66"/>
+      <c r="J67" s="62"/>
+      <c r="K67" s="63"/>
+      <c r="L67" s="66"/>
+      <c r="M67" s="66"/>
+      <c r="N67" s="66"/>
+      <c r="O67" s="67"/>
     </row>
+    <row r="68" spans="2:15" ht="12.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="C3:D3"/>
@@ -46865,11 +47044,10 @@
     <mergeCell ref="M4:N4"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="55" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="56" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;10日通システム株式会社 &amp;C&amp;"ＭＳ ゴシック,Regular"&amp;16標準報酬月額表（厚生年金）&amp;R&amp;"ＭＳ ゴシック,Regular"&amp;10&amp;KFF0000 &amp;K01+000&amp;D　&amp;T　
 &amp;KFF0000 &amp;K01+000page&amp;P</oddHeader>
   </headerFooter>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[SMAL] QMM008 fixed templte
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_標準報酬月額表（厚生年金).xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_標準報酬月額表（厚生年金).xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="マスタリスト" sheetId="11" r:id="rId1"/>
-    <sheet name="マスタリスト (2)" sheetId="21" r:id="rId2"/>
+    <sheet name="マスタリスト (2)" sheetId="22" r:id="rId2"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
@@ -955,7 +955,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1035,9 +1035,6 @@
     <xf numFmtId="40" fontId="4" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="40" fontId="4" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="40" fontId="4" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1051,9 +1048,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="40" fontId="4" fillId="3" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="4" fillId="3" borderId="20" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="40" fontId="4" fillId="3" borderId="21" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1071,9 +1065,6 @@
     <xf numFmtId="40" fontId="4" fillId="0" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="40" fontId="4" fillId="0" borderId="20" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="40" fontId="4" fillId="0" borderId="21" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1089,16 +1080,10 @@
     <xf numFmtId="40" fontId="4" fillId="0" borderId="30" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="40" fontId="4" fillId="0" borderId="31" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="40" fontId="4" fillId="3" borderId="36" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="40" fontId="4" fillId="3" borderId="37" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="4" fillId="3" borderId="38" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="40" fontId="4" fillId="3" borderId="39" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1148,6 +1133,48 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="3" borderId="18" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="3" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="3" borderId="20" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="18" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="20" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="30" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="31" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="3" borderId="36" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="3" borderId="37" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="4" fillId="3" borderId="38" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -44784,27 +44811,27 @@
     </row>
     <row r="3" spans="2:15" ht="18" customHeight="1" thickTop="1">
       <c r="B3" s="19"/>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="54"/>
-      <c r="E3" s="55" t="s">
+      <c r="D3" s="49"/>
+      <c r="E3" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="57" t="s">
+      <c r="F3" s="51"/>
+      <c r="G3" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="57" t="s">
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="52" t="s">
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="47" t="s">
         <v>8</v>
       </c>
     </row>
@@ -44814,23 +44841,23 @@
       <c r="D4" s="11"/>
       <c r="E4" s="12"/>
       <c r="F4" s="13"/>
-      <c r="G4" s="61" t="s">
+      <c r="G4" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="62"/>
-      <c r="I4" s="63" t="s">
+      <c r="H4" s="57"/>
+      <c r="I4" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="64"/>
-      <c r="K4" s="61" t="s">
+      <c r="J4" s="59"/>
+      <c r="K4" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="62"/>
-      <c r="M4" s="63" t="s">
+      <c r="L4" s="57"/>
+      <c r="M4" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="64"/>
-      <c r="O4" s="52"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="47"/>
     </row>
     <row r="5" spans="2:15" ht="18" customHeight="1" thickBot="1">
       <c r="B5" s="19"/>
@@ -44870,999 +44897,999 @@
       <c r="N5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="52"/>
+      <c r="O5" s="47"/>
     </row>
     <row r="6" spans="2:15" ht="18" customHeight="1" thickTop="1">
       <c r="B6" s="19"/>
       <c r="C6" s="16"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
       <c r="J6" s="25"/>
       <c r="K6" s="26"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="30"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="29"/>
     </row>
     <row r="7" spans="2:15" ht="18" customHeight="1">
       <c r="B7" s="19"/>
       <c r="C7" s="17"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="36"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="34"/>
     </row>
     <row r="8" spans="2:15" ht="18" customHeight="1">
       <c r="B8" s="19"/>
       <c r="C8" s="18"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="30"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="29"/>
     </row>
     <row r="9" spans="2:15" ht="18" customHeight="1">
       <c r="B9" s="19"/>
       <c r="C9" s="17"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="36"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="34"/>
     </row>
     <row r="10" spans="2:15" ht="18" customHeight="1">
       <c r="B10" s="19"/>
       <c r="C10" s="18"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="42"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="39"/>
     </row>
     <row r="11" spans="2:15" ht="18" customHeight="1">
       <c r="B11" s="19"/>
       <c r="C11" s="17"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="43"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="40"/>
     </row>
     <row r="12" spans="2:15" ht="18" customHeight="1">
       <c r="B12" s="19"/>
       <c r="C12" s="18"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="42"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="39"/>
     </row>
     <row r="13" spans="2:15" ht="18" customHeight="1">
       <c r="B13" s="19"/>
       <c r="C13" s="17"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="43"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="40"/>
     </row>
     <row r="14" spans="2:15" ht="18" customHeight="1">
       <c r="B14" s="19"/>
       <c r="C14" s="18"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="42"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="39"/>
     </row>
     <row r="15" spans="2:15" ht="18" customHeight="1">
       <c r="B15" s="19"/>
       <c r="C15" s="17"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="43"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="33"/>
+      <c r="O15" s="40"/>
     </row>
     <row r="16" spans="2:15" ht="18" customHeight="1">
       <c r="B16" s="19"/>
       <c r="C16" s="18"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="41"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="41"/>
-      <c r="O16" s="42"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="39"/>
     </row>
     <row r="17" spans="2:15" ht="18" customHeight="1">
       <c r="B17" s="19"/>
       <c r="C17" s="17"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="43"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="33"/>
+      <c r="O17" s="40"/>
     </row>
     <row r="18" spans="2:15" ht="18" customHeight="1">
       <c r="B18" s="19"/>
       <c r="C18" s="18"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="38"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="42"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="39"/>
     </row>
     <row r="19" spans="2:15" ht="18" customHeight="1">
       <c r="B19" s="19"/>
       <c r="C19" s="17"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="43"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
+      <c r="O19" s="40"/>
     </row>
     <row r="20" spans="2:15" ht="18" customHeight="1">
       <c r="B20" s="19"/>
       <c r="C20" s="18"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="42"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="39"/>
     </row>
     <row r="21" spans="2:15" ht="18" customHeight="1">
       <c r="B21" s="19"/>
       <c r="C21" s="17"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="35"/>
-      <c r="O21" s="43"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
+      <c r="O21" s="40"/>
     </row>
     <row r="22" spans="2:15" ht="18" customHeight="1">
       <c r="B22" s="19"/>
       <c r="C22" s="18"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="41"/>
-      <c r="O22" s="42"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="39"/>
     </row>
     <row r="23" spans="2:15" ht="18" customHeight="1">
       <c r="B23" s="19"/>
       <c r="C23" s="17"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="35"/>
-      <c r="O23" s="43"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="33"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="33"/>
+      <c r="O23" s="40"/>
     </row>
     <row r="24" spans="2:15" ht="18" customHeight="1">
       <c r="B24" s="19"/>
       <c r="C24" s="18"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="38"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="41"/>
-      <c r="N24" s="41"/>
-      <c r="O24" s="42"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="39"/>
     </row>
     <row r="25" spans="2:15" ht="18" customHeight="1">
       <c r="B25" s="19"/>
       <c r="C25" s="17"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="35"/>
-      <c r="O25" s="43"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="40"/>
     </row>
     <row r="26" spans="2:15" ht="18" customHeight="1">
       <c r="B26" s="19"/>
       <c r="C26" s="18"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="41"/>
-      <c r="M26" s="41"/>
-      <c r="N26" s="41"/>
-      <c r="O26" s="42"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="39"/>
     </row>
     <row r="27" spans="2:15" ht="18" customHeight="1">
       <c r="B27" s="19"/>
       <c r="C27" s="17"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="35"/>
-      <c r="M27" s="35"/>
-      <c r="N27" s="35"/>
-      <c r="O27" s="43"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="33"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="33"/>
+      <c r="O27" s="40"/>
     </row>
     <row r="28" spans="2:15" ht="18" customHeight="1">
       <c r="B28" s="19"/>
       <c r="C28" s="18"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="41"/>
-      <c r="M28" s="41"/>
-      <c r="N28" s="41"/>
-      <c r="O28" s="42"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="38"/>
+      <c r="O28" s="39"/>
     </row>
     <row r="29" spans="2:15" ht="18" customHeight="1">
       <c r="B29" s="19"/>
       <c r="C29" s="17"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="35"/>
-      <c r="M29" s="35"/>
-      <c r="N29" s="35"/>
-      <c r="O29" s="43"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="33"/>
+      <c r="O29" s="40"/>
     </row>
     <row r="30" spans="2:15" ht="18" customHeight="1">
       <c r="B30" s="19"/>
       <c r="C30" s="18"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="41"/>
-      <c r="M30" s="41"/>
-      <c r="N30" s="41"/>
-      <c r="O30" s="42"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="68"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="39"/>
     </row>
     <row r="31" spans="2:15" ht="18" customHeight="1">
       <c r="B31" s="19"/>
       <c r="C31" s="17"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="35"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="35"/>
-      <c r="M31" s="35"/>
-      <c r="N31" s="35"/>
-      <c r="O31" s="43"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="33"/>
+      <c r="N31" s="33"/>
+      <c r="O31" s="40"/>
     </row>
     <row r="32" spans="2:15" ht="18" customHeight="1">
       <c r="B32" s="19"/>
       <c r="C32" s="18"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="38"/>
-      <c r="L32" s="41"/>
-      <c r="M32" s="41"/>
-      <c r="N32" s="41"/>
-      <c r="O32" s="42"/>
+      <c r="D32" s="66"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="68"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="38"/>
+      <c r="M32" s="38"/>
+      <c r="N32" s="38"/>
+      <c r="O32" s="39"/>
     </row>
     <row r="33" spans="2:15" ht="18" customHeight="1">
       <c r="B33" s="19"/>
       <c r="C33" s="17"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="35"/>
-      <c r="I33" s="35"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="35"/>
-      <c r="M33" s="35"/>
-      <c r="N33" s="35"/>
-      <c r="O33" s="43"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="31"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
+      <c r="N33" s="33"/>
+      <c r="O33" s="40"/>
     </row>
     <row r="34" spans="2:15" ht="18" customHeight="1">
       <c r="B34" s="19"/>
       <c r="C34" s="18"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="41"/>
-      <c r="I34" s="41"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="38"/>
-      <c r="L34" s="41"/>
-      <c r="M34" s="41"/>
-      <c r="N34" s="41"/>
-      <c r="O34" s="42"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="36"/>
+      <c r="L34" s="38"/>
+      <c r="M34" s="38"/>
+      <c r="N34" s="38"/>
+      <c r="O34" s="39"/>
     </row>
     <row r="35" spans="2:15" ht="18" customHeight="1">
       <c r="B35" s="19"/>
       <c r="C35" s="17"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="35"/>
-      <c r="I35" s="35"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="35"/>
-      <c r="M35" s="35"/>
-      <c r="N35" s="35"/>
-      <c r="O35" s="43"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="31"/>
+      <c r="L35" s="33"/>
+      <c r="M35" s="33"/>
+      <c r="N35" s="33"/>
+      <c r="O35" s="40"/>
     </row>
     <row r="36" spans="2:15" ht="18" customHeight="1">
       <c r="B36" s="19"/>
       <c r="C36" s="18"/>
-      <c r="D36" s="37"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="41"/>
-      <c r="J36" s="37"/>
-      <c r="K36" s="38"/>
-      <c r="L36" s="41"/>
-      <c r="M36" s="41"/>
-      <c r="N36" s="41"/>
-      <c r="O36" s="42"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="68"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="38"/>
+      <c r="M36" s="38"/>
+      <c r="N36" s="38"/>
+      <c r="O36" s="39"/>
     </row>
     <row r="37" spans="2:15" ht="18" customHeight="1">
       <c r="B37" s="19"/>
       <c r="C37" s="17"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="32"/>
-      <c r="L37" s="35"/>
-      <c r="M37" s="35"/>
-      <c r="N37" s="35"/>
-      <c r="O37" s="43"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="30"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="33"/>
+      <c r="M37" s="33"/>
+      <c r="N37" s="33"/>
+      <c r="O37" s="40"/>
     </row>
     <row r="38" spans="2:15" ht="18" customHeight="1">
       <c r="B38" s="19"/>
       <c r="C38" s="16"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="45"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28"/>
       <c r="J38" s="25"/>
-      <c r="K38" s="44"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
-      <c r="N38" s="29"/>
-      <c r="O38" s="42"/>
+      <c r="K38" s="41"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="28"/>
+      <c r="N38" s="28"/>
+      <c r="O38" s="39"/>
     </row>
     <row r="39" spans="2:15" ht="18" customHeight="1">
       <c r="B39" s="19"/>
       <c r="C39" s="17"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="35"/>
-      <c r="I39" s="35"/>
-      <c r="J39" s="31"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="35"/>
-      <c r="M39" s="35"/>
-      <c r="N39" s="35"/>
-      <c r="O39" s="43"/>
+      <c r="D39" s="63"/>
+      <c r="E39" s="64"/>
+      <c r="F39" s="65"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="30"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="33"/>
+      <c r="M39" s="33"/>
+      <c r="N39" s="33"/>
+      <c r="O39" s="40"/>
     </row>
     <row r="40" spans="2:15" ht="18" customHeight="1">
       <c r="B40" s="19"/>
       <c r="C40" s="18"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="40"/>
-      <c r="H40" s="41"/>
-      <c r="I40" s="41"/>
-      <c r="J40" s="37"/>
-      <c r="K40" s="38"/>
-      <c r="L40" s="41"/>
-      <c r="M40" s="41"/>
-      <c r="N40" s="41"/>
-      <c r="O40" s="42"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="67"/>
+      <c r="F40" s="68"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="36"/>
+      <c r="L40" s="38"/>
+      <c r="M40" s="38"/>
+      <c r="N40" s="38"/>
+      <c r="O40" s="39"/>
     </row>
     <row r="41" spans="2:15" ht="18" customHeight="1">
       <c r="B41" s="19"/>
       <c r="C41" s="17"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="34"/>
-      <c r="H41" s="35"/>
-      <c r="I41" s="35"/>
-      <c r="J41" s="31"/>
-      <c r="K41" s="32"/>
-      <c r="L41" s="35"/>
-      <c r="M41" s="35"/>
-      <c r="N41" s="35"/>
-      <c r="O41" s="43"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="64"/>
+      <c r="F41" s="65"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="33"/>
+      <c r="J41" s="30"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="33"/>
+      <c r="M41" s="33"/>
+      <c r="N41" s="33"/>
+      <c r="O41" s="40"/>
     </row>
     <row r="42" spans="2:15" ht="18" customHeight="1">
       <c r="B42" s="19"/>
       <c r="C42" s="18"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="41"/>
-      <c r="I42" s="41"/>
-      <c r="J42" s="37"/>
-      <c r="K42" s="38"/>
-      <c r="L42" s="41"/>
-      <c r="M42" s="41"/>
-      <c r="N42" s="41"/>
-      <c r="O42" s="42"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="67"/>
+      <c r="F42" s="68"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="36"/>
+      <c r="L42" s="38"/>
+      <c r="M42" s="38"/>
+      <c r="N42" s="38"/>
+      <c r="O42" s="39"/>
     </row>
     <row r="43" spans="2:15" ht="18" customHeight="1">
       <c r="B43" s="19"/>
       <c r="C43" s="17"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="31"/>
-      <c r="K43" s="32"/>
-      <c r="L43" s="35"/>
-      <c r="M43" s="35"/>
-      <c r="N43" s="35"/>
-      <c r="O43" s="43"/>
+      <c r="D43" s="63"/>
+      <c r="E43" s="64"/>
+      <c r="F43" s="65"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="30"/>
+      <c r="K43" s="31"/>
+      <c r="L43" s="33"/>
+      <c r="M43" s="33"/>
+      <c r="N43" s="33"/>
+      <c r="O43" s="40"/>
     </row>
     <row r="44" spans="2:15" ht="18" customHeight="1">
       <c r="B44" s="19"/>
       <c r="C44" s="18"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="40"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="37"/>
-      <c r="K44" s="38"/>
-      <c r="L44" s="41"/>
-      <c r="M44" s="41"/>
-      <c r="N44" s="41"/>
-      <c r="O44" s="42"/>
+      <c r="D44" s="66"/>
+      <c r="E44" s="67"/>
+      <c r="F44" s="68"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="35"/>
+      <c r="K44" s="36"/>
+      <c r="L44" s="38"/>
+      <c r="M44" s="38"/>
+      <c r="N44" s="38"/>
+      <c r="O44" s="39"/>
     </row>
     <row r="45" spans="2:15" ht="18" customHeight="1">
       <c r="B45" s="19"/>
       <c r="C45" s="17"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="34"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="31"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="35"/>
-      <c r="M45" s="35"/>
-      <c r="N45" s="35"/>
-      <c r="O45" s="43"/>
+      <c r="D45" s="63"/>
+      <c r="E45" s="64"/>
+      <c r="F45" s="65"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="30"/>
+      <c r="K45" s="31"/>
+      <c r="L45" s="33"/>
+      <c r="M45" s="33"/>
+      <c r="N45" s="33"/>
+      <c r="O45" s="40"/>
     </row>
     <row r="46" spans="2:15" ht="18" customHeight="1">
       <c r="B46" s="19"/>
       <c r="C46" s="18"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="39"/>
-      <c r="G46" s="40"/>
-      <c r="H46" s="41"/>
-      <c r="I46" s="41"/>
-      <c r="J46" s="37"/>
-      <c r="K46" s="38"/>
-      <c r="L46" s="41"/>
-      <c r="M46" s="41"/>
-      <c r="N46" s="41"/>
-      <c r="O46" s="42"/>
+      <c r="D46" s="66"/>
+      <c r="E46" s="67"/>
+      <c r="F46" s="68"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="36"/>
+      <c r="L46" s="38"/>
+      <c r="M46" s="38"/>
+      <c r="N46" s="38"/>
+      <c r="O46" s="39"/>
     </row>
     <row r="47" spans="2:15" ht="18" customHeight="1">
       <c r="B47" s="19"/>
       <c r="C47" s="17"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="34"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="35"/>
-      <c r="J47" s="31"/>
-      <c r="K47" s="32"/>
-      <c r="L47" s="35"/>
-      <c r="M47" s="35"/>
-      <c r="N47" s="35"/>
-      <c r="O47" s="43"/>
+      <c r="D47" s="63"/>
+      <c r="E47" s="64"/>
+      <c r="F47" s="65"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="33"/>
+      <c r="I47" s="33"/>
+      <c r="J47" s="30"/>
+      <c r="K47" s="31"/>
+      <c r="L47" s="33"/>
+      <c r="M47" s="33"/>
+      <c r="N47" s="33"/>
+      <c r="O47" s="40"/>
     </row>
     <row r="48" spans="2:15" ht="18" customHeight="1">
       <c r="B48" s="19"/>
       <c r="C48" s="18"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="38"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="40"/>
-      <c r="H48" s="41"/>
-      <c r="I48" s="41"/>
-      <c r="J48" s="37"/>
-      <c r="K48" s="38"/>
-      <c r="L48" s="41"/>
-      <c r="M48" s="41"/>
-      <c r="N48" s="41"/>
-      <c r="O48" s="42"/>
+      <c r="D48" s="66"/>
+      <c r="E48" s="67"/>
+      <c r="F48" s="68"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="38"/>
+      <c r="I48" s="38"/>
+      <c r="J48" s="35"/>
+      <c r="K48" s="36"/>
+      <c r="L48" s="38"/>
+      <c r="M48" s="38"/>
+      <c r="N48" s="38"/>
+      <c r="O48" s="39"/>
     </row>
     <row r="49" spans="2:15" ht="18" customHeight="1">
       <c r="B49" s="19"/>
       <c r="C49" s="17"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="33"/>
-      <c r="G49" s="34"/>
-      <c r="H49" s="35"/>
-      <c r="I49" s="35"/>
-      <c r="J49" s="31"/>
-      <c r="K49" s="32"/>
-      <c r="L49" s="35"/>
-      <c r="M49" s="35"/>
-      <c r="N49" s="35"/>
-      <c r="O49" s="43"/>
+      <c r="D49" s="63"/>
+      <c r="E49" s="64"/>
+      <c r="F49" s="65"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="33"/>
+      <c r="I49" s="33"/>
+      <c r="J49" s="30"/>
+      <c r="K49" s="31"/>
+      <c r="L49" s="33"/>
+      <c r="M49" s="33"/>
+      <c r="N49" s="33"/>
+      <c r="O49" s="40"/>
     </row>
     <row r="50" spans="2:15" ht="18" customHeight="1">
       <c r="B50" s="19"/>
       <c r="C50" s="18"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="38"/>
-      <c r="F50" s="39"/>
-      <c r="G50" s="40"/>
-      <c r="H50" s="41"/>
-      <c r="I50" s="41"/>
-      <c r="J50" s="37"/>
-      <c r="K50" s="38"/>
-      <c r="L50" s="41"/>
-      <c r="M50" s="41"/>
-      <c r="N50" s="41"/>
-      <c r="O50" s="42"/>
+      <c r="D50" s="66"/>
+      <c r="E50" s="67"/>
+      <c r="F50" s="68"/>
+      <c r="G50" s="37"/>
+      <c r="H50" s="38"/>
+      <c r="I50" s="38"/>
+      <c r="J50" s="35"/>
+      <c r="K50" s="36"/>
+      <c r="L50" s="38"/>
+      <c r="M50" s="38"/>
+      <c r="N50" s="38"/>
+      <c r="O50" s="39"/>
     </row>
     <row r="51" spans="2:15" ht="18" customHeight="1">
       <c r="B51" s="19"/>
       <c r="C51" s="17"/>
-      <c r="D51" s="31"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="34"/>
-      <c r="H51" s="35"/>
-      <c r="I51" s="35"/>
-      <c r="J51" s="31"/>
-      <c r="K51" s="32"/>
-      <c r="L51" s="35"/>
-      <c r="M51" s="35"/>
-      <c r="N51" s="35"/>
-      <c r="O51" s="43"/>
+      <c r="D51" s="63"/>
+      <c r="E51" s="64"/>
+      <c r="F51" s="65"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="33"/>
+      <c r="I51" s="33"/>
+      <c r="J51" s="30"/>
+      <c r="K51" s="31"/>
+      <c r="L51" s="33"/>
+      <c r="M51" s="33"/>
+      <c r="N51" s="33"/>
+      <c r="O51" s="40"/>
     </row>
     <row r="52" spans="2:15" ht="18" customHeight="1">
       <c r="B52" s="19"/>
       <c r="C52" s="18"/>
-      <c r="D52" s="37"/>
-      <c r="E52" s="38"/>
-      <c r="F52" s="39"/>
-      <c r="G52" s="40"/>
-      <c r="H52" s="41"/>
-      <c r="I52" s="41"/>
-      <c r="J52" s="37"/>
-      <c r="K52" s="38"/>
-      <c r="L52" s="41"/>
-      <c r="M52" s="41"/>
-      <c r="N52" s="41"/>
-      <c r="O52" s="42"/>
+      <c r="D52" s="66"/>
+      <c r="E52" s="67"/>
+      <c r="F52" s="68"/>
+      <c r="G52" s="37"/>
+      <c r="H52" s="38"/>
+      <c r="I52" s="38"/>
+      <c r="J52" s="35"/>
+      <c r="K52" s="36"/>
+      <c r="L52" s="38"/>
+      <c r="M52" s="38"/>
+      <c r="N52" s="38"/>
+      <c r="O52" s="39"/>
     </row>
     <row r="53" spans="2:15" ht="18" customHeight="1">
       <c r="B53" s="19"/>
       <c r="C53" s="17"/>
-      <c r="D53" s="31"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="33"/>
-      <c r="G53" s="34"/>
-      <c r="H53" s="35"/>
-      <c r="I53" s="35"/>
-      <c r="J53" s="31"/>
-      <c r="K53" s="32"/>
-      <c r="L53" s="35"/>
-      <c r="M53" s="35"/>
-      <c r="N53" s="35"/>
-      <c r="O53" s="43"/>
+      <c r="D53" s="63"/>
+      <c r="E53" s="64"/>
+      <c r="F53" s="65"/>
+      <c r="G53" s="32"/>
+      <c r="H53" s="33"/>
+      <c r="I53" s="33"/>
+      <c r="J53" s="30"/>
+      <c r="K53" s="31"/>
+      <c r="L53" s="33"/>
+      <c r="M53" s="33"/>
+      <c r="N53" s="33"/>
+      <c r="O53" s="40"/>
     </row>
     <row r="54" spans="2:15" ht="18" customHeight="1">
       <c r="B54" s="19"/>
       <c r="C54" s="18"/>
-      <c r="D54" s="37"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="39"/>
-      <c r="G54" s="40"/>
-      <c r="H54" s="41"/>
-      <c r="I54" s="41"/>
-      <c r="J54" s="37"/>
-      <c r="K54" s="38"/>
-      <c r="L54" s="41"/>
-      <c r="M54" s="41"/>
-      <c r="N54" s="41"/>
-      <c r="O54" s="42"/>
+      <c r="D54" s="66"/>
+      <c r="E54" s="67"/>
+      <c r="F54" s="68"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="38"/>
+      <c r="I54" s="38"/>
+      <c r="J54" s="35"/>
+      <c r="K54" s="36"/>
+      <c r="L54" s="38"/>
+      <c r="M54" s="38"/>
+      <c r="N54" s="38"/>
+      <c r="O54" s="39"/>
     </row>
     <row r="55" spans="2:15" ht="18" customHeight="1">
       <c r="B55" s="19"/>
       <c r="C55" s="17"/>
-      <c r="D55" s="31"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="33"/>
-      <c r="G55" s="34"/>
-      <c r="H55" s="35"/>
-      <c r="I55" s="35"/>
-      <c r="J55" s="31"/>
-      <c r="K55" s="32"/>
-      <c r="L55" s="35"/>
-      <c r="M55" s="35"/>
-      <c r="N55" s="35"/>
-      <c r="O55" s="43"/>
+      <c r="D55" s="63"/>
+      <c r="E55" s="64"/>
+      <c r="F55" s="65"/>
+      <c r="G55" s="32"/>
+      <c r="H55" s="33"/>
+      <c r="I55" s="33"/>
+      <c r="J55" s="30"/>
+      <c r="K55" s="31"/>
+      <c r="L55" s="33"/>
+      <c r="M55" s="33"/>
+      <c r="N55" s="33"/>
+      <c r="O55" s="40"/>
     </row>
     <row r="56" spans="2:15" ht="18" customHeight="1">
       <c r="B56" s="19"/>
       <c r="C56" s="18"/>
-      <c r="D56" s="37"/>
-      <c r="E56" s="38"/>
-      <c r="F56" s="39"/>
-      <c r="G56" s="40"/>
-      <c r="H56" s="41"/>
-      <c r="I56" s="41"/>
-      <c r="J56" s="37"/>
-      <c r="K56" s="38"/>
-      <c r="L56" s="41"/>
-      <c r="M56" s="41"/>
-      <c r="N56" s="41"/>
-      <c r="O56" s="42"/>
+      <c r="D56" s="66"/>
+      <c r="E56" s="67"/>
+      <c r="F56" s="68"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="38"/>
+      <c r="I56" s="38"/>
+      <c r="J56" s="35"/>
+      <c r="K56" s="36"/>
+      <c r="L56" s="38"/>
+      <c r="M56" s="38"/>
+      <c r="N56" s="38"/>
+      <c r="O56" s="39"/>
     </row>
     <row r="57" spans="2:15" ht="18" customHeight="1">
       <c r="B57" s="19"/>
       <c r="C57" s="17"/>
-      <c r="D57" s="31"/>
-      <c r="E57" s="32"/>
-      <c r="F57" s="33"/>
-      <c r="G57" s="34"/>
-      <c r="H57" s="35"/>
-      <c r="I57" s="35"/>
-      <c r="J57" s="31"/>
-      <c r="K57" s="32"/>
-      <c r="L57" s="35"/>
-      <c r="M57" s="35"/>
-      <c r="N57" s="35"/>
-      <c r="O57" s="43"/>
+      <c r="D57" s="63"/>
+      <c r="E57" s="64"/>
+      <c r="F57" s="65"/>
+      <c r="G57" s="32"/>
+      <c r="H57" s="33"/>
+      <c r="I57" s="33"/>
+      <c r="J57" s="30"/>
+      <c r="K57" s="31"/>
+      <c r="L57" s="33"/>
+      <c r="M57" s="33"/>
+      <c r="N57" s="33"/>
+      <c r="O57" s="40"/>
     </row>
     <row r="58" spans="2:15" ht="18" customHeight="1">
       <c r="B58" s="19"/>
       <c r="C58" s="18"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="38"/>
-      <c r="F58" s="39"/>
-      <c r="G58" s="40"/>
-      <c r="H58" s="41"/>
-      <c r="I58" s="41"/>
-      <c r="J58" s="37"/>
-      <c r="K58" s="38"/>
-      <c r="L58" s="41"/>
-      <c r="M58" s="41"/>
-      <c r="N58" s="41"/>
-      <c r="O58" s="42"/>
+      <c r="D58" s="66"/>
+      <c r="E58" s="67"/>
+      <c r="F58" s="68"/>
+      <c r="G58" s="37"/>
+      <c r="H58" s="38"/>
+      <c r="I58" s="38"/>
+      <c r="J58" s="35"/>
+      <c r="K58" s="36"/>
+      <c r="L58" s="38"/>
+      <c r="M58" s="38"/>
+      <c r="N58" s="38"/>
+      <c r="O58" s="39"/>
     </row>
     <row r="59" spans="2:15" ht="18" customHeight="1">
       <c r="B59" s="19"/>
       <c r="C59" s="17"/>
-      <c r="D59" s="31"/>
-      <c r="E59" s="32"/>
-      <c r="F59" s="33"/>
-      <c r="G59" s="34"/>
-      <c r="H59" s="35"/>
-      <c r="I59" s="35"/>
-      <c r="J59" s="31"/>
-      <c r="K59" s="32"/>
-      <c r="L59" s="35"/>
-      <c r="M59" s="35"/>
-      <c r="N59" s="35"/>
-      <c r="O59" s="43"/>
+      <c r="D59" s="63"/>
+      <c r="E59" s="64"/>
+      <c r="F59" s="65"/>
+      <c r="G59" s="32"/>
+      <c r="H59" s="33"/>
+      <c r="I59" s="33"/>
+      <c r="J59" s="30"/>
+      <c r="K59" s="31"/>
+      <c r="L59" s="33"/>
+      <c r="M59" s="33"/>
+      <c r="N59" s="33"/>
+      <c r="O59" s="40"/>
     </row>
     <row r="60" spans="2:15" ht="18" customHeight="1">
       <c r="B60" s="19"/>
       <c r="C60" s="18"/>
-      <c r="D60" s="37"/>
-      <c r="E60" s="38"/>
-      <c r="F60" s="39"/>
-      <c r="G60" s="40"/>
-      <c r="H60" s="41"/>
-      <c r="I60" s="41"/>
-      <c r="J60" s="37"/>
-      <c r="K60" s="38"/>
-      <c r="L60" s="41"/>
-      <c r="M60" s="41"/>
-      <c r="N60" s="41"/>
-      <c r="O60" s="42"/>
+      <c r="D60" s="66"/>
+      <c r="E60" s="67"/>
+      <c r="F60" s="68"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="38"/>
+      <c r="I60" s="38"/>
+      <c r="J60" s="35"/>
+      <c r="K60" s="36"/>
+      <c r="L60" s="38"/>
+      <c r="M60" s="38"/>
+      <c r="N60" s="38"/>
+      <c r="O60" s="39"/>
     </row>
     <row r="61" spans="2:15" ht="18" customHeight="1">
       <c r="B61" s="19"/>
       <c r="C61" s="17"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="33"/>
-      <c r="G61" s="34"/>
-      <c r="H61" s="35"/>
-      <c r="I61" s="35"/>
-      <c r="J61" s="31"/>
-      <c r="K61" s="32"/>
-      <c r="L61" s="35"/>
-      <c r="M61" s="35"/>
-      <c r="N61" s="35"/>
-      <c r="O61" s="43"/>
+      <c r="D61" s="63"/>
+      <c r="E61" s="64"/>
+      <c r="F61" s="65"/>
+      <c r="G61" s="32"/>
+      <c r="H61" s="33"/>
+      <c r="I61" s="33"/>
+      <c r="J61" s="30"/>
+      <c r="K61" s="31"/>
+      <c r="L61" s="33"/>
+      <c r="M61" s="33"/>
+      <c r="N61" s="33"/>
+      <c r="O61" s="40"/>
     </row>
     <row r="62" spans="2:15" ht="18" customHeight="1">
       <c r="B62" s="19"/>
       <c r="C62" s="18"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="38"/>
-      <c r="F62" s="39"/>
-      <c r="G62" s="40"/>
-      <c r="H62" s="41"/>
-      <c r="I62" s="41"/>
-      <c r="J62" s="37"/>
-      <c r="K62" s="38"/>
-      <c r="L62" s="41"/>
-      <c r="M62" s="41"/>
-      <c r="N62" s="41"/>
-      <c r="O62" s="42"/>
+      <c r="D62" s="66"/>
+      <c r="E62" s="67"/>
+      <c r="F62" s="68"/>
+      <c r="G62" s="37"/>
+      <c r="H62" s="38"/>
+      <c r="I62" s="38"/>
+      <c r="J62" s="35"/>
+      <c r="K62" s="36"/>
+      <c r="L62" s="38"/>
+      <c r="M62" s="38"/>
+      <c r="N62" s="38"/>
+      <c r="O62" s="39"/>
     </row>
     <row r="63" spans="2:15" ht="18" customHeight="1">
       <c r="B63" s="19"/>
       <c r="C63" s="17"/>
-      <c r="D63" s="31"/>
-      <c r="E63" s="32"/>
-      <c r="F63" s="33"/>
-      <c r="G63" s="34"/>
-      <c r="H63" s="35"/>
-      <c r="I63" s="35"/>
-      <c r="J63" s="31"/>
-      <c r="K63" s="32"/>
-      <c r="L63" s="35"/>
-      <c r="M63" s="35"/>
-      <c r="N63" s="35"/>
-      <c r="O63" s="43"/>
+      <c r="D63" s="63"/>
+      <c r="E63" s="64"/>
+      <c r="F63" s="65"/>
+      <c r="G63" s="32"/>
+      <c r="H63" s="33"/>
+      <c r="I63" s="33"/>
+      <c r="J63" s="30"/>
+      <c r="K63" s="31"/>
+      <c r="L63" s="33"/>
+      <c r="M63" s="33"/>
+      <c r="N63" s="33"/>
+      <c r="O63" s="40"/>
     </row>
     <row r="64" spans="2:15" ht="18" customHeight="1">
       <c r="B64" s="19"/>
       <c r="C64" s="18"/>
-      <c r="D64" s="37"/>
-      <c r="E64" s="38"/>
-      <c r="F64" s="39"/>
-      <c r="G64" s="40"/>
-      <c r="H64" s="41"/>
-      <c r="I64" s="41"/>
-      <c r="J64" s="37"/>
-      <c r="K64" s="38"/>
-      <c r="L64" s="41"/>
-      <c r="M64" s="41"/>
-      <c r="N64" s="41"/>
-      <c r="O64" s="42"/>
+      <c r="D64" s="66"/>
+      <c r="E64" s="67"/>
+      <c r="F64" s="68"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="38"/>
+      <c r="J64" s="35"/>
+      <c r="K64" s="36"/>
+      <c r="L64" s="38"/>
+      <c r="M64" s="38"/>
+      <c r="N64" s="38"/>
+      <c r="O64" s="39"/>
     </row>
     <row r="65" spans="2:15" ht="18" customHeight="1">
       <c r="B65" s="19"/>
       <c r="C65" s="17"/>
-      <c r="D65" s="31"/>
-      <c r="E65" s="32"/>
-      <c r="F65" s="33"/>
-      <c r="G65" s="34"/>
-      <c r="H65" s="35"/>
-      <c r="I65" s="35"/>
-      <c r="J65" s="31"/>
-      <c r="K65" s="32"/>
-      <c r="L65" s="35"/>
-      <c r="M65" s="35"/>
-      <c r="N65" s="35"/>
-      <c r="O65" s="43"/>
+      <c r="D65" s="63"/>
+      <c r="E65" s="64"/>
+      <c r="F65" s="65"/>
+      <c r="G65" s="32"/>
+      <c r="H65" s="33"/>
+      <c r="I65" s="33"/>
+      <c r="J65" s="30"/>
+      <c r="K65" s="31"/>
+      <c r="L65" s="33"/>
+      <c r="M65" s="33"/>
+      <c r="N65" s="33"/>
+      <c r="O65" s="40"/>
     </row>
     <row r="66" spans="2:15" ht="18" customHeight="1">
       <c r="B66" s="19"/>
       <c r="C66" s="18"/>
-      <c r="D66" s="37"/>
-      <c r="E66" s="38"/>
-      <c r="F66" s="39"/>
-      <c r="G66" s="40"/>
-      <c r="H66" s="41"/>
-      <c r="I66" s="41"/>
-      <c r="J66" s="37"/>
-      <c r="K66" s="38"/>
-      <c r="L66" s="41"/>
-      <c r="M66" s="41"/>
-      <c r="N66" s="41"/>
-      <c r="O66" s="42"/>
+      <c r="D66" s="66"/>
+      <c r="E66" s="67"/>
+      <c r="F66" s="68"/>
+      <c r="G66" s="37"/>
+      <c r="H66" s="38"/>
+      <c r="I66" s="38"/>
+      <c r="J66" s="35"/>
+      <c r="K66" s="36"/>
+      <c r="L66" s="38"/>
+      <c r="M66" s="38"/>
+      <c r="N66" s="38"/>
+      <c r="O66" s="39"/>
     </row>
     <row r="67" spans="2:15" ht="18" customHeight="1" thickBot="1">
       <c r="B67" s="19"/>
       <c r="C67" s="24"/>
-      <c r="D67" s="46"/>
-      <c r="E67" s="47"/>
-      <c r="F67" s="48"/>
-      <c r="G67" s="49"/>
-      <c r="H67" s="50"/>
-      <c r="I67" s="50"/>
-      <c r="J67" s="46"/>
-      <c r="K67" s="47"/>
-      <c r="L67" s="50"/>
-      <c r="M67" s="50"/>
-      <c r="N67" s="50"/>
-      <c r="O67" s="51"/>
+      <c r="D67" s="71"/>
+      <c r="E67" s="72"/>
+      <c r="F67" s="73"/>
+      <c r="G67" s="44"/>
+      <c r="H67" s="45"/>
+      <c r="I67" s="45"/>
+      <c r="J67" s="42"/>
+      <c r="K67" s="43"/>
+      <c r="L67" s="45"/>
+      <c r="M67" s="45"/>
+      <c r="N67" s="45"/>
+      <c r="O67" s="46"/>
     </row>
     <row r="68" spans="2:15" ht="12.75" thickTop="1"/>
   </sheetData>
@@ -45939,27 +45966,27 @@
     </row>
     <row r="3" spans="2:15" ht="18" customHeight="1" thickTop="1">
       <c r="B3" s="19"/>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="54"/>
-      <c r="E3" s="55" t="s">
+      <c r="D3" s="49"/>
+      <c r="E3" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="57" t="s">
+      <c r="F3" s="51"/>
+      <c r="G3" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="57" t="s">
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="52" t="s">
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="47" t="s">
         <v>8</v>
       </c>
     </row>
@@ -45969,23 +45996,23 @@
       <c r="D4" s="11"/>
       <c r="E4" s="12"/>
       <c r="F4" s="13"/>
-      <c r="G4" s="61" t="s">
+      <c r="G4" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="62"/>
-      <c r="I4" s="63" t="s">
+      <c r="H4" s="57"/>
+      <c r="I4" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="64"/>
-      <c r="K4" s="61" t="s">
+      <c r="J4" s="59"/>
+      <c r="K4" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="62"/>
-      <c r="M4" s="63" t="s">
+      <c r="L4" s="57"/>
+      <c r="M4" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="64"/>
-      <c r="O4" s="52"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="47"/>
     </row>
     <row r="5" spans="2:15" ht="18" customHeight="1" thickBot="1">
       <c r="B5" s="19"/>
@@ -46025,999 +46052,999 @@
       <c r="N5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="52"/>
+      <c r="O5" s="47"/>
     </row>
     <row r="6" spans="2:15" ht="18" customHeight="1" thickTop="1">
       <c r="B6" s="19"/>
       <c r="C6" s="16"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
       <c r="J6" s="25"/>
       <c r="K6" s="26"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="30"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="29"/>
     </row>
     <row r="7" spans="2:15" ht="18" customHeight="1">
       <c r="B7" s="19"/>
       <c r="C7" s="17"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="36"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="34"/>
     </row>
     <row r="8" spans="2:15" ht="18" customHeight="1">
       <c r="B8" s="19"/>
       <c r="C8" s="18"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="30"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="29"/>
     </row>
     <row r="9" spans="2:15" ht="18" customHeight="1">
       <c r="B9" s="19"/>
       <c r="C9" s="17"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="36"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="34"/>
     </row>
     <row r="10" spans="2:15" ht="18" customHeight="1">
       <c r="B10" s="19"/>
       <c r="C10" s="18"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="42"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="39"/>
     </row>
     <row r="11" spans="2:15" ht="18" customHeight="1">
       <c r="B11" s="19"/>
       <c r="C11" s="17"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="43"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="40"/>
     </row>
     <row r="12" spans="2:15" ht="18" customHeight="1">
       <c r="B12" s="19"/>
       <c r="C12" s="18"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="42"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="39"/>
     </row>
     <row r="13" spans="2:15" ht="18" customHeight="1">
       <c r="B13" s="19"/>
       <c r="C13" s="17"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="43"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="40"/>
     </row>
     <row r="14" spans="2:15" ht="18" customHeight="1">
       <c r="B14" s="19"/>
       <c r="C14" s="18"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="42"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="39"/>
     </row>
     <row r="15" spans="2:15" ht="18" customHeight="1">
       <c r="B15" s="19"/>
       <c r="C15" s="17"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="43"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="33"/>
+      <c r="O15" s="40"/>
     </row>
     <row r="16" spans="2:15" ht="18" customHeight="1">
       <c r="B16" s="19"/>
       <c r="C16" s="18"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="41"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="41"/>
-      <c r="O16" s="42"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="39"/>
     </row>
     <row r="17" spans="2:15" ht="18" customHeight="1">
       <c r="B17" s="19"/>
       <c r="C17" s="17"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="43"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="33"/>
+      <c r="O17" s="40"/>
     </row>
     <row r="18" spans="2:15" ht="18" customHeight="1">
       <c r="B18" s="19"/>
       <c r="C18" s="18"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="38"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="42"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="39"/>
     </row>
     <row r="19" spans="2:15" ht="18" customHeight="1">
       <c r="B19" s="19"/>
       <c r="C19" s="17"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="43"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
+      <c r="O19" s="40"/>
     </row>
     <row r="20" spans="2:15" ht="18" customHeight="1">
       <c r="B20" s="19"/>
       <c r="C20" s="18"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="42"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="39"/>
     </row>
     <row r="21" spans="2:15" ht="18" customHeight="1">
       <c r="B21" s="19"/>
       <c r="C21" s="17"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="35"/>
-      <c r="O21" s="43"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
+      <c r="O21" s="40"/>
     </row>
     <row r="22" spans="2:15" ht="18" customHeight="1">
       <c r="B22" s="19"/>
       <c r="C22" s="18"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="41"/>
-      <c r="O22" s="42"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="39"/>
     </row>
     <row r="23" spans="2:15" ht="18" customHeight="1">
       <c r="B23" s="19"/>
       <c r="C23" s="17"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="35"/>
-      <c r="O23" s="43"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="33"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="33"/>
+      <c r="O23" s="40"/>
     </row>
     <row r="24" spans="2:15" ht="18" customHeight="1">
       <c r="B24" s="19"/>
       <c r="C24" s="18"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="38"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="41"/>
-      <c r="N24" s="41"/>
-      <c r="O24" s="42"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="39"/>
     </row>
     <row r="25" spans="2:15" ht="18" customHeight="1">
       <c r="B25" s="19"/>
       <c r="C25" s="17"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="35"/>
-      <c r="O25" s="43"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="40"/>
     </row>
     <row r="26" spans="2:15" ht="18" customHeight="1">
       <c r="B26" s="19"/>
       <c r="C26" s="18"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="41"/>
-      <c r="M26" s="41"/>
-      <c r="N26" s="41"/>
-      <c r="O26" s="42"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="39"/>
     </row>
     <row r="27" spans="2:15" ht="18" customHeight="1">
       <c r="B27" s="19"/>
       <c r="C27" s="17"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="35"/>
-      <c r="M27" s="35"/>
-      <c r="N27" s="35"/>
-      <c r="O27" s="43"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="33"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="33"/>
+      <c r="O27" s="40"/>
     </row>
     <row r="28" spans="2:15" ht="18" customHeight="1">
       <c r="B28" s="19"/>
       <c r="C28" s="18"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="41"/>
-      <c r="M28" s="41"/>
-      <c r="N28" s="41"/>
-      <c r="O28" s="42"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="38"/>
+      <c r="O28" s="39"/>
     </row>
     <row r="29" spans="2:15" ht="18" customHeight="1">
       <c r="B29" s="19"/>
       <c r="C29" s="17"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="35"/>
-      <c r="M29" s="35"/>
-      <c r="N29" s="35"/>
-      <c r="O29" s="43"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="33"/>
+      <c r="O29" s="40"/>
     </row>
     <row r="30" spans="2:15" ht="18" customHeight="1">
       <c r="B30" s="19"/>
       <c r="C30" s="18"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="41"/>
-      <c r="M30" s="41"/>
-      <c r="N30" s="41"/>
-      <c r="O30" s="42"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="68"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="39"/>
     </row>
     <row r="31" spans="2:15" ht="18" customHeight="1">
       <c r="B31" s="19"/>
       <c r="C31" s="17"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="35"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="35"/>
-      <c r="M31" s="35"/>
-      <c r="N31" s="35"/>
-      <c r="O31" s="43"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="33"/>
+      <c r="N31" s="33"/>
+      <c r="O31" s="40"/>
     </row>
     <row r="32" spans="2:15" ht="18" customHeight="1">
       <c r="B32" s="19"/>
       <c r="C32" s="18"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="38"/>
-      <c r="L32" s="41"/>
-      <c r="M32" s="41"/>
-      <c r="N32" s="41"/>
-      <c r="O32" s="42"/>
+      <c r="D32" s="66"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="68"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="38"/>
+      <c r="M32" s="38"/>
+      <c r="N32" s="38"/>
+      <c r="O32" s="39"/>
     </row>
     <row r="33" spans="2:15" ht="18" customHeight="1">
       <c r="B33" s="19"/>
       <c r="C33" s="17"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="35"/>
-      <c r="I33" s="35"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="35"/>
-      <c r="M33" s="35"/>
-      <c r="N33" s="35"/>
-      <c r="O33" s="43"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="31"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
+      <c r="N33" s="33"/>
+      <c r="O33" s="40"/>
     </row>
     <row r="34" spans="2:15" ht="18" customHeight="1">
       <c r="B34" s="19"/>
       <c r="C34" s="18"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="41"/>
-      <c r="I34" s="41"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="38"/>
-      <c r="L34" s="41"/>
-      <c r="M34" s="41"/>
-      <c r="N34" s="41"/>
-      <c r="O34" s="42"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="36"/>
+      <c r="L34" s="38"/>
+      <c r="M34" s="38"/>
+      <c r="N34" s="38"/>
+      <c r="O34" s="39"/>
     </row>
     <row r="35" spans="2:15" ht="18" customHeight="1">
       <c r="B35" s="19"/>
       <c r="C35" s="17"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="35"/>
-      <c r="I35" s="35"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="35"/>
-      <c r="M35" s="35"/>
-      <c r="N35" s="35"/>
-      <c r="O35" s="43"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="31"/>
+      <c r="L35" s="33"/>
+      <c r="M35" s="33"/>
+      <c r="N35" s="33"/>
+      <c r="O35" s="40"/>
     </row>
     <row r="36" spans="2:15" ht="18" customHeight="1">
       <c r="B36" s="19"/>
       <c r="C36" s="18"/>
-      <c r="D36" s="37"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="41"/>
-      <c r="J36" s="37"/>
-      <c r="K36" s="38"/>
-      <c r="L36" s="41"/>
-      <c r="M36" s="41"/>
-      <c r="N36" s="41"/>
-      <c r="O36" s="42"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="68"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="38"/>
+      <c r="M36" s="38"/>
+      <c r="N36" s="38"/>
+      <c r="O36" s="39"/>
     </row>
     <row r="37" spans="2:15" ht="18" customHeight="1">
       <c r="B37" s="19"/>
       <c r="C37" s="17"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="32"/>
-      <c r="L37" s="35"/>
-      <c r="M37" s="35"/>
-      <c r="N37" s="35"/>
-      <c r="O37" s="43"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="30"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="33"/>
+      <c r="M37" s="33"/>
+      <c r="N37" s="33"/>
+      <c r="O37" s="40"/>
     </row>
     <row r="38" spans="2:15" ht="18" customHeight="1">
       <c r="B38" s="19"/>
       <c r="C38" s="16"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="45"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28"/>
       <c r="J38" s="25"/>
-      <c r="K38" s="44"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
-      <c r="N38" s="29"/>
-      <c r="O38" s="42"/>
+      <c r="K38" s="41"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="28"/>
+      <c r="N38" s="28"/>
+      <c r="O38" s="39"/>
     </row>
     <row r="39" spans="2:15" ht="18" customHeight="1">
       <c r="B39" s="19"/>
       <c r="C39" s="17"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="35"/>
-      <c r="I39" s="35"/>
-      <c r="J39" s="31"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="35"/>
-      <c r="M39" s="35"/>
-      <c r="N39" s="35"/>
-      <c r="O39" s="43"/>
+      <c r="D39" s="63"/>
+      <c r="E39" s="64"/>
+      <c r="F39" s="65"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="30"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="33"/>
+      <c r="M39" s="33"/>
+      <c r="N39" s="33"/>
+      <c r="O39" s="40"/>
     </row>
     <row r="40" spans="2:15" ht="18" customHeight="1">
       <c r="B40" s="19"/>
       <c r="C40" s="18"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="40"/>
-      <c r="H40" s="41"/>
-      <c r="I40" s="41"/>
-      <c r="J40" s="37"/>
-      <c r="K40" s="38"/>
-      <c r="L40" s="41"/>
-      <c r="M40" s="41"/>
-      <c r="N40" s="41"/>
-      <c r="O40" s="42"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="67"/>
+      <c r="F40" s="68"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="36"/>
+      <c r="L40" s="38"/>
+      <c r="M40" s="38"/>
+      <c r="N40" s="38"/>
+      <c r="O40" s="39"/>
     </row>
     <row r="41" spans="2:15" ht="18" customHeight="1">
       <c r="B41" s="19"/>
       <c r="C41" s="17"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="34"/>
-      <c r="H41" s="35"/>
-      <c r="I41" s="35"/>
-      <c r="J41" s="31"/>
-      <c r="K41" s="32"/>
-      <c r="L41" s="35"/>
-      <c r="M41" s="35"/>
-      <c r="N41" s="35"/>
-      <c r="O41" s="43"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="64"/>
+      <c r="F41" s="65"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="33"/>
+      <c r="J41" s="30"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="33"/>
+      <c r="M41" s="33"/>
+      <c r="N41" s="33"/>
+      <c r="O41" s="40"/>
     </row>
     <row r="42" spans="2:15" ht="18" customHeight="1">
       <c r="B42" s="19"/>
       <c r="C42" s="18"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="41"/>
-      <c r="I42" s="41"/>
-      <c r="J42" s="37"/>
-      <c r="K42" s="38"/>
-      <c r="L42" s="41"/>
-      <c r="M42" s="41"/>
-      <c r="N42" s="41"/>
-      <c r="O42" s="42"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="67"/>
+      <c r="F42" s="68"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="36"/>
+      <c r="L42" s="38"/>
+      <c r="M42" s="38"/>
+      <c r="N42" s="38"/>
+      <c r="O42" s="39"/>
     </row>
     <row r="43" spans="2:15" ht="18" customHeight="1">
       <c r="B43" s="19"/>
       <c r="C43" s="17"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="31"/>
-      <c r="K43" s="32"/>
-      <c r="L43" s="35"/>
-      <c r="M43" s="35"/>
-      <c r="N43" s="35"/>
-      <c r="O43" s="43"/>
+      <c r="D43" s="63"/>
+      <c r="E43" s="64"/>
+      <c r="F43" s="65"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="30"/>
+      <c r="K43" s="31"/>
+      <c r="L43" s="33"/>
+      <c r="M43" s="33"/>
+      <c r="N43" s="33"/>
+      <c r="O43" s="40"/>
     </row>
     <row r="44" spans="2:15" ht="18" customHeight="1">
       <c r="B44" s="19"/>
       <c r="C44" s="18"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="40"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="37"/>
-      <c r="K44" s="38"/>
-      <c r="L44" s="41"/>
-      <c r="M44" s="41"/>
-      <c r="N44" s="41"/>
-      <c r="O44" s="42"/>
+      <c r="D44" s="66"/>
+      <c r="E44" s="67"/>
+      <c r="F44" s="68"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="35"/>
+      <c r="K44" s="36"/>
+      <c r="L44" s="38"/>
+      <c r="M44" s="38"/>
+      <c r="N44" s="38"/>
+      <c r="O44" s="39"/>
     </row>
     <row r="45" spans="2:15" ht="18" customHeight="1">
       <c r="B45" s="19"/>
       <c r="C45" s="17"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="34"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="31"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="35"/>
-      <c r="M45" s="35"/>
-      <c r="N45" s="35"/>
-      <c r="O45" s="43"/>
+      <c r="D45" s="63"/>
+      <c r="E45" s="64"/>
+      <c r="F45" s="65"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="30"/>
+      <c r="K45" s="31"/>
+      <c r="L45" s="33"/>
+      <c r="M45" s="33"/>
+      <c r="N45" s="33"/>
+      <c r="O45" s="40"/>
     </row>
     <row r="46" spans="2:15" ht="18" customHeight="1">
       <c r="B46" s="19"/>
       <c r="C46" s="18"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="39"/>
-      <c r="G46" s="40"/>
-      <c r="H46" s="41"/>
-      <c r="I46" s="41"/>
-      <c r="J46" s="37"/>
-      <c r="K46" s="38"/>
-      <c r="L46" s="41"/>
-      <c r="M46" s="41"/>
-      <c r="N46" s="41"/>
-      <c r="O46" s="42"/>
+      <c r="D46" s="66"/>
+      <c r="E46" s="67"/>
+      <c r="F46" s="68"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="36"/>
+      <c r="L46" s="38"/>
+      <c r="M46" s="38"/>
+      <c r="N46" s="38"/>
+      <c r="O46" s="39"/>
     </row>
     <row r="47" spans="2:15" ht="18" customHeight="1">
       <c r="B47" s="19"/>
       <c r="C47" s="17"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="34"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="35"/>
-      <c r="J47" s="31"/>
-      <c r="K47" s="32"/>
-      <c r="L47" s="35"/>
-      <c r="M47" s="35"/>
-      <c r="N47" s="35"/>
-      <c r="O47" s="43"/>
+      <c r="D47" s="63"/>
+      <c r="E47" s="64"/>
+      <c r="F47" s="65"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="33"/>
+      <c r="I47" s="33"/>
+      <c r="J47" s="30"/>
+      <c r="K47" s="31"/>
+      <c r="L47" s="33"/>
+      <c r="M47" s="33"/>
+      <c r="N47" s="33"/>
+      <c r="O47" s="40"/>
     </row>
     <row r="48" spans="2:15" ht="18" customHeight="1">
       <c r="B48" s="19"/>
       <c r="C48" s="18"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="38"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="40"/>
-      <c r="H48" s="41"/>
-      <c r="I48" s="41"/>
-      <c r="J48" s="37"/>
-      <c r="K48" s="38"/>
-      <c r="L48" s="41"/>
-      <c r="M48" s="41"/>
-      <c r="N48" s="41"/>
-      <c r="O48" s="42"/>
+      <c r="D48" s="66"/>
+      <c r="E48" s="67"/>
+      <c r="F48" s="68"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="38"/>
+      <c r="I48" s="38"/>
+      <c r="J48" s="35"/>
+      <c r="K48" s="36"/>
+      <c r="L48" s="38"/>
+      <c r="M48" s="38"/>
+      <c r="N48" s="38"/>
+      <c r="O48" s="39"/>
     </row>
     <row r="49" spans="2:15" ht="18" customHeight="1">
       <c r="B49" s="19"/>
       <c r="C49" s="17"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="33"/>
-      <c r="G49" s="34"/>
-      <c r="H49" s="35"/>
-      <c r="I49" s="35"/>
-      <c r="J49" s="31"/>
-      <c r="K49" s="32"/>
-      <c r="L49" s="35"/>
-      <c r="M49" s="35"/>
-      <c r="N49" s="35"/>
-      <c r="O49" s="43"/>
+      <c r="D49" s="63"/>
+      <c r="E49" s="64"/>
+      <c r="F49" s="65"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="33"/>
+      <c r="I49" s="33"/>
+      <c r="J49" s="30"/>
+      <c r="K49" s="31"/>
+      <c r="L49" s="33"/>
+      <c r="M49" s="33"/>
+      <c r="N49" s="33"/>
+      <c r="O49" s="40"/>
     </row>
     <row r="50" spans="2:15" ht="18" customHeight="1">
       <c r="B50" s="19"/>
       <c r="C50" s="18"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="38"/>
-      <c r="F50" s="39"/>
-      <c r="G50" s="40"/>
-      <c r="H50" s="41"/>
-      <c r="I50" s="41"/>
-      <c r="J50" s="37"/>
-      <c r="K50" s="38"/>
-      <c r="L50" s="41"/>
-      <c r="M50" s="41"/>
-      <c r="N50" s="41"/>
-      <c r="O50" s="42"/>
+      <c r="D50" s="66"/>
+      <c r="E50" s="67"/>
+      <c r="F50" s="68"/>
+      <c r="G50" s="37"/>
+      <c r="H50" s="38"/>
+      <c r="I50" s="38"/>
+      <c r="J50" s="35"/>
+      <c r="K50" s="36"/>
+      <c r="L50" s="38"/>
+      <c r="M50" s="38"/>
+      <c r="N50" s="38"/>
+      <c r="O50" s="39"/>
     </row>
     <row r="51" spans="2:15" ht="18" customHeight="1">
       <c r="B51" s="19"/>
       <c r="C51" s="17"/>
-      <c r="D51" s="31"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="34"/>
-      <c r="H51" s="35"/>
-      <c r="I51" s="35"/>
-      <c r="J51" s="31"/>
-      <c r="K51" s="32"/>
-      <c r="L51" s="35"/>
-      <c r="M51" s="35"/>
-      <c r="N51" s="35"/>
-      <c r="O51" s="43"/>
+      <c r="D51" s="63"/>
+      <c r="E51" s="64"/>
+      <c r="F51" s="65"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="33"/>
+      <c r="I51" s="33"/>
+      <c r="J51" s="30"/>
+      <c r="K51" s="31"/>
+      <c r="L51" s="33"/>
+      <c r="M51" s="33"/>
+      <c r="N51" s="33"/>
+      <c r="O51" s="40"/>
     </row>
     <row r="52" spans="2:15" ht="18" customHeight="1">
       <c r="B52" s="19"/>
       <c r="C52" s="18"/>
-      <c r="D52" s="37"/>
-      <c r="E52" s="38"/>
-      <c r="F52" s="39"/>
-      <c r="G52" s="40"/>
-      <c r="H52" s="41"/>
-      <c r="I52" s="41"/>
-      <c r="J52" s="37"/>
-      <c r="K52" s="38"/>
-      <c r="L52" s="41"/>
-      <c r="M52" s="41"/>
-      <c r="N52" s="41"/>
-      <c r="O52" s="42"/>
+      <c r="D52" s="66"/>
+      <c r="E52" s="67"/>
+      <c r="F52" s="68"/>
+      <c r="G52" s="37"/>
+      <c r="H52" s="38"/>
+      <c r="I52" s="38"/>
+      <c r="J52" s="35"/>
+      <c r="K52" s="36"/>
+      <c r="L52" s="38"/>
+      <c r="M52" s="38"/>
+      <c r="N52" s="38"/>
+      <c r="O52" s="39"/>
     </row>
     <row r="53" spans="2:15" ht="18" customHeight="1">
       <c r="B53" s="19"/>
       <c r="C53" s="17"/>
-      <c r="D53" s="31"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="33"/>
-      <c r="G53" s="34"/>
-      <c r="H53" s="35"/>
-      <c r="I53" s="35"/>
-      <c r="J53" s="31"/>
-      <c r="K53" s="32"/>
-      <c r="L53" s="35"/>
-      <c r="M53" s="35"/>
-      <c r="N53" s="35"/>
-      <c r="O53" s="43"/>
+      <c r="D53" s="63"/>
+      <c r="E53" s="64"/>
+      <c r="F53" s="65"/>
+      <c r="G53" s="32"/>
+      <c r="H53" s="33"/>
+      <c r="I53" s="33"/>
+      <c r="J53" s="30"/>
+      <c r="K53" s="31"/>
+      <c r="L53" s="33"/>
+      <c r="M53" s="33"/>
+      <c r="N53" s="33"/>
+      <c r="O53" s="40"/>
     </row>
     <row r="54" spans="2:15" ht="18" customHeight="1">
       <c r="B54" s="19"/>
       <c r="C54" s="18"/>
-      <c r="D54" s="37"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="39"/>
-      <c r="G54" s="40"/>
-      <c r="H54" s="41"/>
-      <c r="I54" s="41"/>
-      <c r="J54" s="37"/>
-      <c r="K54" s="38"/>
-      <c r="L54" s="41"/>
-      <c r="M54" s="41"/>
-      <c r="N54" s="41"/>
-      <c r="O54" s="42"/>
+      <c r="D54" s="66"/>
+      <c r="E54" s="67"/>
+      <c r="F54" s="68"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="38"/>
+      <c r="I54" s="38"/>
+      <c r="J54" s="35"/>
+      <c r="K54" s="36"/>
+      <c r="L54" s="38"/>
+      <c r="M54" s="38"/>
+      <c r="N54" s="38"/>
+      <c r="O54" s="39"/>
     </row>
     <row r="55" spans="2:15" ht="18" customHeight="1">
       <c r="B55" s="19"/>
       <c r="C55" s="17"/>
-      <c r="D55" s="31"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="33"/>
-      <c r="G55" s="34"/>
-      <c r="H55" s="35"/>
-      <c r="I55" s="35"/>
-      <c r="J55" s="31"/>
-      <c r="K55" s="32"/>
-      <c r="L55" s="35"/>
-      <c r="M55" s="35"/>
-      <c r="N55" s="35"/>
-      <c r="O55" s="43"/>
+      <c r="D55" s="63"/>
+      <c r="E55" s="64"/>
+      <c r="F55" s="65"/>
+      <c r="G55" s="32"/>
+      <c r="H55" s="33"/>
+      <c r="I55" s="33"/>
+      <c r="J55" s="30"/>
+      <c r="K55" s="31"/>
+      <c r="L55" s="33"/>
+      <c r="M55" s="33"/>
+      <c r="N55" s="33"/>
+      <c r="O55" s="40"/>
     </row>
     <row r="56" spans="2:15" ht="18" customHeight="1">
       <c r="B56" s="19"/>
       <c r="C56" s="18"/>
-      <c r="D56" s="37"/>
-      <c r="E56" s="38"/>
-      <c r="F56" s="39"/>
-      <c r="G56" s="40"/>
-      <c r="H56" s="41"/>
-      <c r="I56" s="41"/>
-      <c r="J56" s="37"/>
-      <c r="K56" s="38"/>
-      <c r="L56" s="41"/>
-      <c r="M56" s="41"/>
-      <c r="N56" s="41"/>
-      <c r="O56" s="42"/>
+      <c r="D56" s="66"/>
+      <c r="E56" s="67"/>
+      <c r="F56" s="68"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="38"/>
+      <c r="I56" s="38"/>
+      <c r="J56" s="35"/>
+      <c r="K56" s="36"/>
+      <c r="L56" s="38"/>
+      <c r="M56" s="38"/>
+      <c r="N56" s="38"/>
+      <c r="O56" s="39"/>
     </row>
     <row r="57" spans="2:15" ht="18" customHeight="1">
       <c r="B57" s="19"/>
       <c r="C57" s="17"/>
-      <c r="D57" s="31"/>
-      <c r="E57" s="32"/>
-      <c r="F57" s="33"/>
-      <c r="G57" s="34"/>
-      <c r="H57" s="35"/>
-      <c r="I57" s="35"/>
-      <c r="J57" s="31"/>
-      <c r="K57" s="32"/>
-      <c r="L57" s="35"/>
-      <c r="M57" s="35"/>
-      <c r="N57" s="35"/>
-      <c r="O57" s="43"/>
+      <c r="D57" s="63"/>
+      <c r="E57" s="64"/>
+      <c r="F57" s="65"/>
+      <c r="G57" s="32"/>
+      <c r="H57" s="33"/>
+      <c r="I57" s="33"/>
+      <c r="J57" s="30"/>
+      <c r="K57" s="31"/>
+      <c r="L57" s="33"/>
+      <c r="M57" s="33"/>
+      <c r="N57" s="33"/>
+      <c r="O57" s="40"/>
     </row>
     <row r="58" spans="2:15" ht="18" customHeight="1">
       <c r="B58" s="19"/>
       <c r="C58" s="18"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="38"/>
-      <c r="F58" s="39"/>
-      <c r="G58" s="40"/>
-      <c r="H58" s="41"/>
-      <c r="I58" s="41"/>
-      <c r="J58" s="37"/>
-      <c r="K58" s="38"/>
-      <c r="L58" s="41"/>
-      <c r="M58" s="41"/>
-      <c r="N58" s="41"/>
-      <c r="O58" s="42"/>
+      <c r="D58" s="66"/>
+      <c r="E58" s="67"/>
+      <c r="F58" s="68"/>
+      <c r="G58" s="37"/>
+      <c r="H58" s="38"/>
+      <c r="I58" s="38"/>
+      <c r="J58" s="35"/>
+      <c r="K58" s="36"/>
+      <c r="L58" s="38"/>
+      <c r="M58" s="38"/>
+      <c r="N58" s="38"/>
+      <c r="O58" s="39"/>
     </row>
     <row r="59" spans="2:15" ht="18" customHeight="1">
       <c r="B59" s="19"/>
       <c r="C59" s="17"/>
-      <c r="D59" s="31"/>
-      <c r="E59" s="32"/>
-      <c r="F59" s="33"/>
-      <c r="G59" s="34"/>
-      <c r="H59" s="35"/>
-      <c r="I59" s="35"/>
-      <c r="J59" s="31"/>
-      <c r="K59" s="32"/>
-      <c r="L59" s="35"/>
-      <c r="M59" s="35"/>
-      <c r="N59" s="35"/>
-      <c r="O59" s="43"/>
+      <c r="D59" s="63"/>
+      <c r="E59" s="64"/>
+      <c r="F59" s="65"/>
+      <c r="G59" s="32"/>
+      <c r="H59" s="33"/>
+      <c r="I59" s="33"/>
+      <c r="J59" s="30"/>
+      <c r="K59" s="31"/>
+      <c r="L59" s="33"/>
+      <c r="M59" s="33"/>
+      <c r="N59" s="33"/>
+      <c r="O59" s="40"/>
     </row>
     <row r="60" spans="2:15" ht="18" customHeight="1">
       <c r="B60" s="19"/>
       <c r="C60" s="18"/>
-      <c r="D60" s="37"/>
-      <c r="E60" s="38"/>
-      <c r="F60" s="39"/>
-      <c r="G60" s="40"/>
-      <c r="H60" s="41"/>
-      <c r="I60" s="41"/>
-      <c r="J60" s="37"/>
-      <c r="K60" s="38"/>
-      <c r="L60" s="41"/>
-      <c r="M60" s="41"/>
-      <c r="N60" s="41"/>
-      <c r="O60" s="42"/>
+      <c r="D60" s="66"/>
+      <c r="E60" s="67"/>
+      <c r="F60" s="68"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="38"/>
+      <c r="I60" s="38"/>
+      <c r="J60" s="35"/>
+      <c r="K60" s="36"/>
+      <c r="L60" s="38"/>
+      <c r="M60" s="38"/>
+      <c r="N60" s="38"/>
+      <c r="O60" s="39"/>
     </row>
     <row r="61" spans="2:15" ht="18" customHeight="1">
       <c r="B61" s="19"/>
       <c r="C61" s="17"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="33"/>
-      <c r="G61" s="34"/>
-      <c r="H61" s="35"/>
-      <c r="I61" s="35"/>
-      <c r="J61" s="31"/>
-      <c r="K61" s="32"/>
-      <c r="L61" s="35"/>
-      <c r="M61" s="35"/>
-      <c r="N61" s="35"/>
-      <c r="O61" s="43"/>
+      <c r="D61" s="63"/>
+      <c r="E61" s="64"/>
+      <c r="F61" s="65"/>
+      <c r="G61" s="32"/>
+      <c r="H61" s="33"/>
+      <c r="I61" s="33"/>
+      <c r="J61" s="30"/>
+      <c r="K61" s="31"/>
+      <c r="L61" s="33"/>
+      <c r="M61" s="33"/>
+      <c r="N61" s="33"/>
+      <c r="O61" s="40"/>
     </row>
     <row r="62" spans="2:15" ht="18" customHeight="1">
       <c r="B62" s="19"/>
       <c r="C62" s="18"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="38"/>
-      <c r="F62" s="39"/>
-      <c r="G62" s="40"/>
-      <c r="H62" s="41"/>
-      <c r="I62" s="41"/>
-      <c r="J62" s="37"/>
-      <c r="K62" s="38"/>
-      <c r="L62" s="41"/>
-      <c r="M62" s="41"/>
-      <c r="N62" s="41"/>
-      <c r="O62" s="42"/>
+      <c r="D62" s="66"/>
+      <c r="E62" s="67"/>
+      <c r="F62" s="68"/>
+      <c r="G62" s="37"/>
+      <c r="H62" s="38"/>
+      <c r="I62" s="38"/>
+      <c r="J62" s="35"/>
+      <c r="K62" s="36"/>
+      <c r="L62" s="38"/>
+      <c r="M62" s="38"/>
+      <c r="N62" s="38"/>
+      <c r="O62" s="39"/>
     </row>
     <row r="63" spans="2:15" ht="18" customHeight="1">
       <c r="B63" s="19"/>
       <c r="C63" s="17"/>
-      <c r="D63" s="31"/>
-      <c r="E63" s="32"/>
-      <c r="F63" s="33"/>
-      <c r="G63" s="34"/>
-      <c r="H63" s="35"/>
-      <c r="I63" s="35"/>
-      <c r="J63" s="31"/>
-      <c r="K63" s="32"/>
-      <c r="L63" s="35"/>
-      <c r="M63" s="35"/>
-      <c r="N63" s="35"/>
-      <c r="O63" s="43"/>
+      <c r="D63" s="63"/>
+      <c r="E63" s="64"/>
+      <c r="F63" s="65"/>
+      <c r="G63" s="32"/>
+      <c r="H63" s="33"/>
+      <c r="I63" s="33"/>
+      <c r="J63" s="30"/>
+      <c r="K63" s="31"/>
+      <c r="L63" s="33"/>
+      <c r="M63" s="33"/>
+      <c r="N63" s="33"/>
+      <c r="O63" s="40"/>
     </row>
     <row r="64" spans="2:15" ht="18" customHeight="1">
       <c r="B64" s="19"/>
       <c r="C64" s="18"/>
-      <c r="D64" s="37"/>
-      <c r="E64" s="38"/>
-      <c r="F64" s="39"/>
-      <c r="G64" s="40"/>
-      <c r="H64" s="41"/>
-      <c r="I64" s="41"/>
-      <c r="J64" s="37"/>
-      <c r="K64" s="38"/>
-      <c r="L64" s="41"/>
-      <c r="M64" s="41"/>
-      <c r="N64" s="41"/>
-      <c r="O64" s="42"/>
+      <c r="D64" s="66"/>
+      <c r="E64" s="67"/>
+      <c r="F64" s="68"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="38"/>
+      <c r="J64" s="35"/>
+      <c r="K64" s="36"/>
+      <c r="L64" s="38"/>
+      <c r="M64" s="38"/>
+      <c r="N64" s="38"/>
+      <c r="O64" s="39"/>
     </row>
     <row r="65" spans="2:15" ht="18" customHeight="1">
       <c r="B65" s="19"/>
       <c r="C65" s="17"/>
-      <c r="D65" s="31"/>
-      <c r="E65" s="32"/>
-      <c r="F65" s="33"/>
-      <c r="G65" s="34"/>
-      <c r="H65" s="35"/>
-      <c r="I65" s="35"/>
-      <c r="J65" s="31"/>
-      <c r="K65" s="32"/>
-      <c r="L65" s="35"/>
-      <c r="M65" s="35"/>
-      <c r="N65" s="35"/>
-      <c r="O65" s="43"/>
+      <c r="D65" s="63"/>
+      <c r="E65" s="64"/>
+      <c r="F65" s="65"/>
+      <c r="G65" s="32"/>
+      <c r="H65" s="33"/>
+      <c r="I65" s="33"/>
+      <c r="J65" s="30"/>
+      <c r="K65" s="31"/>
+      <c r="L65" s="33"/>
+      <c r="M65" s="33"/>
+      <c r="N65" s="33"/>
+      <c r="O65" s="40"/>
     </row>
     <row r="66" spans="2:15" ht="18" customHeight="1">
       <c r="B66" s="19"/>
       <c r="C66" s="18"/>
-      <c r="D66" s="37"/>
-      <c r="E66" s="38"/>
-      <c r="F66" s="39"/>
-      <c r="G66" s="40"/>
-      <c r="H66" s="41"/>
-      <c r="I66" s="41"/>
-      <c r="J66" s="37"/>
-      <c r="K66" s="38"/>
-      <c r="L66" s="41"/>
-      <c r="M66" s="41"/>
-      <c r="N66" s="41"/>
-      <c r="O66" s="42"/>
+      <c r="D66" s="66"/>
+      <c r="E66" s="67"/>
+      <c r="F66" s="68"/>
+      <c r="G66" s="37"/>
+      <c r="H66" s="38"/>
+      <c r="I66" s="38"/>
+      <c r="J66" s="35"/>
+      <c r="K66" s="36"/>
+      <c r="L66" s="38"/>
+      <c r="M66" s="38"/>
+      <c r="N66" s="38"/>
+      <c r="O66" s="39"/>
     </row>
     <row r="67" spans="2:15" ht="18" customHeight="1" thickBot="1">
       <c r="B67" s="19"/>
       <c r="C67" s="24"/>
-      <c r="D67" s="46"/>
-      <c r="E67" s="47"/>
-      <c r="F67" s="48"/>
-      <c r="G67" s="49"/>
-      <c r="H67" s="50"/>
-      <c r="I67" s="50"/>
-      <c r="J67" s="46"/>
-      <c r="K67" s="47"/>
-      <c r="L67" s="50"/>
-      <c r="M67" s="50"/>
-      <c r="N67" s="50"/>
-      <c r="O67" s="51"/>
+      <c r="D67" s="71"/>
+      <c r="E67" s="72"/>
+      <c r="F67" s="73"/>
+      <c r="G67" s="44"/>
+      <c r="H67" s="45"/>
+      <c r="I67" s="45"/>
+      <c r="J67" s="42"/>
+      <c r="K67" s="43"/>
+      <c r="L67" s="45"/>
+      <c r="M67" s="45"/>
+      <c r="N67" s="45"/>
+      <c r="O67" s="46"/>
     </row>
     <row r="68" spans="2:15" ht="12.75" thickTop="1"/>
   </sheetData>

</xml_diff>